<commit_message>
Recalcul automatique de la colonne Mention pour les anciennes interventions
</commit_message>
<xml_diff>
--- a/Objets_parlementaires_CDF_EFK.xlsx
+++ b/Objets_parlementaires_CDF_EFK.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="649">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -573,9 +573,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20253835</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À recalculer</t>
   </si>
   <si>
     <t xml:space="preserve">25.3845</t>
@@ -3299,7 +3296,7 @@
         <v>186</v>
       </c>
       <c r="L26" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27">
@@ -3307,7 +3304,7 @@
         <v>20253845</v>
       </c>
       <c r="B27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
@@ -3322,22 +3319,22 @@
         <v>16</v>
       </c>
       <c r="G27" t="s">
+        <v>188</v>
+      </c>
+      <c r="H27" t="s">
         <v>189</v>
-      </c>
-      <c r="H27" t="s">
-        <v>190</v>
       </c>
       <c r="I27" t="s">
         <v>68</v>
       </c>
       <c r="J27" t="s">
+        <v>190</v>
+      </c>
+      <c r="K27" t="s">
         <v>191</v>
       </c>
-      <c r="K27" t="s">
-        <v>192</v>
-      </c>
       <c r="L27" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28">
@@ -3345,13 +3342,13 @@
         <v>20253855</v>
       </c>
       <c r="B28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" t="s">
         <v>182</v>
@@ -3369,13 +3366,13 @@
         <v>145</v>
       </c>
       <c r="J28" t="s">
+        <v>194</v>
+      </c>
+      <c r="K28" t="s">
         <v>195</v>
       </c>
-      <c r="K28" t="s">
-        <v>196</v>
-      </c>
       <c r="L28" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29">
@@ -3383,13 +3380,13 @@
         <v>20253880</v>
       </c>
       <c r="B29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C29" t="s">
         <v>32</v>
       </c>
       <c r="D29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E29" t="s">
         <v>182</v>
@@ -3398,22 +3395,22 @@
         <v>16</v>
       </c>
       <c r="G29" t="s">
+        <v>198</v>
+      </c>
+      <c r="H29" t="s">
         <v>199</v>
-      </c>
-      <c r="H29" t="s">
-        <v>200</v>
       </c>
       <c r="I29" t="s">
         <v>68</v>
       </c>
       <c r="J29" t="s">
+        <v>200</v>
+      </c>
+      <c r="K29" t="s">
         <v>201</v>
       </c>
-      <c r="K29" t="s">
-        <v>202</v>
-      </c>
       <c r="L29" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30">
@@ -3421,13 +3418,13 @@
         <v>20253892</v>
       </c>
       <c r="B30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C30" t="s">
         <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E30" t="s">
         <v>182</v>
@@ -3436,22 +3433,22 @@
         <v>16</v>
       </c>
       <c r="G30" t="s">
+        <v>204</v>
+      </c>
+      <c r="H30" t="s">
         <v>205</v>
-      </c>
-      <c r="H30" t="s">
-        <v>206</v>
       </c>
       <c r="I30" t="s">
         <v>68</v>
       </c>
       <c r="J30" t="s">
+        <v>206</v>
+      </c>
+      <c r="K30" t="s">
         <v>207</v>
       </c>
-      <c r="K30" t="s">
-        <v>208</v>
-      </c>
       <c r="L30" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31">
@@ -3459,13 +3456,13 @@
         <v>20253893</v>
       </c>
       <c r="B31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C31" t="s">
         <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E31" t="s">
         <v>182</v>
@@ -3474,22 +3471,22 @@
         <v>16</v>
       </c>
       <c r="G31" t="s">
+        <v>210</v>
+      </c>
+      <c r="H31" t="s">
         <v>211</v>
-      </c>
-      <c r="H31" t="s">
-        <v>212</v>
       </c>
       <c r="I31" t="s">
         <v>68</v>
       </c>
       <c r="J31" t="s">
+        <v>212</v>
+      </c>
+      <c r="K31" t="s">
         <v>213</v>
       </c>
-      <c r="K31" t="s">
-        <v>214</v>
-      </c>
       <c r="L31" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32">
@@ -3497,37 +3494,37 @@
         <v>20253730</v>
       </c>
       <c r="B32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C32" t="s">
         <v>13</v>
       </c>
       <c r="D32" t="s">
+        <v>215</v>
+      </c>
+      <c r="E32" t="s">
         <v>216</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" t="s">
         <v>217</v>
       </c>
-      <c r="F32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>218</v>
-      </c>
-      <c r="H32" t="s">
-        <v>219</v>
       </c>
       <c r="I32" t="s">
         <v>68</v>
       </c>
       <c r="J32" t="s">
+        <v>219</v>
+      </c>
+      <c r="K32" t="s">
         <v>220</v>
       </c>
-      <c r="K32" t="s">
-        <v>221</v>
-      </c>
       <c r="L32" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33">
@@ -3535,37 +3532,37 @@
         <v>20253630</v>
       </c>
       <c r="B33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C33" t="s">
         <v>32</v>
       </c>
       <c r="D33" t="s">
+        <v>222</v>
+      </c>
+      <c r="E33" t="s">
         <v>223</v>
-      </c>
-      <c r="E33" t="s">
-        <v>224</v>
       </c>
       <c r="F33" t="s">
         <v>26</v>
       </c>
       <c r="G33" t="s">
+        <v>224</v>
+      </c>
+      <c r="H33" t="s">
         <v>225</v>
-      </c>
-      <c r="H33" t="s">
-        <v>226</v>
       </c>
       <c r="I33" t="s">
         <v>44</v>
       </c>
       <c r="J33" t="s">
+        <v>226</v>
+      </c>
+      <c r="K33" t="s">
         <v>227</v>
       </c>
-      <c r="K33" t="s">
-        <v>228</v>
-      </c>
       <c r="L33" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34">
@@ -3573,37 +3570,37 @@
         <v>20253637</v>
       </c>
       <c r="B34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F34" t="s">
         <v>26</v>
       </c>
       <c r="G34" t="s">
+        <v>230</v>
+      </c>
+      <c r="H34" t="s">
         <v>231</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>232</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>233</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>234</v>
       </c>
-      <c r="K34" t="s">
-        <v>235</v>
-      </c>
       <c r="L34" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35">
@@ -3611,37 +3608,37 @@
         <v>20257355</v>
       </c>
       <c r="B35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C35" t="s">
         <v>39</v>
       </c>
       <c r="D35" t="s">
+        <v>236</v>
+      </c>
+      <c r="E35" t="s">
         <v>237</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" t="s">
         <v>238</v>
       </c>
-      <c r="F35" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>239</v>
-      </c>
-      <c r="H35" t="s">
-        <v>240</v>
       </c>
       <c r="I35" t="s">
         <v>44</v>
       </c>
       <c r="J35" t="s">
+        <v>240</v>
+      </c>
+      <c r="K35" t="s">
         <v>241</v>
       </c>
-      <c r="K35" t="s">
-        <v>242</v>
-      </c>
       <c r="L35" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36">
@@ -3649,37 +3646,37 @@
         <v>20257419</v>
       </c>
       <c r="B36" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C36" t="s">
         <v>39</v>
       </c>
       <c r="D36" t="s">
+        <v>243</v>
+      </c>
+      <c r="E36" t="s">
+        <v>237</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" t="s">
         <v>244</v>
       </c>
-      <c r="E36" t="s">
-        <v>238</v>
-      </c>
-      <c r="F36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>245</v>
-      </c>
-      <c r="H36" t="s">
-        <v>246</v>
       </c>
       <c r="I36" t="s">
         <v>44</v>
       </c>
       <c r="J36" t="s">
+        <v>246</v>
+      </c>
+      <c r="K36" t="s">
         <v>247</v>
       </c>
-      <c r="K36" t="s">
-        <v>248</v>
-      </c>
       <c r="L36" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37">
@@ -3687,37 +3684,37 @@
         <v>20253479</v>
       </c>
       <c r="B37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C37" t="s">
         <v>32</v>
       </c>
       <c r="D37" t="s">
+        <v>249</v>
+      </c>
+      <c r="E37" t="s">
         <v>250</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" t="s">
         <v>251</v>
       </c>
-      <c r="F37" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>252</v>
-      </c>
-      <c r="H37" t="s">
-        <v>253</v>
       </c>
       <c r="I37" t="s">
         <v>68</v>
       </c>
       <c r="J37" t="s">
+        <v>253</v>
+      </c>
+      <c r="K37" t="s">
         <v>254</v>
       </c>
-      <c r="K37" t="s">
-        <v>255</v>
-      </c>
       <c r="L37" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38">
@@ -3725,37 +3722,37 @@
         <v>20253444</v>
       </c>
       <c r="B38" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
       </c>
       <c r="D38" t="s">
+        <v>256</v>
+      </c>
+      <c r="E38" t="s">
         <v>257</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" t="s">
         <v>258</v>
       </c>
-      <c r="F38" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>259</v>
-      </c>
-      <c r="H38" t="s">
-        <v>260</v>
       </c>
       <c r="I38" t="s">
         <v>68</v>
       </c>
       <c r="J38" t="s">
+        <v>260</v>
+      </c>
+      <c r="K38" t="s">
         <v>261</v>
       </c>
-      <c r="K38" t="s">
-        <v>262</v>
-      </c>
       <c r="L38" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39">
@@ -3763,35 +3760,35 @@
         <v>20253425</v>
       </c>
       <c r="B39" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C39" t="s">
         <v>13</v>
       </c>
       <c r="D39"/>
       <c r="E39" t="s">
+        <v>263</v>
+      </c>
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" t="s">
         <v>264</v>
       </c>
-      <c r="F39" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>265</v>
-      </c>
-      <c r="H39" t="s">
-        <v>266</v>
       </c>
       <c r="I39" t="s">
         <v>68</v>
       </c>
       <c r="J39" t="s">
+        <v>266</v>
+      </c>
+      <c r="K39" t="s">
         <v>267</v>
       </c>
-      <c r="K39" t="s">
-        <v>268</v>
-      </c>
       <c r="L39" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40">
@@ -3799,7 +3796,7 @@
         <v>20253309</v>
       </c>
       <c r="B40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C40" t="s">
         <v>13</v>
@@ -3808,28 +3805,28 @@
         <v>124</v>
       </c>
       <c r="E40" t="s">
+        <v>269</v>
+      </c>
+      <c r="F40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" t="s">
         <v>270</v>
       </c>
-      <c r="F40" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>271</v>
-      </c>
-      <c r="H40" t="s">
-        <v>272</v>
       </c>
       <c r="I40" t="s">
         <v>68</v>
       </c>
       <c r="J40" t="s">
+        <v>272</v>
+      </c>
+      <c r="K40" t="s">
         <v>273</v>
       </c>
-      <c r="K40" t="s">
-        <v>274</v>
-      </c>
       <c r="L40" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41">
@@ -3837,37 +3834,37 @@
         <v>20253399</v>
       </c>
       <c r="B41" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C41" t="s">
         <v>32</v>
       </c>
       <c r="D41" t="s">
+        <v>275</v>
+      </c>
+      <c r="E41" t="s">
+        <v>269</v>
+      </c>
+      <c r="F41" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" t="s">
         <v>276</v>
       </c>
-      <c r="E41" t="s">
-        <v>270</v>
-      </c>
-      <c r="F41" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>277</v>
-      </c>
-      <c r="H41" t="s">
-        <v>278</v>
       </c>
       <c r="I41" t="s">
         <v>68</v>
       </c>
       <c r="J41" t="s">
+        <v>278</v>
+      </c>
+      <c r="K41" t="s">
         <v>279</v>
       </c>
-      <c r="K41" t="s">
-        <v>280</v>
-      </c>
       <c r="L41" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42">
@@ -3875,37 +3872,37 @@
         <v>20253404</v>
       </c>
       <c r="B42" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C42" t="s">
         <v>13</v>
       </c>
       <c r="D42" t="s">
+        <v>281</v>
+      </c>
+      <c r="E42" t="s">
+        <v>269</v>
+      </c>
+      <c r="F42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" t="s">
         <v>282</v>
       </c>
-      <c r="E42" t="s">
-        <v>270</v>
-      </c>
-      <c r="F42" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>283</v>
-      </c>
-      <c r="H42" t="s">
-        <v>284</v>
       </c>
       <c r="I42" t="s">
         <v>68</v>
       </c>
       <c r="J42" t="s">
+        <v>284</v>
+      </c>
+      <c r="K42" t="s">
         <v>285</v>
       </c>
-      <c r="K42" t="s">
-        <v>286</v>
-      </c>
       <c r="L42" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43">
@@ -3913,37 +3910,37 @@
         <v>20253417</v>
       </c>
       <c r="B43" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C43" t="s">
         <v>13</v>
       </c>
       <c r="D43" t="s">
+        <v>287</v>
+      </c>
+      <c r="E43" t="s">
+        <v>269</v>
+      </c>
+      <c r="F43" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" t="s">
         <v>288</v>
       </c>
-      <c r="E43" t="s">
-        <v>270</v>
-      </c>
-      <c r="F43" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>289</v>
-      </c>
-      <c r="H43" t="s">
-        <v>290</v>
       </c>
       <c r="I43" t="s">
         <v>68</v>
       </c>
       <c r="J43" t="s">
+        <v>290</v>
+      </c>
+      <c r="K43" t="s">
         <v>291</v>
       </c>
-      <c r="K43" t="s">
-        <v>292</v>
-      </c>
       <c r="L43" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44">
@@ -3951,37 +3948,37 @@
         <v>20251011</v>
       </c>
       <c r="B44" t="s">
+        <v>292</v>
+      </c>
+      <c r="C44" t="s">
         <v>293</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>294</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>295</v>
-      </c>
-      <c r="E44" t="s">
-        <v>296</v>
       </c>
       <c r="F44" t="s">
         <v>26</v>
       </c>
       <c r="G44" t="s">
+        <v>296</v>
+      </c>
+      <c r="H44" t="s">
         <v>297</v>
-      </c>
-      <c r="H44" t="s">
-        <v>298</v>
       </c>
       <c r="I44" t="s">
         <v>44</v>
       </c>
       <c r="J44" t="s">
+        <v>298</v>
+      </c>
+      <c r="K44" t="s">
         <v>299</v>
       </c>
-      <c r="K44" t="s">
-        <v>300</v>
-      </c>
       <c r="L44" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45">
@@ -3989,37 +3986,37 @@
         <v>20253194</v>
       </c>
       <c r="B45" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C45" t="s">
         <v>32</v>
       </c>
       <c r="D45" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E45" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F45" t="s">
         <v>26</v>
       </c>
       <c r="G45" t="s">
+        <v>302</v>
+      </c>
+      <c r="H45" t="s">
         <v>303</v>
-      </c>
-      <c r="H45" t="s">
-        <v>304</v>
       </c>
       <c r="I45" t="s">
         <v>44</v>
       </c>
       <c r="J45" t="s">
+        <v>304</v>
+      </c>
+      <c r="K45" t="s">
         <v>305</v>
       </c>
-      <c r="K45" t="s">
-        <v>306</v>
-      </c>
       <c r="L45" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46">
@@ -4027,37 +4024,37 @@
         <v>20253203</v>
       </c>
       <c r="B46" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C46" t="s">
         <v>32</v>
       </c>
       <c r="D46" t="s">
+        <v>307</v>
+      </c>
+      <c r="E46" t="s">
+        <v>295</v>
+      </c>
+      <c r="F46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" t="s">
         <v>308</v>
       </c>
-      <c r="E46" t="s">
-        <v>296</v>
-      </c>
-      <c r="F46" t="s">
-        <v>16</v>
-      </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>309</v>
-      </c>
-      <c r="H46" t="s">
-        <v>310</v>
       </c>
       <c r="I46" t="s">
         <v>44</v>
       </c>
       <c r="J46" t="s">
+        <v>310</v>
+      </c>
+      <c r="K46" t="s">
         <v>311</v>
       </c>
-      <c r="K46" t="s">
-        <v>312</v>
-      </c>
       <c r="L46" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47">
@@ -4065,37 +4062,37 @@
         <v>20253213</v>
       </c>
       <c r="B47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C47" t="s">
         <v>32</v>
       </c>
       <c r="D47" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F47" t="s">
         <v>26</v>
       </c>
       <c r="G47" t="s">
+        <v>314</v>
+      </c>
+      <c r="H47" t="s">
         <v>315</v>
-      </c>
-      <c r="H47" t="s">
-        <v>316</v>
       </c>
       <c r="I47" t="s">
         <v>44</v>
       </c>
       <c r="J47" t="s">
+        <v>316</v>
+      </c>
+      <c r="K47" t="s">
         <v>317</v>
       </c>
-      <c r="K47" t="s">
-        <v>318</v>
-      </c>
       <c r="L47" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48">
@@ -4103,37 +4100,37 @@
         <v>20253214</v>
       </c>
       <c r="B48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C48" t="s">
         <v>32</v>
       </c>
       <c r="D48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E48" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F48" t="s">
         <v>16</v>
       </c>
       <c r="G48" t="s">
+        <v>319</v>
+      </c>
+      <c r="H48" t="s">
         <v>320</v>
-      </c>
-      <c r="H48" t="s">
-        <v>321</v>
       </c>
       <c r="I48" t="s">
         <v>44</v>
       </c>
       <c r="J48" t="s">
+        <v>321</v>
+      </c>
+      <c r="K48" t="s">
         <v>322</v>
       </c>
-      <c r="K48" t="s">
-        <v>323</v>
-      </c>
       <c r="L48" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49">
@@ -4141,37 +4138,37 @@
         <v>20253246</v>
       </c>
       <c r="B49" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C49" t="s">
         <v>13</v>
       </c>
       <c r="D49" t="s">
+        <v>324</v>
+      </c>
+      <c r="E49" t="s">
+        <v>295</v>
+      </c>
+      <c r="F49" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" t="s">
         <v>325</v>
       </c>
-      <c r="E49" t="s">
-        <v>296</v>
-      </c>
-      <c r="F49" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>326</v>
-      </c>
-      <c r="H49" t="s">
-        <v>327</v>
       </c>
       <c r="I49" t="s">
         <v>145</v>
       </c>
       <c r="J49" t="s">
+        <v>327</v>
+      </c>
+      <c r="K49" t="s">
         <v>328</v>
       </c>
-      <c r="K49" t="s">
-        <v>329</v>
-      </c>
       <c r="L49" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50">
@@ -4179,37 +4176,37 @@
         <v>20253093</v>
       </c>
       <c r="B50" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C50" t="s">
         <v>32</v>
       </c>
       <c r="D50" t="s">
+        <v>330</v>
+      </c>
+      <c r="E50" t="s">
         <v>331</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" t="s">
         <v>332</v>
       </c>
-      <c r="F50" t="s">
-        <v>16</v>
-      </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>333</v>
-      </c>
-      <c r="H50" t="s">
-        <v>334</v>
       </c>
       <c r="I50" t="s">
         <v>68</v>
       </c>
       <c r="J50" t="s">
+        <v>334</v>
+      </c>
+      <c r="K50" t="s">
         <v>335</v>
       </c>
-      <c r="K50" t="s">
-        <v>336</v>
-      </c>
       <c r="L50" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51">
@@ -4217,37 +4214,37 @@
         <v>20257213</v>
       </c>
       <c r="B51" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C51" t="s">
         <v>39</v>
       </c>
       <c r="D51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E51" t="s">
+        <v>337</v>
+      </c>
+      <c r="F51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" t="s">
         <v>338</v>
       </c>
-      <c r="F51" t="s">
-        <v>16</v>
-      </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>339</v>
-      </c>
-      <c r="H51" t="s">
-        <v>340</v>
       </c>
       <c r="I51" t="s">
         <v>44</v>
       </c>
       <c r="J51" t="s">
+        <v>340</v>
+      </c>
+      <c r="K51" t="s">
         <v>341</v>
       </c>
-      <c r="K51" t="s">
-        <v>342</v>
-      </c>
       <c r="L51" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52">
@@ -4255,37 +4252,37 @@
         <v>20253054</v>
       </c>
       <c r="B52" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C52" t="s">
         <v>13</v>
       </c>
       <c r="D52" t="s">
+        <v>343</v>
+      </c>
+      <c r="E52" t="s">
         <v>344</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" t="s">
         <v>345</v>
       </c>
-      <c r="F52" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>346</v>
-      </c>
-      <c r="H52" t="s">
-        <v>347</v>
       </c>
       <c r="I52" t="s">
         <v>68</v>
       </c>
       <c r="J52" t="s">
+        <v>347</v>
+      </c>
+      <c r="K52" t="s">
         <v>348</v>
       </c>
-      <c r="K52" t="s">
-        <v>349</v>
-      </c>
       <c r="L52" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53">
@@ -4293,7 +4290,7 @@
         <v>20257102</v>
       </c>
       <c r="B53" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C53" t="s">
         <v>39</v>
@@ -4302,28 +4299,28 @@
         <v>111</v>
       </c>
       <c r="E53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F53" t="s">
         <v>16</v>
       </c>
       <c r="G53" t="s">
+        <v>350</v>
+      </c>
+      <c r="H53" t="s">
         <v>351</v>
-      </c>
-      <c r="H53" t="s">
-        <v>352</v>
       </c>
       <c r="I53" t="s">
         <v>44</v>
       </c>
       <c r="J53" t="s">
+        <v>352</v>
+      </c>
+      <c r="K53" t="s">
         <v>353</v>
       </c>
-      <c r="K53" t="s">
-        <v>354</v>
-      </c>
       <c r="L53" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54">
@@ -4331,37 +4328,37 @@
         <v>20257129</v>
       </c>
       <c r="B54" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C54" t="s">
         <v>39</v>
       </c>
       <c r="D54" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E54" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F54" t="s">
         <v>16</v>
       </c>
       <c r="G54" t="s">
+        <v>355</v>
+      </c>
+      <c r="H54" t="s">
         <v>356</v>
-      </c>
-      <c r="H54" t="s">
-        <v>357</v>
       </c>
       <c r="I54" t="s">
         <v>44</v>
       </c>
       <c r="J54" t="s">
+        <v>357</v>
+      </c>
+      <c r="K54" t="s">
         <v>358</v>
       </c>
-      <c r="K54" t="s">
-        <v>359</v>
-      </c>
       <c r="L54" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55">
@@ -4369,37 +4366,37 @@
         <v>20257138</v>
       </c>
       <c r="B55" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C55" t="s">
         <v>39</v>
       </c>
       <c r="D55" t="s">
+        <v>360</v>
+      </c>
+      <c r="E55" t="s">
+        <v>344</v>
+      </c>
+      <c r="F55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" t="s">
         <v>361</v>
       </c>
-      <c r="E55" t="s">
-        <v>345</v>
-      </c>
-      <c r="F55" t="s">
-        <v>16</v>
-      </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>362</v>
-      </c>
-      <c r="H55" t="s">
-        <v>363</v>
       </c>
       <c r="I55" t="s">
         <v>44</v>
       </c>
       <c r="J55" t="s">
+        <v>363</v>
+      </c>
+      <c r="K55" t="s">
         <v>364</v>
       </c>
-      <c r="K55" t="s">
-        <v>365</v>
-      </c>
       <c r="L55" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56">
@@ -4407,37 +4404,37 @@
         <v>20253031</v>
       </c>
       <c r="B56" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C56" t="s">
         <v>32</v>
       </c>
       <c r="D56" t="s">
+        <v>366</v>
+      </c>
+      <c r="E56" t="s">
         <v>367</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" t="s">
         <v>368</v>
       </c>
-      <c r="F56" t="s">
-        <v>16</v>
-      </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>369</v>
-      </c>
-      <c r="H56" t="s">
-        <v>370</v>
       </c>
       <c r="I56" t="s">
         <v>68</v>
       </c>
       <c r="J56" t="s">
+        <v>370</v>
+      </c>
+      <c r="K56" t="s">
         <v>371</v>
       </c>
-      <c r="K56" t="s">
-        <v>372</v>
-      </c>
       <c r="L56" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57">
@@ -4445,37 +4442,37 @@
         <v>20257012</v>
       </c>
       <c r="B57" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C57" t="s">
         <v>39</v>
       </c>
       <c r="D57" t="s">
+        <v>373</v>
+      </c>
+      <c r="E57" t="s">
+        <v>367</v>
+      </c>
+      <c r="F57" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" t="s">
         <v>374</v>
       </c>
-      <c r="E57" t="s">
-        <v>368</v>
-      </c>
-      <c r="F57" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>375</v>
-      </c>
-      <c r="H57" t="s">
-        <v>376</v>
       </c>
       <c r="I57" t="s">
         <v>44</v>
       </c>
       <c r="J57" t="s">
+        <v>376</v>
+      </c>
+      <c r="K57" t="s">
         <v>377</v>
       </c>
-      <c r="K57" t="s">
-        <v>378</v>
-      </c>
       <c r="L57" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58">
@@ -4483,35 +4480,35 @@
         <v>20253008</v>
       </c>
       <c r="B58" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C58" t="s">
         <v>13</v>
       </c>
       <c r="D58"/>
       <c r="E58" t="s">
+        <v>379</v>
+      </c>
+      <c r="F58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" t="s">
         <v>380</v>
       </c>
-      <c r="F58" t="s">
-        <v>16</v>
-      </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>381</v>
-      </c>
-      <c r="H58" t="s">
-        <v>382</v>
       </c>
       <c r="I58" t="s">
         <v>44</v>
       </c>
       <c r="J58" t="s">
+        <v>382</v>
+      </c>
+      <c r="K58" t="s">
         <v>383</v>
       </c>
-      <c r="K58" t="s">
-        <v>384</v>
-      </c>
       <c r="L58" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59">
@@ -4519,37 +4516,37 @@
         <v>20244404</v>
       </c>
       <c r="B59" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C59" t="s">
         <v>32</v>
       </c>
       <c r="D59" t="s">
+        <v>385</v>
+      </c>
+      <c r="E59" t="s">
         <v>386</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" t="s">
         <v>387</v>
       </c>
-      <c r="F59" t="s">
-        <v>16</v>
-      </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>388</v>
-      </c>
-      <c r="H59" t="s">
-        <v>389</v>
       </c>
       <c r="I59" t="s">
         <v>44</v>
       </c>
       <c r="J59" t="s">
+        <v>389</v>
+      </c>
+      <c r="K59" t="s">
         <v>390</v>
       </c>
-      <c r="K59" t="s">
-        <v>391</v>
-      </c>
       <c r="L59" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60">
@@ -4557,37 +4554,37 @@
         <v>20244419</v>
       </c>
       <c r="B60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C60" t="s">
         <v>32</v>
       </c>
       <c r="D60" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E60" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F60" t="s">
         <v>26</v>
       </c>
       <c r="G60" t="s">
+        <v>392</v>
+      </c>
+      <c r="H60" t="s">
         <v>393</v>
-      </c>
-      <c r="H60" t="s">
-        <v>394</v>
       </c>
       <c r="I60" t="s">
         <v>44</v>
       </c>
       <c r="J60" t="s">
+        <v>394</v>
+      </c>
+      <c r="K60" t="s">
         <v>395</v>
       </c>
-      <c r="K60" t="s">
-        <v>396</v>
-      </c>
       <c r="L60" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61">
@@ -4595,37 +4592,37 @@
         <v>20247975</v>
       </c>
       <c r="B61" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C61" t="s">
         <v>39</v>
       </c>
       <c r="D61" t="s">
+        <v>397</v>
+      </c>
+      <c r="E61" t="s">
         <v>398</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" t="s">
         <v>399</v>
       </c>
-      <c r="F61" t="s">
-        <v>16</v>
-      </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>400</v>
-      </c>
-      <c r="H61" t="s">
-        <v>401</v>
       </c>
       <c r="I61" t="s">
         <v>44</v>
       </c>
       <c r="J61" t="s">
+        <v>401</v>
+      </c>
+      <c r="K61" t="s">
         <v>402</v>
       </c>
-      <c r="K61" t="s">
-        <v>403</v>
-      </c>
       <c r="L61" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62">
@@ -4633,37 +4630,37 @@
         <v>20248043</v>
       </c>
       <c r="B62" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C62" t="s">
         <v>39</v>
       </c>
       <c r="D62" t="s">
+        <v>404</v>
+      </c>
+      <c r="E62" t="s">
+        <v>398</v>
+      </c>
+      <c r="F62" t="s">
+        <v>16</v>
+      </c>
+      <c r="G62" t="s">
         <v>405</v>
       </c>
-      <c r="E62" t="s">
-        <v>399</v>
-      </c>
-      <c r="F62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>406</v>
-      </c>
-      <c r="H62" t="s">
-        <v>407</v>
       </c>
       <c r="I62" t="s">
         <v>44</v>
       </c>
       <c r="J62" t="s">
+        <v>407</v>
+      </c>
+      <c r="K62" t="s">
         <v>408</v>
       </c>
-      <c r="K62" t="s">
-        <v>409</v>
-      </c>
       <c r="L62" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63">
@@ -4671,37 +4668,37 @@
         <v>20244290</v>
       </c>
       <c r="B63" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C63" t="s">
         <v>32</v>
       </c>
       <c r="D63" t="s">
+        <v>410</v>
+      </c>
+      <c r="E63" t="s">
         <v>411</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" t="s">
         <v>412</v>
       </c>
-      <c r="F63" t="s">
-        <v>16</v>
-      </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>413</v>
-      </c>
-      <c r="H63" t="s">
-        <v>414</v>
       </c>
       <c r="I63" t="s">
         <v>68</v>
       </c>
       <c r="J63" t="s">
+        <v>414</v>
+      </c>
+      <c r="K63" t="s">
         <v>415</v>
       </c>
-      <c r="K63" t="s">
-        <v>416</v>
-      </c>
       <c r="L63" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64">
@@ -4709,37 +4706,37 @@
         <v>20244278</v>
       </c>
       <c r="B64" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C64" t="s">
         <v>32</v>
       </c>
       <c r="D64" t="s">
+        <v>417</v>
+      </c>
+      <c r="E64" t="s">
         <v>418</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" t="s">
         <v>419</v>
       </c>
-      <c r="F64" t="s">
-        <v>16</v>
-      </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>420</v>
-      </c>
-      <c r="H64" t="s">
-        <v>421</v>
       </c>
       <c r="I64" t="s">
         <v>68</v>
       </c>
       <c r="J64" t="s">
+        <v>421</v>
+      </c>
+      <c r="K64" t="s">
         <v>422</v>
       </c>
-      <c r="K64" t="s">
-        <v>423</v>
-      </c>
       <c r="L64" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65">
@@ -4747,37 +4744,37 @@
         <v>20244082</v>
       </c>
       <c r="B65" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C65" t="s">
         <v>32</v>
       </c>
       <c r="D65" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E65" t="s">
+        <v>424</v>
+      </c>
+      <c r="F65" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" t="s">
         <v>425</v>
       </c>
-      <c r="F65" t="s">
-        <v>16</v>
-      </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>426</v>
-      </c>
-      <c r="H65" t="s">
-        <v>427</v>
       </c>
       <c r="I65" t="s">
         <v>68</v>
       </c>
       <c r="J65" t="s">
+        <v>427</v>
+      </c>
+      <c r="K65" t="s">
         <v>428</v>
       </c>
-      <c r="K65" t="s">
-        <v>429</v>
-      </c>
       <c r="L65" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66">
@@ -4785,37 +4782,37 @@
         <v>20244112</v>
       </c>
       <c r="B66" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C66" t="s">
         <v>32</v>
       </c>
       <c r="D66" t="s">
+        <v>430</v>
+      </c>
+      <c r="E66" t="s">
+        <v>424</v>
+      </c>
+      <c r="F66" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" t="s">
         <v>431</v>
       </c>
-      <c r="E66" t="s">
-        <v>425</v>
-      </c>
-      <c r="F66" t="s">
-        <v>16</v>
-      </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>432</v>
-      </c>
-      <c r="H66" t="s">
-        <v>433</v>
       </c>
       <c r="I66" t="s">
         <v>68</v>
       </c>
       <c r="J66" t="s">
+        <v>433</v>
+      </c>
+      <c r="K66" t="s">
         <v>434</v>
       </c>
-      <c r="K66" t="s">
-        <v>435</v>
-      </c>
       <c r="L66" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67">
@@ -4823,7 +4820,7 @@
         <v>20244131</v>
       </c>
       <c r="B67" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C67" t="s">
         <v>32</v>
@@ -4832,28 +4829,28 @@
         <v>49</v>
       </c>
       <c r="E67" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F67" t="s">
         <v>16</v>
       </c>
       <c r="G67" t="s">
+        <v>436</v>
+      </c>
+      <c r="H67" t="s">
         <v>437</v>
-      </c>
-      <c r="H67" t="s">
-        <v>438</v>
       </c>
       <c r="I67" t="s">
         <v>68</v>
       </c>
       <c r="J67" t="s">
+        <v>438</v>
+      </c>
+      <c r="K67" t="s">
         <v>439</v>
       </c>
-      <c r="K67" t="s">
-        <v>440</v>
-      </c>
       <c r="L67" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68">
@@ -4861,7 +4858,7 @@
         <v>20244132</v>
       </c>
       <c r="B68" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C68" t="s">
         <v>63</v>
@@ -4870,28 +4867,28 @@
         <v>124</v>
       </c>
       <c r="E68" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F68" t="s">
         <v>16</v>
       </c>
       <c r="G68" t="s">
+        <v>441</v>
+      </c>
+      <c r="H68" t="s">
         <v>442</v>
-      </c>
-      <c r="H68" t="s">
-        <v>443</v>
       </c>
       <c r="I68" t="s">
         <v>68</v>
       </c>
       <c r="J68" t="s">
+        <v>443</v>
+      </c>
+      <c r="K68" t="s">
         <v>444</v>
       </c>
-      <c r="K68" t="s">
-        <v>445</v>
-      </c>
       <c r="L68" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69">
@@ -4899,7 +4896,7 @@
         <v>20244133</v>
       </c>
       <c r="B69" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C69" t="s">
         <v>13</v>
@@ -4908,28 +4905,28 @@
         <v>124</v>
       </c>
       <c r="E69" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F69" t="s">
         <v>16</v>
       </c>
       <c r="G69" t="s">
+        <v>446</v>
+      </c>
+      <c r="H69" t="s">
         <v>447</v>
-      </c>
-      <c r="H69" t="s">
-        <v>448</v>
       </c>
       <c r="I69" t="s">
         <v>68</v>
       </c>
       <c r="J69" t="s">
+        <v>448</v>
+      </c>
+      <c r="K69" t="s">
         <v>449</v>
       </c>
-      <c r="K69" t="s">
-        <v>450</v>
-      </c>
       <c r="L69" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70">
@@ -4937,37 +4934,37 @@
         <v>20244137</v>
       </c>
       <c r="B70" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C70" t="s">
         <v>32</v>
       </c>
       <c r="D70" t="s">
+        <v>451</v>
+      </c>
+      <c r="E70" t="s">
+        <v>424</v>
+      </c>
+      <c r="F70" t="s">
+        <v>16</v>
+      </c>
+      <c r="G70" t="s">
         <v>452</v>
       </c>
-      <c r="E70" t="s">
-        <v>425</v>
-      </c>
-      <c r="F70" t="s">
-        <v>16</v>
-      </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>453</v>
-      </c>
-      <c r="H70" t="s">
-        <v>454</v>
       </c>
       <c r="I70" t="s">
         <v>68</v>
       </c>
       <c r="J70" t="s">
+        <v>454</v>
+      </c>
+      <c r="K70" t="s">
         <v>455</v>
       </c>
-      <c r="K70" t="s">
-        <v>456</v>
-      </c>
       <c r="L70" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71">
@@ -4975,37 +4972,37 @@
         <v>20243937</v>
       </c>
       <c r="B71" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C71" t="s">
         <v>13</v>
       </c>
       <c r="D71" t="s">
+        <v>457</v>
+      </c>
+      <c r="E71" t="s">
         <v>458</v>
-      </c>
-      <c r="E71" t="s">
-        <v>459</v>
       </c>
       <c r="F71" t="s">
         <v>26</v>
       </c>
       <c r="G71" t="s">
+        <v>459</v>
+      </c>
+      <c r="H71" t="s">
         <v>460</v>
-      </c>
-      <c r="H71" t="s">
-        <v>461</v>
       </c>
       <c r="I71" t="s">
         <v>177</v>
       </c>
       <c r="J71" t="s">
+        <v>461</v>
+      </c>
+      <c r="K71" t="s">
         <v>462</v>
       </c>
-      <c r="K71" t="s">
-        <v>463</v>
-      </c>
       <c r="L71" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72">
@@ -5013,37 +5010,37 @@
         <v>20243948</v>
       </c>
       <c r="B72" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C72" t="s">
         <v>32</v>
       </c>
       <c r="D72" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E72" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F72" t="s">
         <v>26</v>
       </c>
       <c r="G72" t="s">
+        <v>465</v>
+      </c>
+      <c r="H72" t="s">
         <v>466</v>
-      </c>
-      <c r="H72" t="s">
-        <v>467</v>
       </c>
       <c r="I72" t="s">
         <v>44</v>
       </c>
       <c r="J72" t="s">
+        <v>467</v>
+      </c>
+      <c r="K72" t="s">
         <v>468</v>
       </c>
-      <c r="K72" t="s">
-        <v>469</v>
-      </c>
       <c r="L72" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73">
@@ -5051,37 +5048,37 @@
         <v>20247720</v>
       </c>
       <c r="B73" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C73" t="s">
         <v>39</v>
       </c>
       <c r="D73" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E73" t="s">
+        <v>470</v>
+      </c>
+      <c r="F73" t="s">
+        <v>16</v>
+      </c>
+      <c r="G73" t="s">
         <v>471</v>
       </c>
-      <c r="F73" t="s">
-        <v>16</v>
-      </c>
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>472</v>
-      </c>
-      <c r="H73" t="s">
-        <v>473</v>
       </c>
       <c r="I73" t="s">
         <v>44</v>
       </c>
       <c r="J73" t="s">
+        <v>473</v>
+      </c>
+      <c r="K73" t="s">
         <v>474</v>
       </c>
-      <c r="K73" t="s">
-        <v>475</v>
-      </c>
       <c r="L73" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74">
@@ -5089,37 +5086,37 @@
         <v>20247726</v>
       </c>
       <c r="B74" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C74" t="s">
         <v>39</v>
       </c>
       <c r="D74" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E74" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F74" t="s">
         <v>16</v>
       </c>
       <c r="G74" t="s">
+        <v>476</v>
+      </c>
+      <c r="H74" t="s">
         <v>477</v>
-      </c>
-      <c r="H74" t="s">
-        <v>478</v>
       </c>
       <c r="I74" t="s">
         <v>44</v>
       </c>
       <c r="J74" t="s">
+        <v>478</v>
+      </c>
+      <c r="K74" t="s">
         <v>479</v>
       </c>
-      <c r="K74" t="s">
-        <v>480</v>
-      </c>
       <c r="L74" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="75">
@@ -5127,7 +5124,7 @@
         <v>20247773</v>
       </c>
       <c r="B75" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C75" t="s">
         <v>39</v>
@@ -5136,28 +5133,28 @@
         <v>118</v>
       </c>
       <c r="E75" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F75" t="s">
         <v>16</v>
       </c>
       <c r="G75" t="s">
+        <v>481</v>
+      </c>
+      <c r="H75" t="s">
         <v>482</v>
-      </c>
-      <c r="H75" t="s">
-        <v>483</v>
       </c>
       <c r="I75" t="s">
         <v>44</v>
       </c>
       <c r="J75" t="s">
+        <v>483</v>
+      </c>
+      <c r="K75" t="s">
         <v>484</v>
       </c>
-      <c r="K75" t="s">
-        <v>485</v>
-      </c>
       <c r="L75" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76">
@@ -5165,7 +5162,7 @@
         <v>20247774</v>
       </c>
       <c r="B76" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C76" t="s">
         <v>39</v>
@@ -5174,28 +5171,28 @@
         <v>118</v>
       </c>
       <c r="E76" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F76" t="s">
         <v>16</v>
       </c>
       <c r="G76" t="s">
+        <v>486</v>
+      </c>
+      <c r="H76" t="s">
         <v>487</v>
-      </c>
-      <c r="H76" t="s">
-        <v>488</v>
       </c>
       <c r="I76" t="s">
         <v>44</v>
       </c>
       <c r="J76" t="s">
+        <v>488</v>
+      </c>
+      <c r="K76" t="s">
         <v>489</v>
       </c>
-      <c r="K76" t="s">
-        <v>490</v>
-      </c>
       <c r="L76" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="77">
@@ -5203,37 +5200,37 @@
         <v>20243858</v>
       </c>
       <c r="B77" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C77" t="s">
         <v>32</v>
       </c>
       <c r="D77" t="s">
+        <v>491</v>
+      </c>
+      <c r="E77" t="s">
         <v>492</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" t="s">
         <v>493</v>
       </c>
-      <c r="F77" t="s">
-        <v>16</v>
-      </c>
-      <c r="G77" t="s">
+      <c r="H77" t="s">
         <v>494</v>
-      </c>
-      <c r="H77" t="s">
-        <v>495</v>
       </c>
       <c r="I77" t="s">
         <v>68</v>
       </c>
       <c r="J77" t="s">
+        <v>495</v>
+      </c>
+      <c r="K77" t="s">
         <v>496</v>
       </c>
-      <c r="K77" t="s">
-        <v>497</v>
-      </c>
       <c r="L77" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="78">
@@ -5241,37 +5238,37 @@
         <v>20243877</v>
       </c>
       <c r="B78" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C78" t="s">
         <v>32</v>
       </c>
       <c r="D78" t="s">
+        <v>498</v>
+      </c>
+      <c r="E78" t="s">
+        <v>492</v>
+      </c>
+      <c r="F78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78" t="s">
         <v>499</v>
       </c>
-      <c r="E78" t="s">
-        <v>493</v>
-      </c>
-      <c r="F78" t="s">
-        <v>16</v>
-      </c>
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>500</v>
-      </c>
-      <c r="H78" t="s">
-        <v>501</v>
       </c>
       <c r="I78" t="s">
         <v>68</v>
       </c>
       <c r="J78" t="s">
+        <v>501</v>
+      </c>
+      <c r="K78" t="s">
         <v>502</v>
       </c>
-      <c r="K78" t="s">
-        <v>503</v>
-      </c>
       <c r="L78" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="79">
@@ -5279,7 +5276,7 @@
         <v>20247622</v>
       </c>
       <c r="B79" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C79" t="s">
         <v>39</v>
@@ -5288,28 +5285,28 @@
         <v>49</v>
       </c>
       <c r="E79" t="s">
+        <v>504</v>
+      </c>
+      <c r="F79" t="s">
+        <v>16</v>
+      </c>
+      <c r="G79" t="s">
         <v>505</v>
       </c>
-      <c r="F79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G79" t="s">
+      <c r="H79" t="s">
         <v>506</v>
-      </c>
-      <c r="H79" t="s">
-        <v>507</v>
       </c>
       <c r="I79" t="s">
         <v>44</v>
       </c>
       <c r="J79" t="s">
+        <v>507</v>
+      </c>
+      <c r="K79" t="s">
         <v>508</v>
       </c>
-      <c r="K79" t="s">
-        <v>509</v>
-      </c>
       <c r="L79" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="80">
@@ -5317,37 +5314,37 @@
         <v>20247649</v>
       </c>
       <c r="B80" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C80" t="s">
         <v>39</v>
       </c>
       <c r="D80" t="s">
+        <v>510</v>
+      </c>
+      <c r="E80" t="s">
+        <v>504</v>
+      </c>
+      <c r="F80" t="s">
+        <v>16</v>
+      </c>
+      <c r="G80" t="s">
         <v>511</v>
       </c>
-      <c r="E80" t="s">
-        <v>505</v>
-      </c>
-      <c r="F80" t="s">
-        <v>16</v>
-      </c>
-      <c r="G80" t="s">
+      <c r="H80" t="s">
         <v>512</v>
-      </c>
-      <c r="H80" t="s">
-        <v>513</v>
       </c>
       <c r="I80" t="s">
         <v>44</v>
       </c>
       <c r="J80" t="s">
+        <v>513</v>
+      </c>
+      <c r="K80" t="s">
         <v>514</v>
       </c>
-      <c r="K80" t="s">
-        <v>515</v>
-      </c>
       <c r="L80" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="81">
@@ -5355,37 +5352,37 @@
         <v>20243709</v>
       </c>
       <c r="B81" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C81" t="s">
         <v>32</v>
       </c>
       <c r="D81" t="s">
+        <v>516</v>
+      </c>
+      <c r="E81" t="s">
         <v>517</v>
       </c>
-      <c r="E81" t="s">
+      <c r="F81" t="s">
+        <v>16</v>
+      </c>
+      <c r="G81" t="s">
         <v>518</v>
       </c>
-      <c r="F81" t="s">
-        <v>16</v>
-      </c>
-      <c r="G81" t="s">
+      <c r="H81" t="s">
         <v>519</v>
-      </c>
-      <c r="H81" t="s">
-        <v>520</v>
       </c>
       <c r="I81" t="s">
         <v>68</v>
       </c>
       <c r="J81" t="s">
+        <v>520</v>
+      </c>
+      <c r="K81" t="s">
         <v>521</v>
       </c>
-      <c r="K81" t="s">
-        <v>522</v>
-      </c>
       <c r="L81" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="82">
@@ -5393,37 +5390,37 @@
         <v>20243773</v>
       </c>
       <c r="B82" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C82" t="s">
         <v>32</v>
       </c>
       <c r="D82" t="s">
+        <v>523</v>
+      </c>
+      <c r="E82" t="s">
+        <v>517</v>
+      </c>
+      <c r="F82" t="s">
+        <v>16</v>
+      </c>
+      <c r="G82" t="s">
         <v>524</v>
       </c>
-      <c r="E82" t="s">
-        <v>518</v>
-      </c>
-      <c r="F82" t="s">
-        <v>16</v>
-      </c>
-      <c r="G82" t="s">
+      <c r="H82" t="s">
         <v>525</v>
-      </c>
-      <c r="H82" t="s">
-        <v>526</v>
       </c>
       <c r="I82" t="s">
         <v>68</v>
       </c>
       <c r="J82" t="s">
+        <v>526</v>
+      </c>
+      <c r="K82" t="s">
         <v>527</v>
       </c>
-      <c r="K82" t="s">
-        <v>528</v>
-      </c>
       <c r="L82" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="83">
@@ -5431,37 +5428,37 @@
         <v>20243776</v>
       </c>
       <c r="B83" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C83" t="s">
         <v>13</v>
       </c>
       <c r="D83" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E83" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F83" t="s">
         <v>16</v>
       </c>
       <c r="G83" t="s">
+        <v>529</v>
+      </c>
+      <c r="H83" t="s">
         <v>530</v>
-      </c>
-      <c r="H83" t="s">
-        <v>531</v>
       </c>
       <c r="I83" t="s">
         <v>44</v>
       </c>
       <c r="J83" t="s">
+        <v>531</v>
+      </c>
+      <c r="K83" t="s">
         <v>532</v>
       </c>
-      <c r="K83" t="s">
-        <v>533</v>
-      </c>
       <c r="L83" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84">
@@ -5469,37 +5466,37 @@
         <v>20243609</v>
       </c>
       <c r="B84" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C84" t="s">
         <v>13</v>
       </c>
       <c r="D84" t="s">
+        <v>534</v>
+      </c>
+      <c r="E84" t="s">
         <v>535</v>
       </c>
-      <c r="E84" t="s">
+      <c r="F84" t="s">
+        <v>16</v>
+      </c>
+      <c r="G84" t="s">
         <v>536</v>
       </c>
-      <c r="F84" t="s">
-        <v>16</v>
-      </c>
-      <c r="G84" t="s">
+      <c r="H84" t="s">
         <v>537</v>
       </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>538</v>
       </c>
-      <c r="I84" t="s">
+      <c r="J84" t="s">
         <v>539</v>
       </c>
-      <c r="J84" t="s">
+      <c r="K84" t="s">
         <v>540</v>
       </c>
-      <c r="K84" t="s">
-        <v>541</v>
-      </c>
       <c r="L84" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="85">
@@ -5507,37 +5504,37 @@
         <v>20243574</v>
       </c>
       <c r="B85" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C85" t="s">
         <v>32</v>
       </c>
       <c r="D85" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E85" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F85" t="s">
         <v>26</v>
       </c>
       <c r="G85" t="s">
+        <v>543</v>
+      </c>
+      <c r="H85" t="s">
         <v>544</v>
-      </c>
-      <c r="H85" t="s">
-        <v>545</v>
       </c>
       <c r="I85" t="s">
         <v>44</v>
       </c>
       <c r="J85" t="s">
+        <v>545</v>
+      </c>
+      <c r="K85" t="s">
         <v>546</v>
       </c>
-      <c r="K85" t="s">
-        <v>547</v>
-      </c>
       <c r="L85" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86">
@@ -5545,37 +5542,37 @@
         <v>20243557</v>
       </c>
       <c r="B86" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C86" t="s">
         <v>32</v>
       </c>
       <c r="D86" t="s">
+        <v>548</v>
+      </c>
+      <c r="E86" t="s">
         <v>549</v>
       </c>
-      <c r="E86" t="s">
+      <c r="F86" t="s">
+        <v>16</v>
+      </c>
+      <c r="G86" t="s">
         <v>550</v>
       </c>
-      <c r="F86" t="s">
-        <v>16</v>
-      </c>
-      <c r="G86" t="s">
+      <c r="H86" t="s">
         <v>551</v>
-      </c>
-      <c r="H86" t="s">
-        <v>552</v>
       </c>
       <c r="I86" t="s">
         <v>44</v>
       </c>
       <c r="J86" t="s">
+        <v>552</v>
+      </c>
+      <c r="K86" t="s">
         <v>553</v>
       </c>
-      <c r="K86" t="s">
-        <v>554</v>
-      </c>
       <c r="L86" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="87">
@@ -5583,35 +5580,35 @@
         <v>20243471</v>
       </c>
       <c r="B87" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C87" t="s">
         <v>13</v>
       </c>
       <c r="D87"/>
       <c r="E87" t="s">
+        <v>555</v>
+      </c>
+      <c r="F87" t="s">
+        <v>16</v>
+      </c>
+      <c r="G87" t="s">
         <v>556</v>
       </c>
-      <c r="F87" t="s">
-        <v>16</v>
-      </c>
-      <c r="G87" t="s">
+      <c r="H87" t="s">
         <v>557</v>
-      </c>
-      <c r="H87" t="s">
-        <v>558</v>
       </c>
       <c r="I87" t="s">
         <v>44</v>
       </c>
       <c r="J87" t="s">
+        <v>558</v>
+      </c>
+      <c r="K87" t="s">
         <v>559</v>
       </c>
-      <c r="K87" t="s">
-        <v>560</v>
-      </c>
       <c r="L87" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88">
@@ -5619,35 +5616,35 @@
         <v>20243468</v>
       </c>
       <c r="B88" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C88" t="s">
         <v>63</v>
       </c>
       <c r="D88"/>
       <c r="E88" t="s">
+        <v>561</v>
+      </c>
+      <c r="F88" t="s">
+        <v>16</v>
+      </c>
+      <c r="G88" t="s">
         <v>562</v>
       </c>
-      <c r="F88" t="s">
-        <v>16</v>
-      </c>
-      <c r="G88" t="s">
+      <c r="H88" t="s">
         <v>563</v>
-      </c>
-      <c r="H88" t="s">
-        <v>564</v>
       </c>
       <c r="I88" t="s">
         <v>177</v>
       </c>
       <c r="J88" t="s">
+        <v>564</v>
+      </c>
+      <c r="K88" t="s">
         <v>565</v>
       </c>
-      <c r="K88" t="s">
-        <v>566</v>
-      </c>
       <c r="L88" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="89">
@@ -5655,35 +5652,35 @@
         <v>20243467</v>
       </c>
       <c r="B89" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C89" t="s">
         <v>13</v>
       </c>
       <c r="D89"/>
       <c r="E89" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F89" t="s">
         <v>26</v>
       </c>
       <c r="G89" t="s">
+        <v>568</v>
+      </c>
+      <c r="H89" t="s">
         <v>569</v>
-      </c>
-      <c r="H89" t="s">
-        <v>570</v>
       </c>
       <c r="I89" t="s">
         <v>44</v>
       </c>
       <c r="J89" t="s">
+        <v>570</v>
+      </c>
+      <c r="K89" t="s">
         <v>571</v>
       </c>
-      <c r="K89" t="s">
-        <v>572</v>
-      </c>
       <c r="L89" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="90">
@@ -5691,37 +5688,37 @@
         <v>20243318</v>
       </c>
       <c r="B90" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C90" t="s">
         <v>32</v>
       </c>
       <c r="D90" t="s">
+        <v>573</v>
+      </c>
+      <c r="E90" t="s">
         <v>574</v>
       </c>
-      <c r="E90" t="s">
+      <c r="F90" t="s">
+        <v>16</v>
+      </c>
+      <c r="G90" t="s">
         <v>575</v>
       </c>
-      <c r="F90" t="s">
-        <v>16</v>
-      </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>576</v>
-      </c>
-      <c r="H90" t="s">
-        <v>577</v>
       </c>
       <c r="I90" t="s">
         <v>68</v>
       </c>
       <c r="J90" t="s">
+        <v>577</v>
+      </c>
+      <c r="K90" t="s">
         <v>578</v>
       </c>
-      <c r="K90" t="s">
-        <v>579</v>
-      </c>
       <c r="L90" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="91">
@@ -5729,37 +5726,37 @@
         <v>20243234</v>
       </c>
       <c r="B91" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C91" t="s">
         <v>13</v>
       </c>
       <c r="D91" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E91" t="s">
+        <v>580</v>
+      </c>
+      <c r="F91" t="s">
+        <v>16</v>
+      </c>
+      <c r="G91" t="s">
         <v>581</v>
       </c>
-      <c r="F91" t="s">
-        <v>16</v>
-      </c>
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>582</v>
-      </c>
-      <c r="H91" t="s">
-        <v>583</v>
       </c>
       <c r="I91" t="s">
         <v>44</v>
       </c>
       <c r="J91" t="s">
+        <v>583</v>
+      </c>
+      <c r="K91" t="s">
         <v>584</v>
       </c>
-      <c r="K91" t="s">
-        <v>585</v>
-      </c>
       <c r="L91" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="92">
@@ -5767,37 +5764,37 @@
         <v>20243259</v>
       </c>
       <c r="B92" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C92" t="s">
         <v>32</v>
       </c>
       <c r="D92" t="s">
+        <v>586</v>
+      </c>
+      <c r="E92" t="s">
+        <v>580</v>
+      </c>
+      <c r="F92" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" t="s">
         <v>587</v>
       </c>
-      <c r="E92" t="s">
-        <v>581</v>
-      </c>
-      <c r="F92" t="s">
-        <v>16</v>
-      </c>
-      <c r="G92" t="s">
+      <c r="H92" t="s">
         <v>588</v>
-      </c>
-      <c r="H92" t="s">
-        <v>589</v>
       </c>
       <c r="I92" t="s">
         <v>44</v>
       </c>
       <c r="J92" t="s">
+        <v>589</v>
+      </c>
+      <c r="K92" t="s">
         <v>590</v>
       </c>
-      <c r="K92" t="s">
-        <v>591</v>
-      </c>
       <c r="L92" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="93">
@@ -5805,37 +5802,37 @@
         <v>20243169</v>
       </c>
       <c r="B93" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C93" t="s">
         <v>13</v>
       </c>
       <c r="D93" t="s">
+        <v>592</v>
+      </c>
+      <c r="E93" t="s">
         <v>593</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F93" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" t="s">
         <v>594</v>
       </c>
-      <c r="F93" t="s">
-        <v>16</v>
-      </c>
-      <c r="G93" t="s">
+      <c r="H93" t="s">
         <v>595</v>
-      </c>
-      <c r="H93" t="s">
-        <v>596</v>
       </c>
       <c r="I93" t="s">
         <v>44</v>
       </c>
       <c r="J93" t="s">
+        <v>596</v>
+      </c>
+      <c r="K93" t="s">
         <v>597</v>
       </c>
-      <c r="K93" t="s">
-        <v>598</v>
-      </c>
       <c r="L93" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="94">
@@ -5843,7 +5840,7 @@
         <v>20243077</v>
       </c>
       <c r="B94" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C94" t="s">
         <v>13</v>
@@ -5852,28 +5849,28 @@
         <v>14</v>
       </c>
       <c r="E94" t="s">
+        <v>599</v>
+      </c>
+      <c r="F94" t="s">
+        <v>16</v>
+      </c>
+      <c r="G94" t="s">
         <v>600</v>
       </c>
-      <c r="F94" t="s">
-        <v>16</v>
-      </c>
-      <c r="G94" t="s">
+      <c r="H94" t="s">
         <v>601</v>
-      </c>
-      <c r="H94" t="s">
-        <v>602</v>
       </c>
       <c r="I94" t="s">
         <v>68</v>
       </c>
       <c r="J94" t="s">
+        <v>602</v>
+      </c>
+      <c r="K94" t="s">
         <v>603</v>
       </c>
-      <c r="K94" t="s">
-        <v>604</v>
-      </c>
       <c r="L94" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="95">
@@ -5881,37 +5878,37 @@
         <v>20247112</v>
       </c>
       <c r="B95" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C95" t="s">
         <v>39</v>
       </c>
       <c r="D95" t="s">
+        <v>605</v>
+      </c>
+      <c r="E95" t="s">
         <v>606</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F95" t="s">
+        <v>16</v>
+      </c>
+      <c r="G95" t="s">
         <v>607</v>
       </c>
-      <c r="F95" t="s">
-        <v>16</v>
-      </c>
-      <c r="G95" t="s">
+      <c r="H95" t="s">
         <v>608</v>
-      </c>
-      <c r="H95" t="s">
-        <v>609</v>
       </c>
       <c r="I95" t="s">
         <v>44</v>
       </c>
       <c r="J95" t="s">
+        <v>609</v>
+      </c>
+      <c r="K95" t="s">
         <v>610</v>
       </c>
-      <c r="K95" t="s">
-        <v>611</v>
-      </c>
       <c r="L95" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="96">
@@ -5919,37 +5916,37 @@
         <v>20247015</v>
       </c>
       <c r="B96" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C96" t="s">
         <v>39</v>
       </c>
       <c r="D96" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E96" t="s">
+        <v>612</v>
+      </c>
+      <c r="F96" t="s">
+        <v>16</v>
+      </c>
+      <c r="G96" t="s">
         <v>613</v>
       </c>
-      <c r="F96" t="s">
-        <v>16</v>
-      </c>
-      <c r="G96" t="s">
+      <c r="H96" t="s">
         <v>614</v>
-      </c>
-      <c r="H96" t="s">
-        <v>615</v>
       </c>
       <c r="I96" t="s">
         <v>44</v>
       </c>
       <c r="J96" t="s">
+        <v>615</v>
+      </c>
+      <c r="K96" t="s">
         <v>616</v>
       </c>
-      <c r="K96" t="s">
-        <v>617</v>
-      </c>
       <c r="L96" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97">
@@ -5957,7 +5954,7 @@
         <v>20234494</v>
       </c>
       <c r="B97" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C97" t="s">
         <v>32</v>
@@ -5966,28 +5963,28 @@
         <v>130</v>
       </c>
       <c r="E97" t="s">
+        <v>618</v>
+      </c>
+      <c r="F97" t="s">
+        <v>16</v>
+      </c>
+      <c r="G97" t="s">
         <v>619</v>
       </c>
-      <c r="F97" t="s">
-        <v>16</v>
-      </c>
-      <c r="G97" t="s">
+      <c r="H97" t="s">
         <v>620</v>
-      </c>
-      <c r="H97" t="s">
-        <v>621</v>
       </c>
       <c r="I97" t="s">
         <v>44</v>
       </c>
       <c r="J97" t="s">
+        <v>621</v>
+      </c>
+      <c r="K97" t="s">
         <v>622</v>
       </c>
-      <c r="K97" t="s">
-        <v>623</v>
-      </c>
       <c r="L97" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98">
@@ -5995,7 +5992,7 @@
         <v>20234461</v>
       </c>
       <c r="B98" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C98" t="s">
         <v>32</v>
@@ -6004,28 +6001,28 @@
         <v>92</v>
       </c>
       <c r="E98" t="s">
+        <v>624</v>
+      </c>
+      <c r="F98" t="s">
+        <v>16</v>
+      </c>
+      <c r="G98" t="s">
         <v>625</v>
       </c>
-      <c r="F98" t="s">
-        <v>16</v>
-      </c>
-      <c r="G98" t="s">
+      <c r="H98" t="s">
         <v>626</v>
-      </c>
-      <c r="H98" t="s">
-        <v>627</v>
       </c>
       <c r="I98" t="s">
         <v>44</v>
       </c>
       <c r="J98" t="s">
+        <v>627</v>
+      </c>
+      <c r="K98" t="s">
         <v>628</v>
       </c>
-      <c r="K98" t="s">
-        <v>629</v>
-      </c>
       <c r="L98" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="99">
@@ -6033,37 +6030,37 @@
         <v>20234375</v>
       </c>
       <c r="B99" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C99" t="s">
         <v>32</v>
       </c>
       <c r="D99" t="s">
+        <v>630</v>
+      </c>
+      <c r="E99" t="s">
         <v>631</v>
       </c>
-      <c r="E99" t="s">
+      <c r="F99" t="s">
+        <v>16</v>
+      </c>
+      <c r="G99" t="s">
         <v>632</v>
       </c>
-      <c r="F99" t="s">
-        <v>16</v>
-      </c>
-      <c r="G99" t="s">
+      <c r="H99" t="s">
         <v>633</v>
-      </c>
-      <c r="H99" t="s">
-        <v>634</v>
       </c>
       <c r="I99" t="s">
         <v>44</v>
       </c>
       <c r="J99" t="s">
+        <v>634</v>
+      </c>
+      <c r="K99" t="s">
         <v>635</v>
       </c>
-      <c r="K99" t="s">
-        <v>636</v>
-      </c>
       <c r="L99" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100">
@@ -6071,37 +6068,37 @@
         <v>20234353</v>
       </c>
       <c r="B100" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C100" t="s">
         <v>32</v>
       </c>
       <c r="D100" t="s">
+        <v>637</v>
+      </c>
+      <c r="E100" t="s">
         <v>638</v>
       </c>
-      <c r="E100" t="s">
+      <c r="F100" t="s">
+        <v>16</v>
+      </c>
+      <c r="G100" t="s">
         <v>639</v>
       </c>
-      <c r="F100" t="s">
-        <v>16</v>
-      </c>
-      <c r="G100" t="s">
+      <c r="H100" t="s">
         <v>640</v>
-      </c>
-      <c r="H100" t="s">
-        <v>641</v>
       </c>
       <c r="I100" t="s">
         <v>44</v>
       </c>
       <c r="J100" t="s">
+        <v>641</v>
+      </c>
+      <c r="K100" t="s">
         <v>642</v>
       </c>
-      <c r="K100" t="s">
-        <v>643</v>
-      </c>
       <c r="L100" t="s">
-        <v>187</v>
+        <v>47</v>
       </c>
     </row>
     <row r="101">
@@ -6109,35 +6106,35 @@
         <v>20234346</v>
       </c>
       <c r="B101" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C101" t="s">
         <v>13</v>
       </c>
       <c r="D101"/>
       <c r="E101" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F101" t="s">
         <v>26</v>
       </c>
       <c r="G101" t="s">
+        <v>645</v>
+      </c>
+      <c r="H101" t="s">
         <v>646</v>
-      </c>
-      <c r="H101" t="s">
-        <v>647</v>
       </c>
       <c r="I101" t="s">
         <v>44</v>
       </c>
       <c r="J101" t="s">
+        <v>647</v>
+      </c>
+      <c r="K101" t="s">
         <v>648</v>
       </c>
-      <c r="K101" t="s">
-        <v>649</v>
-      </c>
       <c r="L101" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout des noms de commissions pour les objets parlementaires déposés par une commission
- Récupération automatique du nom de la commission via BusinessRole et Committee
- Les objets sans auteur (SubmittedBy = NA) sont maintenant complétés avec le nom de la commission
- Recalcul automatique des objets existants sans auteur
</commit_message>
<xml_diff>
--- a/Objets_parlementaires_CDF_EFK.xlsx
+++ b/Objets_parlementaires_CDF_EFK.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="655">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -803,6 +803,9 @@
     <t xml:space="preserve">25.3425</t>
   </si>
   <si>
+    <t xml:space="preserve">Commission des finances Conseil national</t>
+  </si>
+  <si>
     <t xml:space="preserve">2025-04-04</t>
   </si>
   <si>
@@ -1151,6 +1154,9 @@
     <t xml:space="preserve">25.3008</t>
   </si>
   <si>
+    <t xml:space="preserve">Commission de l'économie et des redevances Conseil national</t>
+  </si>
+  <si>
     <t xml:space="preserve">2025-01-21</t>
   </si>
   <si>
@@ -1679,6 +1685,9 @@
     <t xml:space="preserve">24.3471</t>
   </si>
   <si>
+    <t xml:space="preserve">Commission de la sécurité sociale et de la santé publique Conseil national</t>
+  </si>
+  <si>
     <t xml:space="preserve">2024-05-02</t>
   </si>
   <si>
@@ -1697,6 +1706,9 @@
     <t xml:space="preserve">24.3468</t>
   </si>
   <si>
+    <t xml:space="preserve">Commission des transports et des télécommunications Conseil national</t>
+  </si>
+  <si>
     <t xml:space="preserve">2024-04-30</t>
   </si>
   <si>
@@ -1715,6 +1727,9 @@
     <t xml:space="preserve">24.3467</t>
   </si>
   <si>
+    <t xml:space="preserve">Commission de la politique de sécurité Conseil des États</t>
+  </si>
+  <si>
     <t xml:space="preserve">2024-04-25</t>
   </si>
   <si>
@@ -1944,6 +1959,9 @@
   </si>
   <si>
     <t xml:space="preserve">23.4346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commission des institutions politiques Conseil des États</t>
   </si>
   <si>
     <t xml:space="preserve">2023-11-20</t>
@@ -3765,27 +3783,29 @@
       <c r="C39" t="s">
         <v>13</v>
       </c>
-      <c r="D39"/>
+      <c r="D39" t="s">
+        <v>263</v>
+      </c>
       <c r="E39" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F39" t="s">
         <v>16</v>
       </c>
       <c r="G39" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H39" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I39" t="s">
         <v>68</v>
       </c>
       <c r="J39" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K39" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L39" t="s">
         <v>22</v>
@@ -3796,7 +3816,7 @@
         <v>20253309</v>
       </c>
       <c r="B40" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C40" t="s">
         <v>13</v>
@@ -3805,25 +3825,25 @@
         <v>124</v>
       </c>
       <c r="E40" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F40" t="s">
         <v>16</v>
       </c>
       <c r="G40" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H40" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I40" t="s">
         <v>68</v>
       </c>
       <c r="J40" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="K40" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L40" t="s">
         <v>22</v>
@@ -3834,34 +3854,34 @@
         <v>20253399</v>
       </c>
       <c r="B41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C41" t="s">
         <v>32</v>
       </c>
       <c r="D41" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E41" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F41" t="s">
         <v>16</v>
       </c>
       <c r="G41" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H41" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I41" t="s">
         <v>68</v>
       </c>
       <c r="J41" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="K41" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="L41" t="s">
         <v>54</v>
@@ -3872,34 +3892,34 @@
         <v>20253404</v>
       </c>
       <c r="B42" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C42" t="s">
         <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E42" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F42" t="s">
         <v>16</v>
       </c>
       <c r="G42" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H42" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I42" t="s">
         <v>68</v>
       </c>
       <c r="J42" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="K42" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L42" t="s">
         <v>47</v>
@@ -3910,34 +3930,34 @@
         <v>20253417</v>
       </c>
       <c r="B43" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C43" t="s">
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E43" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F43" t="s">
         <v>16</v>
       </c>
       <c r="G43" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H43" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I43" t="s">
         <v>68</v>
       </c>
       <c r="J43" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="K43" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="L43" t="s">
         <v>47</v>
@@ -3948,34 +3968,34 @@
         <v>20251011</v>
       </c>
       <c r="B44" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C44" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D44" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E44" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F44" t="s">
         <v>26</v>
       </c>
       <c r="G44" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H44" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I44" t="s">
         <v>44</v>
       </c>
       <c r="J44" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K44" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L44" t="s">
         <v>47</v>
@@ -3986,34 +4006,34 @@
         <v>20253194</v>
       </c>
       <c r="B45" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C45" t="s">
         <v>32</v>
       </c>
       <c r="D45" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E45" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F45" t="s">
         <v>26</v>
       </c>
       <c r="G45" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H45" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I45" t="s">
         <v>44</v>
       </c>
       <c r="J45" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="K45" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="L45" t="s">
         <v>47</v>
@@ -4024,34 +4044,34 @@
         <v>20253203</v>
       </c>
       <c r="B46" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C46" t="s">
         <v>32</v>
       </c>
       <c r="D46" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E46" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F46" t="s">
         <v>16</v>
       </c>
       <c r="G46" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H46" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="I46" t="s">
         <v>44</v>
       </c>
       <c r="J46" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="K46" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L46" t="s">
         <v>54</v>
@@ -4062,34 +4082,34 @@
         <v>20253213</v>
       </c>
       <c r="B47" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C47" t="s">
         <v>32</v>
       </c>
       <c r="D47" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E47" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F47" t="s">
         <v>26</v>
       </c>
       <c r="G47" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H47" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="I47" t="s">
         <v>44</v>
       </c>
       <c r="J47" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="K47" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="L47" t="s">
         <v>47</v>
@@ -4100,34 +4120,34 @@
         <v>20253214</v>
       </c>
       <c r="B48" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C48" t="s">
         <v>32</v>
       </c>
       <c r="D48" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E48" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F48" t="s">
         <v>16</v>
       </c>
       <c r="G48" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H48" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="I48" t="s">
         <v>44</v>
       </c>
       <c r="J48" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="K48" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="L48" t="s">
         <v>47</v>
@@ -4138,34 +4158,34 @@
         <v>20253246</v>
       </c>
       <c r="B49" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C49" t="s">
         <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E49" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F49" t="s">
         <v>16</v>
       </c>
       <c r="G49" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="H49" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="I49" t="s">
         <v>145</v>
       </c>
       <c r="J49" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="K49" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="L49" t="s">
         <v>22</v>
@@ -4176,34 +4196,34 @@
         <v>20253093</v>
       </c>
       <c r="B50" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C50" t="s">
         <v>32</v>
       </c>
       <c r="D50" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E50" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F50" t="s">
         <v>16</v>
       </c>
       <c r="G50" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="H50" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="I50" t="s">
         <v>68</v>
       </c>
       <c r="J50" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K50" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="L50" t="s">
         <v>22</v>
@@ -4214,34 +4234,34 @@
         <v>20257213</v>
       </c>
       <c r="B51" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C51" t="s">
         <v>39</v>
       </c>
       <c r="D51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E51" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F51" t="s">
         <v>16</v>
       </c>
       <c r="G51" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="H51" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="I51" t="s">
         <v>44</v>
       </c>
       <c r="J51" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K51" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="L51" t="s">
         <v>22</v>
@@ -4252,34 +4272,34 @@
         <v>20253054</v>
       </c>
       <c r="B52" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C52" t="s">
         <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E52" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F52" t="s">
         <v>16</v>
       </c>
       <c r="G52" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H52" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="I52" t="s">
         <v>68</v>
       </c>
       <c r="J52" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="K52" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="L52" t="s">
         <v>47</v>
@@ -4290,7 +4310,7 @@
         <v>20257102</v>
       </c>
       <c r="B53" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C53" t="s">
         <v>39</v>
@@ -4299,25 +4319,25 @@
         <v>111</v>
       </c>
       <c r="E53" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F53" t="s">
         <v>16</v>
       </c>
       <c r="G53" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="H53" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="I53" t="s">
         <v>44</v>
       </c>
       <c r="J53" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="K53" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="L53" t="s">
         <v>47</v>
@@ -4328,7 +4348,7 @@
         <v>20257129</v>
       </c>
       <c r="B54" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C54" t="s">
         <v>39</v>
@@ -4337,25 +4357,25 @@
         <v>256</v>
       </c>
       <c r="E54" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F54" t="s">
         <v>16</v>
       </c>
       <c r="G54" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="H54" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="I54" t="s">
         <v>44</v>
       </c>
       <c r="J54" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="K54" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="L54" t="s">
         <v>22</v>
@@ -4366,34 +4386,34 @@
         <v>20257138</v>
       </c>
       <c r="B55" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C55" t="s">
         <v>39</v>
       </c>
       <c r="D55" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E55" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F55" t="s">
         <v>16</v>
       </c>
       <c r="G55" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H55" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="I55" t="s">
         <v>44</v>
       </c>
       <c r="J55" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="K55" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L55" t="s">
         <v>47</v>
@@ -4404,34 +4424,34 @@
         <v>20253031</v>
       </c>
       <c r="B56" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C56" t="s">
         <v>32</v>
       </c>
       <c r="D56" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E56" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F56" t="s">
         <v>16</v>
       </c>
       <c r="G56" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="H56" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="I56" t="s">
         <v>68</v>
       </c>
       <c r="J56" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="K56" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="L56" t="s">
         <v>47</v>
@@ -4442,34 +4462,34 @@
         <v>20257012</v>
       </c>
       <c r="B57" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C57" t="s">
         <v>39</v>
       </c>
       <c r="D57" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E57" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F57" t="s">
         <v>16</v>
       </c>
       <c r="G57" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H57" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="I57" t="s">
         <v>44</v>
       </c>
       <c r="J57" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="K57" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="L57" t="s">
         <v>54</v>
@@ -4480,32 +4500,34 @@
         <v>20253008</v>
       </c>
       <c r="B58" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C58" t="s">
         <v>13</v>
       </c>
-      <c r="D58"/>
+      <c r="D58" t="s">
+        <v>380</v>
+      </c>
       <c r="E58" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="F58" t="s">
         <v>16</v>
       </c>
       <c r="G58" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="H58" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I58" t="s">
         <v>44</v>
       </c>
       <c r="J58" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="K58" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="L58" t="s">
         <v>47</v>
@@ -4516,34 +4538,34 @@
         <v>20244404</v>
       </c>
       <c r="B59" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C59" t="s">
         <v>32</v>
       </c>
       <c r="D59" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E59" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="F59" t="s">
         <v>16</v>
       </c>
       <c r="G59" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="H59" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="I59" t="s">
         <v>44</v>
       </c>
       <c r="J59" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="K59" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="L59" t="s">
         <v>47</v>
@@ -4554,7 +4576,7 @@
         <v>20244419</v>
       </c>
       <c r="B60" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C60" t="s">
         <v>32</v>
@@ -4563,25 +4585,25 @@
         <v>222</v>
       </c>
       <c r="E60" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="F60" t="s">
         <v>26</v>
       </c>
       <c r="G60" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="H60" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="I60" t="s">
         <v>44</v>
       </c>
       <c r="J60" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="K60" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="L60" t="s">
         <v>47</v>
@@ -4592,34 +4614,34 @@
         <v>20247975</v>
       </c>
       <c r="B61" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C61" t="s">
         <v>39</v>
       </c>
       <c r="D61" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="E61" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="F61" t="s">
         <v>16</v>
       </c>
       <c r="G61" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="H61" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="I61" t="s">
         <v>44</v>
       </c>
       <c r="J61" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="K61" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="L61" t="s">
         <v>22</v>
@@ -4630,34 +4652,34 @@
         <v>20248043</v>
       </c>
       <c r="B62" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C62" t="s">
         <v>39</v>
       </c>
       <c r="D62" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="E62" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="F62" t="s">
         <v>16</v>
       </c>
       <c r="G62" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="H62" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="I62" t="s">
         <v>44</v>
       </c>
       <c r="J62" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="K62" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="L62" t="s">
         <v>22</v>
@@ -4668,34 +4690,34 @@
         <v>20244290</v>
       </c>
       <c r="B63" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C63" t="s">
         <v>32</v>
       </c>
       <c r="D63" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="E63" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="F63" t="s">
         <v>16</v>
       </c>
       <c r="G63" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="H63" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="I63" t="s">
         <v>68</v>
       </c>
       <c r="J63" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="K63" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="L63" t="s">
         <v>47</v>
@@ -4706,34 +4728,34 @@
         <v>20244278</v>
       </c>
       <c r="B64" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C64" t="s">
         <v>32</v>
       </c>
       <c r="D64" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="E64" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="F64" t="s">
         <v>16</v>
       </c>
       <c r="G64" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="H64" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I64" t="s">
         <v>68</v>
       </c>
       <c r="J64" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="K64" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="L64" t="s">
         <v>22</v>
@@ -4744,34 +4766,34 @@
         <v>20244082</v>
       </c>
       <c r="B65" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C65" t="s">
         <v>32</v>
       </c>
       <c r="D65" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E65" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="F65" t="s">
         <v>16</v>
       </c>
       <c r="G65" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="H65" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="I65" t="s">
         <v>68</v>
       </c>
       <c r="J65" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="K65" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="L65" t="s">
         <v>47</v>
@@ -4782,34 +4804,34 @@
         <v>20244112</v>
       </c>
       <c r="B66" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C66" t="s">
         <v>32</v>
       </c>
       <c r="D66" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="E66" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="F66" t="s">
         <v>16</v>
       </c>
       <c r="G66" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="H66" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="I66" t="s">
         <v>68</v>
       </c>
       <c r="J66" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="K66" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="L66" t="s">
         <v>54</v>
@@ -4820,7 +4842,7 @@
         <v>20244131</v>
       </c>
       <c r="B67" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C67" t="s">
         <v>32</v>
@@ -4829,25 +4851,25 @@
         <v>49</v>
       </c>
       <c r="E67" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="F67" t="s">
         <v>16</v>
       </c>
       <c r="G67" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="H67" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="I67" t="s">
         <v>68</v>
       </c>
       <c r="J67" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="K67" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="L67" t="s">
         <v>47</v>
@@ -4858,7 +4880,7 @@
         <v>20244132</v>
       </c>
       <c r="B68" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C68" t="s">
         <v>63</v>
@@ -4867,25 +4889,25 @@
         <v>124</v>
       </c>
       <c r="E68" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="F68" t="s">
         <v>16</v>
       </c>
       <c r="G68" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="H68" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="I68" t="s">
         <v>68</v>
       </c>
       <c r="J68" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="K68" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="L68" t="s">
         <v>54</v>
@@ -4896,7 +4918,7 @@
         <v>20244133</v>
       </c>
       <c r="B69" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C69" t="s">
         <v>13</v>
@@ -4905,25 +4927,25 @@
         <v>124</v>
       </c>
       <c r="E69" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="F69" t="s">
         <v>16</v>
       </c>
       <c r="G69" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="H69" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="I69" t="s">
         <v>68</v>
       </c>
       <c r="J69" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="K69" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="L69" t="s">
         <v>54</v>
@@ -4934,34 +4956,34 @@
         <v>20244137</v>
       </c>
       <c r="B70" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C70" t="s">
         <v>32</v>
       </c>
       <c r="D70" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="E70" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="F70" t="s">
         <v>16</v>
       </c>
       <c r="G70" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="H70" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="I70" t="s">
         <v>68</v>
       </c>
       <c r="J70" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="K70" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="L70" t="s">
         <v>54</v>
@@ -4972,34 +4994,34 @@
         <v>20243937</v>
       </c>
       <c r="B71" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C71" t="s">
         <v>13</v>
       </c>
       <c r="D71" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="E71" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="F71" t="s">
         <v>26</v>
       </c>
       <c r="G71" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="H71" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="I71" t="s">
         <v>177</v>
       </c>
       <c r="J71" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="K71" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="L71" t="s">
         <v>22</v>
@@ -5010,34 +5032,34 @@
         <v>20243948</v>
       </c>
       <c r="B72" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C72" t="s">
         <v>32</v>
       </c>
       <c r="D72" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="E72" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="F72" t="s">
         <v>26</v>
       </c>
       <c r="G72" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="H72" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I72" t="s">
         <v>44</v>
       </c>
       <c r="J72" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="K72" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="L72" t="s">
         <v>47</v>
@@ -5048,7 +5070,7 @@
         <v>20247720</v>
       </c>
       <c r="B73" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C73" t="s">
         <v>39</v>
@@ -5057,25 +5079,25 @@
         <v>256</v>
       </c>
       <c r="E73" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="F73" t="s">
         <v>16</v>
       </c>
       <c r="G73" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="H73" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="I73" t="s">
         <v>44</v>
       </c>
       <c r="J73" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="K73" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="L73" t="s">
         <v>22</v>
@@ -5086,34 +5108,34 @@
         <v>20247726</v>
       </c>
       <c r="B74" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C74" t="s">
         <v>39</v>
       </c>
       <c r="D74" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E74" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="F74" t="s">
         <v>16</v>
       </c>
       <c r="G74" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="H74" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="I74" t="s">
         <v>44</v>
       </c>
       <c r="J74" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="K74" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="L74" t="s">
         <v>47</v>
@@ -5124,7 +5146,7 @@
         <v>20247773</v>
       </c>
       <c r="B75" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C75" t="s">
         <v>39</v>
@@ -5133,25 +5155,25 @@
         <v>118</v>
       </c>
       <c r="E75" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="F75" t="s">
         <v>16</v>
       </c>
       <c r="G75" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="H75" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="I75" t="s">
         <v>44</v>
       </c>
       <c r="J75" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="K75" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="L75" t="s">
         <v>54</v>
@@ -5162,7 +5184,7 @@
         <v>20247774</v>
       </c>
       <c r="B76" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C76" t="s">
         <v>39</v>
@@ -5171,25 +5193,25 @@
         <v>118</v>
       </c>
       <c r="E76" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="F76" t="s">
         <v>16</v>
       </c>
       <c r="G76" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="H76" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="I76" t="s">
         <v>44</v>
       </c>
       <c r="J76" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="K76" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="L76" t="s">
         <v>54</v>
@@ -5200,34 +5222,34 @@
         <v>20243858</v>
       </c>
       <c r="B77" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="C77" t="s">
         <v>32</v>
       </c>
       <c r="D77" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="E77" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="F77" t="s">
         <v>16</v>
       </c>
       <c r="G77" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="H77" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="I77" t="s">
         <v>68</v>
       </c>
       <c r="J77" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="K77" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="L77" t="s">
         <v>22</v>
@@ -5238,34 +5260,34 @@
         <v>20243877</v>
       </c>
       <c r="B78" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C78" t="s">
         <v>32</v>
       </c>
       <c r="D78" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="E78" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="F78" t="s">
         <v>16</v>
       </c>
       <c r="G78" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="H78" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="I78" t="s">
         <v>68</v>
       </c>
       <c r="J78" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="K78" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="L78" t="s">
         <v>47</v>
@@ -5276,7 +5298,7 @@
         <v>20247622</v>
       </c>
       <c r="B79" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C79" t="s">
         <v>39</v>
@@ -5285,25 +5307,25 @@
         <v>49</v>
       </c>
       <c r="E79" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="F79" t="s">
         <v>16</v>
       </c>
       <c r="G79" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="H79" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="I79" t="s">
         <v>44</v>
       </c>
       <c r="J79" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="K79" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="L79" t="s">
         <v>47</v>
@@ -5314,34 +5336,34 @@
         <v>20247649</v>
       </c>
       <c r="B80" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C80" t="s">
         <v>39</v>
       </c>
       <c r="D80" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="E80" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="F80" t="s">
         <v>16</v>
       </c>
       <c r="G80" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="H80" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="I80" t="s">
         <v>44</v>
       </c>
       <c r="J80" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="K80" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="L80" t="s">
         <v>47</v>
@@ -5352,34 +5374,34 @@
         <v>20243709</v>
       </c>
       <c r="B81" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C81" t="s">
         <v>32</v>
       </c>
       <c r="D81" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E81" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="F81" t="s">
         <v>16</v>
       </c>
       <c r="G81" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="H81" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="I81" t="s">
         <v>68</v>
       </c>
       <c r="J81" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="K81" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="L81" t="s">
         <v>54</v>
@@ -5390,34 +5412,34 @@
         <v>20243773</v>
       </c>
       <c r="B82" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="C82" t="s">
         <v>32</v>
       </c>
       <c r="D82" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="E82" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="F82" t="s">
         <v>16</v>
       </c>
       <c r="G82" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="H82" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="I82" t="s">
         <v>68</v>
       </c>
       <c r="J82" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="K82" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="L82" t="s">
         <v>47</v>
@@ -5428,34 +5450,34 @@
         <v>20243776</v>
       </c>
       <c r="B83" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="C83" t="s">
         <v>13</v>
       </c>
       <c r="D83" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="E83" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="F83" t="s">
         <v>16</v>
       </c>
       <c r="G83" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="H83" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="I83" t="s">
         <v>44</v>
       </c>
       <c r="J83" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="K83" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="L83" t="s">
         <v>22</v>
@@ -5466,34 +5488,34 @@
         <v>20243609</v>
       </c>
       <c r="B84" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="C84" t="s">
         <v>13</v>
       </c>
       <c r="D84" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="E84" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="F84" t="s">
         <v>16</v>
       </c>
       <c r="G84" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="H84" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="I84" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="J84" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="K84" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="L84" t="s">
         <v>47</v>
@@ -5504,7 +5526,7 @@
         <v>20243574</v>
       </c>
       <c r="B85" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C85" t="s">
         <v>32</v>
@@ -5513,25 +5535,25 @@
         <v>229</v>
       </c>
       <c r="E85" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="F85" t="s">
         <v>26</v>
       </c>
       <c r="G85" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="H85" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="I85" t="s">
         <v>44</v>
       </c>
       <c r="J85" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="K85" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="L85" t="s">
         <v>22</v>
@@ -5542,34 +5564,34 @@
         <v>20243557</v>
       </c>
       <c r="B86" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C86" t="s">
         <v>32</v>
       </c>
       <c r="D86" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="E86" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="F86" t="s">
         <v>16</v>
       </c>
       <c r="G86" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="H86" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="I86" t="s">
         <v>44</v>
       </c>
       <c r="J86" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="K86" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="L86" t="s">
         <v>47</v>
@@ -5580,32 +5602,34 @@
         <v>20243471</v>
       </c>
       <c r="B87" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="C87" t="s">
         <v>13</v>
       </c>
-      <c r="D87"/>
+      <c r="D87" t="s">
+        <v>557</v>
+      </c>
       <c r="E87" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="F87" t="s">
         <v>16</v>
       </c>
       <c r="G87" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="H87" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="I87" t="s">
         <v>44</v>
       </c>
       <c r="J87" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="K87" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="L87" t="s">
         <v>22</v>
@@ -5616,32 +5640,34 @@
         <v>20243468</v>
       </c>
       <c r="B88" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="C88" t="s">
         <v>63</v>
       </c>
-      <c r="D88"/>
+      <c r="D88" t="s">
+        <v>564</v>
+      </c>
       <c r="E88" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="F88" t="s">
         <v>16</v>
       </c>
       <c r="G88" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="H88" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="I88" t="s">
         <v>177</v>
       </c>
       <c r="J88" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="K88" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="L88" t="s">
         <v>47</v>
@@ -5652,32 +5678,34 @@
         <v>20243467</v>
       </c>
       <c r="B89" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="C89" t="s">
         <v>13</v>
       </c>
-      <c r="D89"/>
+      <c r="D89" t="s">
+        <v>571</v>
+      </c>
       <c r="E89" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
       <c r="F89" t="s">
         <v>26</v>
       </c>
       <c r="G89" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
       <c r="H89" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
       <c r="I89" t="s">
         <v>44</v>
       </c>
       <c r="J89" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
       <c r="K89" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="L89" t="s">
         <v>47</v>
@@ -5688,34 +5716,34 @@
         <v>20243318</v>
       </c>
       <c r="B90" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
       <c r="C90" t="s">
         <v>32</v>
       </c>
       <c r="D90" t="s">
-        <v>573</v>
+        <v>578</v>
       </c>
       <c r="E90" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="F90" t="s">
         <v>16</v>
       </c>
       <c r="G90" t="s">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="H90" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="I90" t="s">
         <v>68</v>
       </c>
       <c r="J90" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
       <c r="K90" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="L90" t="s">
         <v>54</v>
@@ -5726,34 +5754,34 @@
         <v>20243234</v>
       </c>
       <c r="B91" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
       <c r="C91" t="s">
         <v>13</v>
       </c>
       <c r="D91" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E91" t="s">
-        <v>580</v>
+        <v>585</v>
       </c>
       <c r="F91" t="s">
         <v>16</v>
       </c>
       <c r="G91" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
       <c r="H91" t="s">
-        <v>582</v>
+        <v>587</v>
       </c>
       <c r="I91" t="s">
         <v>44</v>
       </c>
       <c r="J91" t="s">
-        <v>583</v>
+        <v>588</v>
       </c>
       <c r="K91" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="L91" t="s">
         <v>47</v>
@@ -5764,34 +5792,34 @@
         <v>20243259</v>
       </c>
       <c r="B92" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="C92" t="s">
         <v>32</v>
       </c>
       <c r="D92" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="E92" t="s">
-        <v>580</v>
+        <v>585</v>
       </c>
       <c r="F92" t="s">
         <v>16</v>
       </c>
       <c r="G92" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
       <c r="H92" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="I92" t="s">
         <v>44</v>
       </c>
       <c r="J92" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
       <c r="K92" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="L92" t="s">
         <v>47</v>
@@ -5802,34 +5830,34 @@
         <v>20243169</v>
       </c>
       <c r="B93" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="C93" t="s">
         <v>13</v>
       </c>
       <c r="D93" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="E93" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="F93" t="s">
         <v>16</v>
       </c>
       <c r="G93" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="H93" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="I93" t="s">
         <v>44</v>
       </c>
       <c r="J93" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="K93" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="L93" t="s">
         <v>47</v>
@@ -5840,7 +5868,7 @@
         <v>20243077</v>
       </c>
       <c r="B94" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
       <c r="C94" t="s">
         <v>13</v>
@@ -5849,25 +5877,25 @@
         <v>14</v>
       </c>
       <c r="E94" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="F94" t="s">
         <v>16</v>
       </c>
       <c r="G94" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="H94" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="I94" t="s">
         <v>68</v>
       </c>
       <c r="J94" t="s">
-        <v>602</v>
+        <v>607</v>
       </c>
       <c r="K94" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
       <c r="L94" t="s">
         <v>47</v>
@@ -5878,34 +5906,34 @@
         <v>20247112</v>
       </c>
       <c r="B95" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="C95" t="s">
         <v>39</v>
       </c>
       <c r="D95" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="E95" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="F95" t="s">
         <v>16</v>
       </c>
       <c r="G95" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="H95" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="I95" t="s">
         <v>44</v>
       </c>
       <c r="J95" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
       <c r="K95" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
       <c r="L95" t="s">
         <v>54</v>
@@ -5916,7 +5944,7 @@
         <v>20247015</v>
       </c>
       <c r="B96" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="C96" t="s">
         <v>39</v>
@@ -5925,25 +5953,25 @@
         <v>256</v>
       </c>
       <c r="E96" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
       <c r="F96" t="s">
         <v>16</v>
       </c>
       <c r="G96" t="s">
-        <v>613</v>
+        <v>618</v>
       </c>
       <c r="H96" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="I96" t="s">
         <v>44</v>
       </c>
       <c r="J96" t="s">
-        <v>615</v>
+        <v>620</v>
       </c>
       <c r="K96" t="s">
-        <v>616</v>
+        <v>621</v>
       </c>
       <c r="L96" t="s">
         <v>22</v>
@@ -5954,7 +5982,7 @@
         <v>20234494</v>
       </c>
       <c r="B97" t="s">
-        <v>617</v>
+        <v>622</v>
       </c>
       <c r="C97" t="s">
         <v>32</v>
@@ -5963,25 +5991,25 @@
         <v>130</v>
       </c>
       <c r="E97" t="s">
-        <v>618</v>
+        <v>623</v>
       </c>
       <c r="F97" t="s">
         <v>16</v>
       </c>
       <c r="G97" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
       <c r="H97" t="s">
-        <v>620</v>
+        <v>625</v>
       </c>
       <c r="I97" t="s">
         <v>44</v>
       </c>
       <c r="J97" t="s">
-        <v>621</v>
+        <v>626</v>
       </c>
       <c r="K97" t="s">
-        <v>622</v>
+        <v>627</v>
       </c>
       <c r="L97" t="s">
         <v>22</v>
@@ -5992,7 +6020,7 @@
         <v>20234461</v>
       </c>
       <c r="B98" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
       <c r="C98" t="s">
         <v>32</v>
@@ -6001,25 +6029,25 @@
         <v>92</v>
       </c>
       <c r="E98" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="F98" t="s">
         <v>16</v>
       </c>
       <c r="G98" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
       <c r="H98" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="I98" t="s">
         <v>44</v>
       </c>
       <c r="J98" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
       <c r="K98" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
       <c r="L98" t="s">
         <v>47</v>
@@ -6030,34 +6058,34 @@
         <v>20234375</v>
       </c>
       <c r="B99" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
       <c r="C99" t="s">
         <v>32</v>
       </c>
       <c r="D99" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
       <c r="E99" t="s">
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="F99" t="s">
         <v>16</v>
       </c>
       <c r="G99" t="s">
-        <v>632</v>
+        <v>637</v>
       </c>
       <c r="H99" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
       <c r="I99" t="s">
         <v>44</v>
       </c>
       <c r="J99" t="s">
-        <v>634</v>
+        <v>639</v>
       </c>
       <c r="K99" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="L99" t="s">
         <v>22</v>
@@ -6068,34 +6096,34 @@
         <v>20234353</v>
       </c>
       <c r="B100" t="s">
-        <v>636</v>
+        <v>641</v>
       </c>
       <c r="C100" t="s">
         <v>32</v>
       </c>
       <c r="D100" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="E100" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
       <c r="F100" t="s">
         <v>16</v>
       </c>
       <c r="G100" t="s">
-        <v>639</v>
+        <v>644</v>
       </c>
       <c r="H100" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="I100" t="s">
         <v>44</v>
       </c>
       <c r="J100" t="s">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="K100" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
       <c r="L100" t="s">
         <v>47</v>
@@ -6106,32 +6134,34 @@
         <v>20234346</v>
       </c>
       <c r="B101" t="s">
-        <v>643</v>
+        <v>648</v>
       </c>
       <c r="C101" t="s">
         <v>13</v>
       </c>
-      <c r="D101"/>
+      <c r="D101" t="s">
+        <v>649</v>
+      </c>
       <c r="E101" t="s">
-        <v>644</v>
+        <v>650</v>
       </c>
       <c r="F101" t="s">
         <v>26</v>
       </c>
       <c r="G101" t="s">
-        <v>645</v>
+        <v>651</v>
       </c>
       <c r="H101" t="s">
-        <v>646</v>
+        <v>652</v>
       </c>
       <c r="I101" t="s">
         <v>44</v>
       </c>
       <c r="J101" t="s">
-        <v>647</v>
+        <v>653</v>
       </c>
       <c r="K101" t="s">
-        <v>648</v>
+        <v>654</v>
       </c>
       <c r="L101" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Mise à jour données parlement - 2026-02-13
- Nouveau fichier Nouveautés avec les vrais changements
</commit_message>
<xml_diff>
--- a/Objets_parlementaires_CDF_EFK.xlsx
+++ b/Objets_parlementaires_CDF_EFK.xlsx
@@ -77,45 +77,51 @@
     <t xml:space="preserve">La rémunération des tâches confiées à l'OFDF dans les aéroports de Genève et Bâle doit profiter à l'OFDF !</t>
   </si>
   <si>
+    <t xml:space="preserve">Stellungnahme zum Vorstoss liegt vor / L’avis relatif à l’intervention est disponible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.parlament.ch/de/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Élu &amp; Conseil fédéral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.4620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michel Matthias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-12-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daten der Bundesverwaltung mehrfach nutzbar machen – als Basis für vertrauenswürdige KI in der Schweiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Favoriser la fiabilité de l’IA en Suisse en rendant réutilisables les données de l’administration fédérale</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eingereicht / Déposé</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.parlament.ch/de/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254785</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254785</t>
+    <t xml:space="preserve">https://www.parlament.ch/de/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254620</t>
   </si>
   <si>
     <t xml:space="preserve">Élu</t>
   </si>
   <si>
-    <t xml:space="preserve">25.4620</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michel Matthias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-12-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daten der Bundesverwaltung mehrfach nutzbar machen – als Basis für vertrauenswürdige KI in der Schweiz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Favoriser la fiabilité de l’IA en Suisse en rendant réutilisables les données de l’administration fédérale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.parlament.ch/de/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254620</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254620</t>
-  </si>
-  <si>
     <t xml:space="preserve">25.4696</t>
   </si>
   <si>
@@ -191,9 +197,6 @@
     <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20258273</t>
   </si>
   <si>
-    <t xml:space="preserve">Élu &amp; Conseil fédéral</t>
-  </si>
-  <si>
     <t xml:space="preserve">25.4463</t>
   </si>
   <si>
@@ -234,9 +237,6 @@
   </si>
   <si>
     <t xml:space="preserve">Coordination plus efficace des moyens de transport dans le cadre des programmes d'agglomération</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stellungnahme zum Vorstoss liegt vor / L’avis relatif à l’intervention est disponible</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.parlament.ch/de/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254281</t>
@@ -2474,16 +2474,16 @@
         <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
@@ -2491,16 +2491,16 @@
         <v>20254696</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
         <v>28</v>
@@ -2509,19 +2509,19 @@
         <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s">
         <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M4" t="s">
         <v>24</v>
@@ -2532,40 +2532,40 @@
         <v>20258194</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
@@ -2573,40 +2573,40 @@
         <v>20258273</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
         <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M6" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -2614,40 +2614,40 @@
         <v>20254463</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G7" t="s">
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J7" t="s">
         <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M7" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
@@ -2655,31 +2655,31 @@
         <v>20254281</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J8" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K8" t="s">
         <v>75</v>
@@ -2688,7 +2688,7 @@
         <v>76</v>
       </c>
       <c r="M8" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
@@ -2708,7 +2708,7 @@
         <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
@@ -2720,7 +2720,7 @@
         <v>80</v>
       </c>
       <c r="J9" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K9" t="s">
         <v>81</v>
@@ -2729,7 +2729,7 @@
         <v>82</v>
       </c>
       <c r="M9" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10">
@@ -2761,7 +2761,7 @@
         <v>87</v>
       </c>
       <c r="J10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K10" t="s">
         <v>88</v>
@@ -2770,7 +2770,7 @@
         <v>89</v>
       </c>
       <c r="M10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11">
@@ -2811,7 +2811,7 @@
         <v>96</v>
       </c>
       <c r="M11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12">
@@ -2822,13 +2822,13 @@
         <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
         <v>98</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
@@ -2843,7 +2843,7 @@
         <v>100</v>
       </c>
       <c r="J12" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K12" t="s">
         <v>101</v>
@@ -2852,7 +2852,7 @@
         <v>102</v>
       </c>
       <c r="M12" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
@@ -2869,7 +2869,7 @@
         <v>104</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
         <v>85</v>
@@ -2884,7 +2884,7 @@
         <v>106</v>
       </c>
       <c r="J13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K13" t="s">
         <v>107</v>
@@ -2893,7 +2893,7 @@
         <v>108</v>
       </c>
       <c r="M13" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
@@ -2904,7 +2904,7 @@
         <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
         <v>110</v>
@@ -2925,7 +2925,7 @@
         <v>113</v>
       </c>
       <c r="J14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K14" t="s">
         <v>114</v>
@@ -2934,7 +2934,7 @@
         <v>115</v>
       </c>
       <c r="M14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
@@ -2945,13 +2945,13 @@
         <v>116</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
         <v>117</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s">
         <v>118</v>
@@ -2966,7 +2966,7 @@
         <v>120</v>
       </c>
       <c r="J15" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K15" t="s">
         <v>121</v>
@@ -2975,7 +2975,7 @@
         <v>122</v>
       </c>
       <c r="M15" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
@@ -2986,7 +2986,7 @@
         <v>123</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
         <v>124</v>
@@ -3007,7 +3007,7 @@
         <v>127</v>
       </c>
       <c r="J16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K16" t="s">
         <v>128</v>
@@ -3016,7 +3016,7 @@
         <v>129</v>
       </c>
       <c r="M16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17">
@@ -3027,7 +3027,7 @@
         <v>130</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17" t="s">
         <v>131</v>
@@ -3048,7 +3048,7 @@
         <v>134</v>
       </c>
       <c r="J17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K17" t="s">
         <v>135</v>
@@ -3057,7 +3057,7 @@
         <v>136</v>
       </c>
       <c r="M17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
@@ -3068,13 +3068,13 @@
         <v>137</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
         <v>138</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
         <v>118</v>
@@ -3089,7 +3089,7 @@
         <v>140</v>
       </c>
       <c r="J18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K18" t="s">
         <v>141</v>
@@ -3098,7 +3098,7 @@
         <v>142</v>
       </c>
       <c r="M18" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19">
@@ -3109,7 +3109,7 @@
         <v>143</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
         <v>144</v>
@@ -3128,7 +3128,7 @@
         <v>147</v>
       </c>
       <c r="J19" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K19" t="s">
         <v>148</v>
@@ -3137,7 +3137,7 @@
         <v>149</v>
       </c>
       <c r="M19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20">
@@ -3176,7 +3176,7 @@
         <v>155</v>
       </c>
       <c r="M20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21">
@@ -3187,7 +3187,7 @@
         <v>156</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -3208,7 +3208,7 @@
         <v>158</v>
       </c>
       <c r="J21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K21" t="s">
         <v>159</v>
@@ -3217,7 +3217,7 @@
         <v>160</v>
       </c>
       <c r="M21" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22">
@@ -3228,13 +3228,13 @@
         <v>161</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
         <v>162</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F22" t="s">
         <v>152</v>
@@ -3249,7 +3249,7 @@
         <v>164</v>
       </c>
       <c r="J22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K22" t="s">
         <v>165</v>
@@ -3258,7 +3258,7 @@
         <v>166</v>
       </c>
       <c r="M22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23">
@@ -3269,7 +3269,7 @@
         <v>167</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
         <v>168</v>
@@ -3290,7 +3290,7 @@
         <v>171</v>
       </c>
       <c r="J23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K23" t="s">
         <v>172</v>
@@ -3299,7 +3299,7 @@
         <v>173</v>
       </c>
       <c r="M23" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24">
@@ -3310,7 +3310,7 @@
         <v>174</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
         <v>131</v>
@@ -3331,7 +3331,7 @@
         <v>177</v>
       </c>
       <c r="J24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K24" t="s">
         <v>178</v>
@@ -3340,7 +3340,7 @@
         <v>179</v>
       </c>
       <c r="M24" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25">
@@ -3379,7 +3379,7 @@
         <v>187</v>
       </c>
       <c r="M25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26">
@@ -3420,7 +3420,7 @@
         <v>194</v>
       </c>
       <c r="M26" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27">
@@ -3431,13 +3431,13 @@
         <v>195</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
         <v>138</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
         <v>190</v>
@@ -3452,7 +3452,7 @@
         <v>197</v>
       </c>
       <c r="J27" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K27" t="s">
         <v>198</v>
@@ -3461,7 +3461,7 @@
         <v>199</v>
       </c>
       <c r="M27" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28">
@@ -3502,7 +3502,7 @@
         <v>203</v>
       </c>
       <c r="M28" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29">
@@ -3513,7 +3513,7 @@
         <v>204</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
         <v>205</v>
@@ -3534,7 +3534,7 @@
         <v>207</v>
       </c>
       <c r="J29" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K29" t="s">
         <v>208</v>
@@ -3543,7 +3543,7 @@
         <v>209</v>
       </c>
       <c r="M29" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30">
@@ -3554,7 +3554,7 @@
         <v>210</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
         <v>211</v>
@@ -3575,7 +3575,7 @@
         <v>214</v>
       </c>
       <c r="J30" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K30" t="s">
         <v>215</v>
@@ -3584,7 +3584,7 @@
         <v>216</v>
       </c>
       <c r="M30" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31">
@@ -3595,7 +3595,7 @@
         <v>217</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s">
         <v>218</v>
@@ -3616,7 +3616,7 @@
         <v>220</v>
       </c>
       <c r="J31" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K31" t="s">
         <v>221</v>
@@ -3625,7 +3625,7 @@
         <v>222</v>
       </c>
       <c r="M31" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32">
@@ -3642,7 +3642,7 @@
         <v>224</v>
       </c>
       <c r="E32" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F32" t="s">
         <v>225</v>
@@ -3657,7 +3657,7 @@
         <v>227</v>
       </c>
       <c r="J32" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K32" t="s">
         <v>228</v>
@@ -3666,7 +3666,7 @@
         <v>229</v>
       </c>
       <c r="M32" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33">
@@ -3677,7 +3677,7 @@
         <v>230</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D33" t="s">
         <v>231</v>
@@ -3698,7 +3698,7 @@
         <v>234</v>
       </c>
       <c r="J33" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K33" t="s">
         <v>235</v>
@@ -3707,7 +3707,7 @@
         <v>236</v>
       </c>
       <c r="M33" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34">
@@ -3748,7 +3748,7 @@
         <v>243</v>
       </c>
       <c r="M34" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35">
@@ -3759,7 +3759,7 @@
         <v>244</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D35" t="s">
         <v>245</v>
@@ -3780,7 +3780,7 @@
         <v>248</v>
       </c>
       <c r="J35" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K35" t="s">
         <v>249</v>
@@ -3789,7 +3789,7 @@
         <v>250</v>
       </c>
       <c r="M35" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36">
@@ -3800,7 +3800,7 @@
         <v>251</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D36" t="s">
         <v>252</v>
@@ -3821,7 +3821,7 @@
         <v>254</v>
       </c>
       <c r="J36" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K36" t="s">
         <v>255</v>
@@ -3830,7 +3830,7 @@
         <v>256</v>
       </c>
       <c r="M36" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37">
@@ -3841,13 +3841,13 @@
         <v>257</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
         <v>258</v>
       </c>
       <c r="E37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F37" t="s">
         <v>259</v>
@@ -3862,7 +3862,7 @@
         <v>261</v>
       </c>
       <c r="J37" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K37" t="s">
         <v>262</v>
@@ -3871,7 +3871,7 @@
         <v>263</v>
       </c>
       <c r="M37" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38">
@@ -3903,7 +3903,7 @@
         <v>268</v>
       </c>
       <c r="J38" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K38" t="s">
         <v>269</v>
@@ -3912,7 +3912,7 @@
         <v>270</v>
       </c>
       <c r="M38" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39">
@@ -3942,7 +3942,7 @@
         <v>275</v>
       </c>
       <c r="J39" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K39" t="s">
         <v>276</v>
@@ -3951,7 +3951,7 @@
         <v>277</v>
       </c>
       <c r="M39" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40">
@@ -3983,7 +3983,7 @@
         <v>281</v>
       </c>
       <c r="J40" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K40" t="s">
         <v>282</v>
@@ -3992,7 +3992,7 @@
         <v>283</v>
       </c>
       <c r="M40" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41">
@@ -4003,13 +4003,13 @@
         <v>284</v>
       </c>
       <c r="C41" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D41" t="s">
         <v>285</v>
       </c>
       <c r="E41" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F41" t="s">
         <v>279</v>
@@ -4024,7 +4024,7 @@
         <v>287</v>
       </c>
       <c r="J41" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K41" t="s">
         <v>288</v>
@@ -4033,7 +4033,7 @@
         <v>289</v>
       </c>
       <c r="M41" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42">
@@ -4050,7 +4050,7 @@
         <v>291</v>
       </c>
       <c r="E42" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F42" t="s">
         <v>279</v>
@@ -4065,7 +4065,7 @@
         <v>293</v>
       </c>
       <c r="J42" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K42" t="s">
         <v>294</v>
@@ -4074,7 +4074,7 @@
         <v>295</v>
       </c>
       <c r="M42" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43">
@@ -4106,7 +4106,7 @@
         <v>299</v>
       </c>
       <c r="J43" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K43" t="s">
         <v>300</v>
@@ -4115,7 +4115,7 @@
         <v>301</v>
       </c>
       <c r="M43" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44">
@@ -4132,7 +4132,7 @@
         <v>304</v>
       </c>
       <c r="E44" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F44" t="s">
         <v>305</v>
@@ -4147,7 +4147,7 @@
         <v>307</v>
       </c>
       <c r="J44" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K44" t="s">
         <v>308</v>
@@ -4156,7 +4156,7 @@
         <v>309</v>
       </c>
       <c r="M44" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45">
@@ -4167,7 +4167,7 @@
         <v>310</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D45" t="s">
         <v>311</v>
@@ -4188,7 +4188,7 @@
         <v>313</v>
       </c>
       <c r="J45" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K45" t="s">
         <v>314</v>
@@ -4197,7 +4197,7 @@
         <v>315</v>
       </c>
       <c r="M45" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46">
@@ -4208,7 +4208,7 @@
         <v>316</v>
       </c>
       <c r="C46" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D46" t="s">
         <v>317</v>
@@ -4229,7 +4229,7 @@
         <v>319</v>
       </c>
       <c r="J46" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K46" t="s">
         <v>320</v>
@@ -4238,7 +4238,7 @@
         <v>321</v>
       </c>
       <c r="M46" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47">
@@ -4249,7 +4249,7 @@
         <v>322</v>
       </c>
       <c r="C47" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
         <v>323</v>
@@ -4270,7 +4270,7 @@
         <v>325</v>
       </c>
       <c r="J47" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K47" t="s">
         <v>326</v>
@@ -4279,7 +4279,7 @@
         <v>327</v>
       </c>
       <c r="M47" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48">
@@ -4290,7 +4290,7 @@
         <v>328</v>
       </c>
       <c r="C48" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D48" t="s">
         <v>317</v>
@@ -4311,7 +4311,7 @@
         <v>330</v>
       </c>
       <c r="J48" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K48" t="s">
         <v>331</v>
@@ -4320,7 +4320,7 @@
         <v>332</v>
       </c>
       <c r="M48" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49">
@@ -4361,7 +4361,7 @@
         <v>338</v>
       </c>
       <c r="M49" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50">
@@ -4372,13 +4372,13 @@
         <v>339</v>
       </c>
       <c r="C50" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D50" t="s">
         <v>340</v>
       </c>
       <c r="E50" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F50" t="s">
         <v>341</v>
@@ -4393,7 +4393,7 @@
         <v>343</v>
       </c>
       <c r="J50" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K50" t="s">
         <v>344</v>
@@ -4402,7 +4402,7 @@
         <v>345</v>
       </c>
       <c r="M50" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51">
@@ -4413,13 +4413,13 @@
         <v>346</v>
       </c>
       <c r="C51" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D51" t="s">
         <v>285</v>
       </c>
       <c r="E51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F51" t="s">
         <v>347</v>
@@ -4434,7 +4434,7 @@
         <v>349</v>
       </c>
       <c r="J51" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K51" t="s">
         <v>350</v>
@@ -4443,7 +4443,7 @@
         <v>351</v>
       </c>
       <c r="M51" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52">
@@ -4475,7 +4475,7 @@
         <v>357</v>
       </c>
       <c r="J52" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K52" t="s">
         <v>358</v>
@@ -4484,7 +4484,7 @@
         <v>359</v>
       </c>
       <c r="M52" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53">
@@ -4495,13 +4495,13 @@
         <v>360</v>
       </c>
       <c r="C53" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D53" t="s">
         <v>117</v>
       </c>
       <c r="E53" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F53" t="s">
         <v>355</v>
@@ -4516,7 +4516,7 @@
         <v>362</v>
       </c>
       <c r="J53" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K53" t="s">
         <v>363</v>
@@ -4525,7 +4525,7 @@
         <v>364</v>
       </c>
       <c r="M53" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54">
@@ -4536,7 +4536,7 @@
         <v>365</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D54" t="s">
         <v>265</v>
@@ -4557,7 +4557,7 @@
         <v>367</v>
       </c>
       <c r="J54" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K54" t="s">
         <v>368</v>
@@ -4566,7 +4566,7 @@
         <v>369</v>
       </c>
       <c r="M54" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55">
@@ -4577,13 +4577,13 @@
         <v>370</v>
       </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D55" t="s">
         <v>371</v>
       </c>
       <c r="E55" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F55" t="s">
         <v>355</v>
@@ -4598,7 +4598,7 @@
         <v>373</v>
       </c>
       <c r="J55" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K55" t="s">
         <v>374</v>
@@ -4607,7 +4607,7 @@
         <v>375</v>
       </c>
       <c r="M55" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56">
@@ -4618,7 +4618,7 @@
         <v>376</v>
       </c>
       <c r="C56" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D56" t="s">
         <v>377</v>
@@ -4639,7 +4639,7 @@
         <v>381</v>
       </c>
       <c r="J56" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K56" t="s">
         <v>382</v>
@@ -4648,7 +4648,7 @@
         <v>383</v>
       </c>
       <c r="M56" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57">
@@ -4659,7 +4659,7 @@
         <v>384</v>
       </c>
       <c r="C57" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D57" t="s">
         <v>385</v>
@@ -4680,7 +4680,7 @@
         <v>387</v>
       </c>
       <c r="J57" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K57" t="s">
         <v>388</v>
@@ -4689,7 +4689,7 @@
         <v>389</v>
       </c>
       <c r="M57" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58">
@@ -4719,7 +4719,7 @@
         <v>394</v>
       </c>
       <c r="J58" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K58" t="s">
         <v>395</v>
@@ -4728,7 +4728,7 @@
         <v>396</v>
       </c>
       <c r="M58" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59">
@@ -4739,7 +4739,7 @@
         <v>397</v>
       </c>
       <c r="C59" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D59" t="s">
         <v>398</v>
@@ -4760,7 +4760,7 @@
         <v>401</v>
       </c>
       <c r="J59" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K59" t="s">
         <v>402</v>
@@ -4769,7 +4769,7 @@
         <v>403</v>
       </c>
       <c r="M59" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60">
@@ -4780,7 +4780,7 @@
         <v>404</v>
       </c>
       <c r="C60" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D60" t="s">
         <v>231</v>
@@ -4801,7 +4801,7 @@
         <v>406</v>
       </c>
       <c r="J60" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K60" t="s">
         <v>407</v>
@@ -4810,7 +4810,7 @@
         <v>408</v>
       </c>
       <c r="M60" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61">
@@ -4821,7 +4821,7 @@
         <v>409</v>
       </c>
       <c r="C61" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D61" t="s">
         <v>410</v>
@@ -4842,7 +4842,7 @@
         <v>413</v>
       </c>
       <c r="J61" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K61" t="s">
         <v>414</v>
@@ -4851,7 +4851,7 @@
         <v>415</v>
       </c>
       <c r="M61" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62">
@@ -4862,7 +4862,7 @@
         <v>416</v>
       </c>
       <c r="C62" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D62" t="s">
         <v>417</v>
@@ -4883,7 +4883,7 @@
         <v>419</v>
       </c>
       <c r="J62" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K62" t="s">
         <v>420</v>
@@ -4892,7 +4892,7 @@
         <v>421</v>
       </c>
       <c r="M62" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="63">
@@ -4903,13 +4903,13 @@
         <v>422</v>
       </c>
       <c r="C63" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D63" t="s">
         <v>423</v>
       </c>
       <c r="E63" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F63" t="s">
         <v>424</v>
@@ -4924,7 +4924,7 @@
         <v>426</v>
       </c>
       <c r="J63" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K63" t="s">
         <v>427</v>
@@ -4933,7 +4933,7 @@
         <v>428</v>
       </c>
       <c r="M63" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64">
@@ -4944,13 +4944,13 @@
         <v>429</v>
       </c>
       <c r="C64" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D64" t="s">
         <v>430</v>
       </c>
       <c r="E64" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F64" t="s">
         <v>431</v>
@@ -4965,7 +4965,7 @@
         <v>433</v>
       </c>
       <c r="J64" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K64" t="s">
         <v>434</v>
@@ -4974,7 +4974,7 @@
         <v>435</v>
       </c>
       <c r="M64" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="65">
@@ -4985,7 +4985,7 @@
         <v>436</v>
       </c>
       <c r="C65" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D65" t="s">
         <v>297</v>
@@ -5006,7 +5006,7 @@
         <v>439</v>
       </c>
       <c r="J65" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K65" t="s">
         <v>440</v>
@@ -5015,7 +5015,7 @@
         <v>441</v>
       </c>
       <c r="M65" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66">
@@ -5026,13 +5026,13 @@
         <v>442</v>
       </c>
       <c r="C66" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D66" t="s">
         <v>443</v>
       </c>
       <c r="E66" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F66" t="s">
         <v>437</v>
@@ -5047,7 +5047,7 @@
         <v>445</v>
       </c>
       <c r="J66" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K66" t="s">
         <v>446</v>
@@ -5056,7 +5056,7 @@
         <v>447</v>
       </c>
       <c r="M66" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67">
@@ -5067,13 +5067,13 @@
         <v>448</v>
       </c>
       <c r="C67" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D67" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E67" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F67" t="s">
         <v>437</v>
@@ -5088,7 +5088,7 @@
         <v>450</v>
       </c>
       <c r="J67" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K67" t="s">
         <v>451</v>
@@ -5097,7 +5097,7 @@
         <v>452</v>
       </c>
       <c r="M67" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68">
@@ -5108,7 +5108,7 @@
         <v>453</v>
       </c>
       <c r="C68" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D68" t="s">
         <v>131</v>
@@ -5129,7 +5129,7 @@
         <v>455</v>
       </c>
       <c r="J68" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K68" t="s">
         <v>456</v>
@@ -5138,7 +5138,7 @@
         <v>457</v>
       </c>
       <c r="M68" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69">
@@ -5170,7 +5170,7 @@
         <v>460</v>
       </c>
       <c r="J69" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K69" t="s">
         <v>461</v>
@@ -5179,7 +5179,7 @@
         <v>462</v>
       </c>
       <c r="M69" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70">
@@ -5190,13 +5190,13 @@
         <v>463</v>
       </c>
       <c r="C70" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D70" t="s">
         <v>464</v>
       </c>
       <c r="E70" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F70" t="s">
         <v>437</v>
@@ -5211,7 +5211,7 @@
         <v>466</v>
       </c>
       <c r="J70" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K70" t="s">
         <v>467</v>
@@ -5220,7 +5220,7 @@
         <v>468</v>
       </c>
       <c r="M70" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71">
@@ -5261,7 +5261,7 @@
         <v>475</v>
       </c>
       <c r="M71" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72">
@@ -5272,13 +5272,13 @@
         <v>476</v>
       </c>
       <c r="C72" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D72" t="s">
         <v>477</v>
       </c>
       <c r="E72" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F72" t="s">
         <v>471</v>
@@ -5293,7 +5293,7 @@
         <v>479</v>
       </c>
       <c r="J72" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K72" t="s">
         <v>480</v>
@@ -5302,7 +5302,7 @@
         <v>481</v>
       </c>
       <c r="M72" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73">
@@ -5313,7 +5313,7 @@
         <v>482</v>
       </c>
       <c r="C73" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D73" t="s">
         <v>265</v>
@@ -5334,7 +5334,7 @@
         <v>485</v>
       </c>
       <c r="J73" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K73" t="s">
         <v>486</v>
@@ -5343,7 +5343,7 @@
         <v>487</v>
       </c>
       <c r="M73" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74">
@@ -5354,7 +5354,7 @@
         <v>488</v>
       </c>
       <c r="C74" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D74" t="s">
         <v>297</v>
@@ -5375,7 +5375,7 @@
         <v>490</v>
       </c>
       <c r="J74" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K74" t="s">
         <v>491</v>
@@ -5384,7 +5384,7 @@
         <v>492</v>
       </c>
       <c r="M74" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="75">
@@ -5395,7 +5395,7 @@
         <v>493</v>
       </c>
       <c r="C75" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D75" t="s">
         <v>124</v>
@@ -5416,7 +5416,7 @@
         <v>495</v>
       </c>
       <c r="J75" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K75" t="s">
         <v>496</v>
@@ -5425,7 +5425,7 @@
         <v>497</v>
       </c>
       <c r="M75" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76">
@@ -5436,7 +5436,7 @@
         <v>498</v>
       </c>
       <c r="C76" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D76" t="s">
         <v>124</v>
@@ -5457,7 +5457,7 @@
         <v>500</v>
       </c>
       <c r="J76" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K76" t="s">
         <v>501</v>
@@ -5466,7 +5466,7 @@
         <v>502</v>
       </c>
       <c r="M76" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77">
@@ -5477,7 +5477,7 @@
         <v>503</v>
       </c>
       <c r="C77" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D77" t="s">
         <v>504</v>
@@ -5498,7 +5498,7 @@
         <v>507</v>
       </c>
       <c r="J77" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K77" t="s">
         <v>508</v>
@@ -5507,7 +5507,7 @@
         <v>509</v>
       </c>
       <c r="M77" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="78">
@@ -5518,7 +5518,7 @@
         <v>510</v>
       </c>
       <c r="C78" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D78" t="s">
         <v>511</v>
@@ -5539,7 +5539,7 @@
         <v>513</v>
       </c>
       <c r="J78" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K78" t="s">
         <v>514</v>
@@ -5548,7 +5548,7 @@
         <v>515</v>
       </c>
       <c r="M78" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="79">
@@ -5559,13 +5559,13 @@
         <v>516</v>
       </c>
       <c r="C79" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D79" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E79" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F79" t="s">
         <v>517</v>
@@ -5580,7 +5580,7 @@
         <v>519</v>
       </c>
       <c r="J79" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K79" t="s">
         <v>520</v>
@@ -5589,7 +5589,7 @@
         <v>521</v>
       </c>
       <c r="M79" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="80">
@@ -5600,7 +5600,7 @@
         <v>522</v>
       </c>
       <c r="C80" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D80" t="s">
         <v>523</v>
@@ -5621,7 +5621,7 @@
         <v>525</v>
       </c>
       <c r="J80" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K80" t="s">
         <v>526</v>
@@ -5630,7 +5630,7 @@
         <v>527</v>
       </c>
       <c r="M80" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81">
@@ -5641,13 +5641,13 @@
         <v>528</v>
       </c>
       <c r="C81" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D81" t="s">
         <v>529</v>
       </c>
       <c r="E81" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F81" t="s">
         <v>530</v>
@@ -5662,7 +5662,7 @@
         <v>532</v>
       </c>
       <c r="J81" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K81" t="s">
         <v>533</v>
@@ -5671,7 +5671,7 @@
         <v>534</v>
       </c>
       <c r="M81" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="82">
@@ -5682,13 +5682,13 @@
         <v>535</v>
       </c>
       <c r="C82" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D82" t="s">
         <v>536</v>
       </c>
       <c r="E82" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F82" t="s">
         <v>530</v>
@@ -5703,7 +5703,7 @@
         <v>538</v>
       </c>
       <c r="J82" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K82" t="s">
         <v>539</v>
@@ -5712,7 +5712,7 @@
         <v>540</v>
       </c>
       <c r="M82" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83">
@@ -5729,7 +5729,7 @@
         <v>536</v>
       </c>
       <c r="E83" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F83" t="s">
         <v>530</v>
@@ -5744,7 +5744,7 @@
         <v>543</v>
       </c>
       <c r="J83" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K83" t="s">
         <v>544</v>
@@ -5753,7 +5753,7 @@
         <v>545</v>
       </c>
       <c r="M83" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="84">
@@ -5794,7 +5794,7 @@
         <v>553</v>
       </c>
       <c r="M84" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85">
@@ -5805,7 +5805,7 @@
         <v>554</v>
       </c>
       <c r="C85" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D85" t="s">
         <v>238</v>
@@ -5826,7 +5826,7 @@
         <v>557</v>
       </c>
       <c r="J85" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K85" t="s">
         <v>558</v>
@@ -5835,7 +5835,7 @@
         <v>559</v>
       </c>
       <c r="M85" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="86">
@@ -5846,7 +5846,7 @@
         <v>560</v>
       </c>
       <c r="C86" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D86" t="s">
         <v>561</v>
@@ -5867,7 +5867,7 @@
         <v>564</v>
       </c>
       <c r="J86" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K86" t="s">
         <v>565</v>
@@ -5876,7 +5876,7 @@
         <v>566</v>
       </c>
       <c r="M86" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="87">
@@ -5906,7 +5906,7 @@
         <v>571</v>
       </c>
       <c r="J87" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K87" t="s">
         <v>572</v>
@@ -5915,7 +5915,7 @@
         <v>573</v>
       </c>
       <c r="M87" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88">
@@ -5926,7 +5926,7 @@
         <v>574</v>
       </c>
       <c r="C88" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D88" t="s">
         <v>575</v>
@@ -5954,7 +5954,7 @@
         <v>580</v>
       </c>
       <c r="M88" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="89">
@@ -5984,7 +5984,7 @@
         <v>585</v>
       </c>
       <c r="J89" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K89" t="s">
         <v>586</v>
@@ -5993,7 +5993,7 @@
         <v>587</v>
       </c>
       <c r="M89" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="90">
@@ -6004,13 +6004,13 @@
         <v>588</v>
       </c>
       <c r="C90" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D90" t="s">
         <v>589</v>
       </c>
       <c r="E90" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F90" t="s">
         <v>590</v>
@@ -6025,7 +6025,7 @@
         <v>592</v>
       </c>
       <c r="J90" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K90" t="s">
         <v>593</v>
@@ -6034,7 +6034,7 @@
         <v>594</v>
       </c>
       <c r="M90" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91">
@@ -6066,7 +6066,7 @@
         <v>598</v>
       </c>
       <c r="J91" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K91" t="s">
         <v>599</v>
@@ -6075,7 +6075,7 @@
         <v>600</v>
       </c>
       <c r="M91" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="92">
@@ -6086,13 +6086,13 @@
         <v>601</v>
       </c>
       <c r="C92" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D92" t="s">
         <v>602</v>
       </c>
       <c r="E92" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F92" t="s">
         <v>596</v>
@@ -6107,7 +6107,7 @@
         <v>604</v>
       </c>
       <c r="J92" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K92" t="s">
         <v>605</v>
@@ -6116,7 +6116,7 @@
         <v>606</v>
       </c>
       <c r="M92" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="93">
@@ -6148,7 +6148,7 @@
         <v>611</v>
       </c>
       <c r="J93" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K93" t="s">
         <v>612</v>
@@ -6157,7 +6157,7 @@
         <v>613</v>
       </c>
       <c r="M93" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="94">
@@ -6189,7 +6189,7 @@
         <v>617</v>
       </c>
       <c r="J94" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K94" t="s">
         <v>618</v>
@@ -6198,7 +6198,7 @@
         <v>619</v>
       </c>
       <c r="M94" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="95">
@@ -6209,13 +6209,13 @@
         <v>620</v>
       </c>
       <c r="C95" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D95" t="s">
         <v>621</v>
       </c>
       <c r="E95" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F95" t="s">
         <v>622</v>
@@ -6230,7 +6230,7 @@
         <v>624</v>
       </c>
       <c r="J95" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K95" t="s">
         <v>625</v>
@@ -6239,7 +6239,7 @@
         <v>626</v>
       </c>
       <c r="M95" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96">
@@ -6250,7 +6250,7 @@
         <v>627</v>
       </c>
       <c r="C96" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D96" t="s">
         <v>265</v>
@@ -6271,7 +6271,7 @@
         <v>630</v>
       </c>
       <c r="J96" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K96" t="s">
         <v>631</v>
@@ -6280,7 +6280,7 @@
         <v>632</v>
       </c>
       <c r="M96" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="97">
@@ -6291,13 +6291,13 @@
         <v>633</v>
       </c>
       <c r="C97" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D97" t="s">
         <v>138</v>
       </c>
       <c r="E97" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F97" t="s">
         <v>634</v>
@@ -6312,7 +6312,7 @@
         <v>636</v>
       </c>
       <c r="J97" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K97" t="s">
         <v>637</v>
@@ -6321,7 +6321,7 @@
         <v>638</v>
       </c>
       <c r="M97" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="98">
@@ -6332,13 +6332,13 @@
         <v>639</v>
       </c>
       <c r="C98" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D98" t="s">
         <v>98</v>
       </c>
       <c r="E98" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F98" t="s">
         <v>640</v>
@@ -6353,7 +6353,7 @@
         <v>642</v>
       </c>
       <c r="J98" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K98" t="s">
         <v>643</v>
@@ -6362,7 +6362,7 @@
         <v>644</v>
       </c>
       <c r="M98" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="99">
@@ -6373,7 +6373,7 @@
         <v>645</v>
       </c>
       <c r="C99" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D99" t="s">
         <v>646</v>
@@ -6394,7 +6394,7 @@
         <v>649</v>
       </c>
       <c r="J99" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K99" t="s">
         <v>650</v>
@@ -6403,7 +6403,7 @@
         <v>651</v>
       </c>
       <c r="M99" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="100">
@@ -6414,7 +6414,7 @@
         <v>652</v>
       </c>
       <c r="C100" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D100" t="s">
         <v>653</v>
@@ -6435,7 +6435,7 @@
         <v>656</v>
       </c>
       <c r="J100" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K100" t="s">
         <v>657</v>
@@ -6444,7 +6444,7 @@
         <v>658</v>
       </c>
       <c r="M100" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="101">
@@ -6474,7 +6474,7 @@
         <v>663</v>
       </c>
       <c r="J101" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K101" t="s">
         <v>664</v>
@@ -6483,7 +6483,7 @@
         <v>665</v>
       </c>
       <c r="M101" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update parliament data - 2026-02-15
</commit_message>
<xml_diff>
--- a/Objets_parlementaires_CDF_EFK.xlsx
+++ b/Objets_parlementaires_CDF_EFK.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="662">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">Élu &amp; Conseil fédéral</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-14</t>
+    <t xml:space="preserve">2026-02-15</t>
   </si>
   <si>
     <t xml:space="preserve">25.4620</t>
@@ -1860,24 +1860,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20243169</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.3077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-03-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dringende Wiederherstellung der Verteidigungsfähigkeit der Schweizer Armee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rétablir d'urgence la capacité de défense de notre armée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.parlament.ch/de/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20243077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20243077</t>
   </si>
   <si>
     <t xml:space="preserve">24.7112</t>
@@ -2074,8 +2056,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N101" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:N101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N100" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:N100"/>
   <tableColumns count="14">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Numéro"/>
@@ -6323,61 +6305,61 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>20243077</v>
+        <v>20247112</v>
       </c>
       <c r="B94" t="s">
         <v>616</v>
       </c>
       <c r="C94" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D94" t="s">
-        <v>16</v>
+        <v>617</v>
       </c>
       <c r="E94" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="F94" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="G94" t="s">
         <v>19</v>
       </c>
       <c r="H94" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="I94" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="J94" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="K94" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="L94" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="M94" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N94"/>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>20247112</v>
+        <v>20247015</v>
       </c>
       <c r="B95" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C95" t="s">
         <v>47</v>
       </c>
       <c r="D95" t="s">
-        <v>623</v>
+        <v>267</v>
       </c>
       <c r="E95" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="F95" t="s">
         <v>624</v>
@@ -6401,25 +6383,25 @@
         <v>628</v>
       </c>
       <c r="M95" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="N95"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>20247015</v>
+        <v>20234494</v>
       </c>
       <c r="B96" t="s">
         <v>629</v>
       </c>
       <c r="C96" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D96" t="s">
-        <v>267</v>
+        <v>140</v>
       </c>
       <c r="E96" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F96" t="s">
         <v>630</v>
@@ -6449,7 +6431,7 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>20234494</v>
+        <v>20234461</v>
       </c>
       <c r="B97" t="s">
         <v>635</v>
@@ -6458,7 +6440,7 @@
         <v>39</v>
       </c>
       <c r="D97" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="E97" t="s">
         <v>58</v>
@@ -6485,13 +6467,13 @@
         <v>640</v>
       </c>
       <c r="M97" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N97"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>20234461</v>
+        <v>20234375</v>
       </c>
       <c r="B98" t="s">
         <v>641</v>
@@ -6500,160 +6482,118 @@
         <v>39</v>
       </c>
       <c r="D98" t="s">
-        <v>100</v>
+        <v>642</v>
       </c>
       <c r="E98" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="F98" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="G98" t="s">
         <v>19</v>
       </c>
       <c r="H98" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="I98" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="J98" t="s">
         <v>52</v>
       </c>
       <c r="K98" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="L98" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="M98" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N98"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>20234375</v>
+        <v>20234353</v>
       </c>
       <c r="B99" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C99" t="s">
         <v>39</v>
       </c>
       <c r="D99" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E99" t="s">
         <v>17</v>
       </c>
       <c r="F99" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="G99" t="s">
         <v>19</v>
       </c>
       <c r="H99" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="I99" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="J99" t="s">
         <v>52</v>
       </c>
       <c r="K99" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="L99" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="M99" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N99"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>20234353</v>
+        <v>20234346</v>
       </c>
       <c r="B100" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="C100" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D100" t="s">
-        <v>655</v>
-      </c>
-      <c r="E100" t="s">
-        <v>17</v>
-      </c>
+        <v>656</v>
+      </c>
+      <c r="E100"/>
       <c r="F100" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="G100" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H100" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="I100" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="J100" t="s">
         <v>52</v>
       </c>
       <c r="K100" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="L100" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="M100" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N100"/>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>20234346</v>
-      </c>
-      <c r="B101" t="s">
-        <v>661</v>
-      </c>
-      <c r="C101" t="s">
-        <v>15</v>
-      </c>
-      <c r="D101" t="s">
-        <v>662</v>
-      </c>
-      <c r="E101"/>
-      <c r="F101" t="s">
-        <v>663</v>
-      </c>
-      <c r="G101" t="s">
-        <v>31</v>
-      </c>
-      <c r="H101" t="s">
-        <v>664</v>
-      </c>
-      <c r="I101" t="s">
-        <v>665</v>
-      </c>
-      <c r="J101" t="s">
-        <v>52</v>
-      </c>
-      <c r="K101" t="s">
-        <v>666</v>
-      </c>
-      <c r="L101" t="s">
-        <v>667</v>
-      </c>
-      <c r="M101" t="s">
-        <v>37</v>
-      </c>
-      <c r="N101"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update parliament data - 2026-02-16
</commit_message>
<xml_diff>
--- a/Objets_parlementaires_CDF_EFK.xlsx
+++ b/Objets_parlementaires_CDF_EFK.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="668">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">Élu &amp; Conseil fédéral</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-15</t>
+    <t xml:space="preserve">2026-02-16</t>
   </si>
   <si>
     <t xml:space="preserve">25.4620</t>
@@ -224,6 +224,36 @@
     <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254463</t>
   </si>
   <si>
+    <t xml:space="preserve">25.479</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pa. Iv.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golay Roger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-09-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genug Bürokratie! Für einen Frühlingsputz der Gesetze und Verordnungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trop de bureaucratie ! Pour un grand ménage dans les lois et ordonnances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zugewiesen an die behandelnde Kommission / Attribué à la commission compétente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.parlament.ch/de/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20250479</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20250479</t>
+  </si>
+  <si>
     <t xml:space="preserve">25.4281</t>
   </si>
   <si>
@@ -236,9 +266,6 @@
     <t xml:space="preserve">PSS</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-09-26</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wirksamere Koordination der Verkehrsmittel im Rahmen von Agglomerationsprogrammen</t>
   </si>
   <si>
@@ -302,9 +329,6 @@
     <t xml:space="preserve">Garantir la sécurité de l'approvisionnement et un accès rapide aux médicaments innovants</t>
   </si>
   <si>
-    <t xml:space="preserve">Zugewiesen an die behandelnde Kommission / Attribué à la commission compétente</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.parlament.ch/de/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254188</t>
   </si>
   <si>
@@ -1077,12 +1101,6 @@
   </si>
   <si>
     <t xml:space="preserve">25.3054</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Golay Roger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCG</t>
   </si>
   <si>
     <t xml:space="preserve">2025-03-05</t>
@@ -2056,8 +2074,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N100" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:N100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N101" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:N101"/>
   <tableColumns count="14">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Numéro"/>
@@ -2673,7 +2691,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>20254281</v>
+        <v>20250479</v>
       </c>
       <c r="B8" t="s">
         <v>70</v>
@@ -2700,16 +2718,16 @@
         <v>76</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="K8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M8" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="N8" t="s">
         <v>26</v>
@@ -2717,19 +2735,19 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>20254317</v>
+        <v>20254281</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="F9" t="s">
         <v>74</v>
@@ -2738,19 +2756,19 @@
         <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I9" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="K9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="L9" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M9" t="s">
         <v>25</v>
@@ -2761,43 +2779,43 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>20254145</v>
+        <v>20254317</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="K10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="M10" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N10" t="s">
         <v>26</v>
@@ -2805,40 +2823,40 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>20254188</v>
+        <v>20254145</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="G11" t="s">
         <v>31</v>
       </c>
       <c r="H11" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I11" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="K11" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="L11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M11" t="s">
         <v>55</v>
@@ -2849,43 +2867,43 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>20254225</v>
+        <v>20254188</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H12" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I12" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="K12" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="M12" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N12" t="s">
         <v>26</v>
@@ -2893,43 +2911,43 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>20254234</v>
+        <v>20254225</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I13" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="K13" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="M13" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="N13" t="s">
         <v>26</v>
@@ -2937,43 +2955,43 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>20254071</v>
+        <v>20254234</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="F14" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M14" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N14" t="s">
         <v>26</v>
@@ -2981,43 +2999,43 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>20254024</v>
+        <v>20254071</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C15" t="s">
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G15" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H15" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I15" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="K15" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L15" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M15" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N15" t="s">
         <v>26</v>
@@ -3025,43 +3043,43 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>20257863</v>
+        <v>20254024</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E16" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
       <c r="F16" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G16" t="s">
         <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="K16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="L16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M16" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N16" t="s">
         <v>26</v>
@@ -3069,43 +3087,43 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>20257888</v>
+        <v>20257863</v>
       </c>
       <c r="B17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F17" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G17" t="s">
         <v>19</v>
       </c>
       <c r="H17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M17" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N17" t="s">
         <v>26</v>
@@ -3113,43 +3131,43 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>20257890</v>
+        <v>20257888</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C18" t="s">
         <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>142</v>
       </c>
       <c r="F18" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="G18" t="s">
         <v>19</v>
       </c>
       <c r="H18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I18" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K18" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="L18" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="M18" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="N18" t="s">
         <v>26</v>
@@ -3157,41 +3175,43 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>20254003</v>
+        <v>20257890</v>
       </c>
       <c r="B19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
-      </c>
-      <c r="E19"/>
+        <v>148</v>
+      </c>
+      <c r="E19" t="s">
+        <v>58</v>
+      </c>
       <c r="F19" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
       <c r="H19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="K19" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="L19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M19" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N19" t="s">
         <v>26</v>
@@ -3199,38 +3219,38 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>20253984</v>
+        <v>20254003</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E20"/>
       <c r="F20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G20" t="s">
         <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>88</v>
+        <v>156</v>
       </c>
       <c r="I20" t="s">
-        <v>89</v>
+        <v>157</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>155</v>
+        <v>22</v>
       </c>
       <c r="K20" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="L20" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="M20" t="s">
         <v>55</v>
@@ -3241,40 +3261,38 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20257663</v>
+        <v>20253984</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="E21"/>
       <c r="F21" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="G21" t="s">
         <v>19</v>
       </c>
       <c r="H21" t="s">
-        <v>159</v>
+        <v>97</v>
       </c>
       <c r="I21" t="s">
-        <v>160</v>
+        <v>98</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>52</v>
+        <v>163</v>
       </c>
       <c r="K21" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="L21" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="M21" t="s">
         <v>55</v>
@@ -3285,40 +3303,40 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>20257698</v>
+        <v>20257663</v>
       </c>
       <c r="B22" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C22" t="s">
         <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>164</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="F22" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="G22" t="s">
         <v>19</v>
       </c>
       <c r="H22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="I22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="L22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="M22" t="s">
         <v>55</v>
@@ -3329,43 +3347,43 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>20253971</v>
+        <v>20257698</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="F23" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I23" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M23" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N23" t="s">
         <v>26</v>
@@ -3373,40 +3391,40 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>20257601</v>
+        <v>20253971</v>
       </c>
       <c r="B24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>178</v>
       </c>
       <c r="E24" t="s">
-        <v>134</v>
+        <v>29</v>
       </c>
       <c r="F24" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G24" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H24" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="I24" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K24" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="L24" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="M24" t="s">
         <v>25</v>
@@ -3417,32 +3435,34 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>20253941</v>
+        <v>20257601</v>
       </c>
       <c r="B25" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>183</v>
-      </c>
-      <c r="E25"/>
+        <v>141</v>
+      </c>
+      <c r="E25" t="s">
+        <v>142</v>
+      </c>
       <c r="F25" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G25" t="s">
         <v>19</v>
       </c>
       <c r="H25" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I25" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>187</v>
+        <v>52</v>
       </c>
       <c r="K25" t="s">
         <v>188</v>
@@ -3451,7 +3471,7 @@
         <v>189</v>
       </c>
       <c r="M25" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N25" t="s">
         <v>26</v>
@@ -3459,7 +3479,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>20253835</v>
+        <v>20253941</v>
       </c>
       <c r="B26" t="s">
         <v>190</v>
@@ -3470,9 +3490,7 @@
       <c r="D26" t="s">
         <v>191</v>
       </c>
-      <c r="E26" t="s">
-        <v>29</v>
-      </c>
+      <c r="E26"/>
       <c r="F26" t="s">
         <v>192</v>
       </c>
@@ -3485,56 +3503,58 @@
       <c r="I26" t="s">
         <v>194</v>
       </c>
-      <c r="J26" t="s">
-        <v>155</v>
+      <c r="J26" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="K26" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L26" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M26" t="s">
-        <v>37</v>
-      </c>
-      <c r="N26"/>
+        <v>55</v>
+      </c>
+      <c r="N26" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>20253845</v>
+        <v>20253835</v>
       </c>
       <c r="B27" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>140</v>
+        <v>199</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="F27" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="G27" t="s">
         <v>19</v>
       </c>
       <c r="H27" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="I27" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J27" t="s">
-        <v>22</v>
+        <v>163</v>
       </c>
       <c r="K27" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="L27" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="M27" t="s">
         <v>37</v>
@@ -3543,40 +3563,40 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>20253855</v>
+        <v>20253845</v>
       </c>
       <c r="B28" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>203</v>
+        <v>148</v>
       </c>
       <c r="E28" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F28" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="G28" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H28" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="I28" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="J28" t="s">
-        <v>155</v>
+        <v>22</v>
       </c>
       <c r="K28" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="L28" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="M28" t="s">
         <v>37</v>
@@ -3585,40 +3605,40 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>20253880</v>
+        <v>20253855</v>
       </c>
       <c r="B29" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D29" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F29" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="G29" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H29" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="I29" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="J29" t="s">
-        <v>22</v>
+        <v>163</v>
       </c>
       <c r="K29" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="L29" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="M29" t="s">
         <v>37</v>
@@ -3627,40 +3647,40 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>20253892</v>
+        <v>20253880</v>
       </c>
       <c r="B30" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C30" t="s">
         <v>39</v>
       </c>
       <c r="D30" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E30" t="s">
-        <v>214</v>
+        <v>17</v>
       </c>
       <c r="F30" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="G30" t="s">
         <v>19</v>
       </c>
       <c r="H30" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I30" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J30" t="s">
         <v>22</v>
       </c>
       <c r="K30" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L30" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M30" t="s">
         <v>37</v>
@@ -3669,193 +3689,193 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>20253893</v>
+        <v>20253892</v>
       </c>
       <c r="B31" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E31" t="s">
-        <v>29</v>
+        <v>222</v>
       </c>
       <c r="F31" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="G31" t="s">
         <v>19</v>
       </c>
       <c r="H31" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I31" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J31" t="s">
         <v>22</v>
       </c>
       <c r="K31" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="L31" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="M31" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="N31"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>20253730</v>
+        <v>20253893</v>
       </c>
       <c r="B32" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E32" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="F32" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
       <c r="G32" t="s">
         <v>19</v>
       </c>
       <c r="H32" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I32" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J32" t="s">
         <v>22</v>
       </c>
       <c r="K32" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L32" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="M32" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N32"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>20253630</v>
+        <v>20253730</v>
       </c>
       <c r="B33" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E33" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F33" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G33" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H33" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I33" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="J33" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="K33" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L33" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M33" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N33"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>20253637</v>
+        <v>20253630</v>
       </c>
       <c r="B34" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E34" t="s">
-        <v>214</v>
+        <v>29</v>
       </c>
       <c r="F34" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="G34" t="s">
         <v>31</v>
       </c>
       <c r="H34" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="I34" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="J34" t="s">
-        <v>243</v>
+        <v>52</v>
       </c>
       <c r="K34" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="L34" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M34" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N34"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>20257355</v>
+        <v>20253637</v>
       </c>
       <c r="B35" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E35" t="s">
-        <v>17</v>
+        <v>222</v>
       </c>
       <c r="F35" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G35" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H35" t="s">
         <v>249</v>
@@ -3864,13 +3884,13 @@
         <v>250</v>
       </c>
       <c r="J35" t="s">
-        <v>52</v>
+        <v>251</v>
       </c>
       <c r="K35" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="L35" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M35" t="s">
         <v>55</v>
@@ -3879,40 +3899,40 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>20257419</v>
+        <v>20257355</v>
       </c>
       <c r="B36" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C36" t="s">
         <v>47</v>
       </c>
       <c r="D36" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E36" t="s">
         <v>17</v>
       </c>
       <c r="F36" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="G36" t="s">
         <v>19</v>
       </c>
       <c r="H36" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="I36" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="J36" t="s">
         <v>52</v>
       </c>
       <c r="K36" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="L36" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="M36" t="s">
         <v>55</v>
@@ -3921,164 +3941,164 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>20253479</v>
+        <v>20257419</v>
       </c>
       <c r="B37" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C37" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D37" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E37" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="F37" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="G37" t="s">
         <v>19</v>
       </c>
       <c r="H37" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I37" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="J37" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="K37" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="L37" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M37" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N37"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>20253444</v>
+        <v>20253479</v>
       </c>
       <c r="B38" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D38" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E38" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="F38" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G38" t="s">
         <v>19</v>
       </c>
       <c r="H38" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I38" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J38" t="s">
         <v>22</v>
       </c>
       <c r="K38" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="L38" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M38" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="N38"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>20253425</v>
+        <v>20253444</v>
       </c>
       <c r="B39" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C39" t="s">
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>274</v>
-      </c>
-      <c r="E39"/>
+        <v>275</v>
+      </c>
+      <c r="E39" t="s">
+        <v>29</v>
+      </c>
       <c r="F39" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G39" t="s">
         <v>19</v>
       </c>
       <c r="H39" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="I39" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="J39" t="s">
         <v>22</v>
       </c>
       <c r="K39" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L39" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M39" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="N39"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>20253309</v>
+        <v>20253425</v>
       </c>
       <c r="B40" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C40" t="s">
         <v>15</v>
       </c>
       <c r="D40" t="s">
-        <v>133</v>
-      </c>
-      <c r="E40" t="s">
-        <v>134</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="E40"/>
       <c r="F40" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G40" t="s">
         <v>19</v>
       </c>
       <c r="H40" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="I40" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="J40" t="s">
         <v>22</v>
       </c>
       <c r="K40" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="L40" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="M40" t="s">
         <v>37</v>
@@ -4087,124 +4107,124 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>20253399</v>
+        <v>20253309</v>
       </c>
       <c r="B41" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>287</v>
+        <v>141</v>
       </c>
       <c r="E41" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="F41" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="G41" t="s">
         <v>19</v>
       </c>
       <c r="H41" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="I41" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="J41" t="s">
         <v>22</v>
       </c>
       <c r="K41" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="L41" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="M41" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="N41"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>20253404</v>
+        <v>20253399</v>
       </c>
       <c r="B42" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C42" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D42" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E42" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F42" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="G42" t="s">
         <v>19</v>
       </c>
       <c r="H42" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="I42" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="J42" t="s">
         <v>22</v>
       </c>
       <c r="K42" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="L42" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="M42" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N42"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>20253417</v>
+        <v>20253404</v>
       </c>
       <c r="B43" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C43" t="s">
         <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E43" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="F43" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="G43" t="s">
         <v>19</v>
       </c>
       <c r="H43" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="I43" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="J43" t="s">
         <v>22</v>
       </c>
       <c r="K43" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="L43" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="M43" t="s">
         <v>55</v>
@@ -4213,25 +4233,25 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>20251011</v>
+        <v>20253417</v>
       </c>
       <c r="B44" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C44" t="s">
-        <v>305</v>
+        <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E44" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="F44" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="G44" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H44" t="s">
         <v>308</v>
@@ -4240,7 +4260,7 @@
         <v>309</v>
       </c>
       <c r="J44" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="K44" t="s">
         <v>310</v>
@@ -4255,40 +4275,40 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>20253194</v>
+        <v>20251011</v>
       </c>
       <c r="B45" t="s">
         <v>312</v>
       </c>
       <c r="C45" t="s">
-        <v>39</v>
+        <v>313</v>
       </c>
       <c r="D45" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E45" t="s">
-        <v>214</v>
+        <v>58</v>
       </c>
       <c r="F45" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="G45" t="s">
         <v>31</v>
       </c>
       <c r="H45" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="I45" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="J45" t="s">
         <v>52</v>
       </c>
       <c r="K45" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="L45" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="M45" t="s">
         <v>55</v>
@@ -4297,124 +4317,124 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>20253203</v>
+        <v>20253194</v>
       </c>
       <c r="B46" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C46" t="s">
         <v>39</v>
       </c>
       <c r="D46" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E46" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="F46" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="G46" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H46" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="I46" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="J46" t="s">
         <v>52</v>
       </c>
       <c r="K46" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="L46" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="M46" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N46"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>20253213</v>
+        <v>20253203</v>
       </c>
       <c r="B47" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C47" t="s">
         <v>39</v>
       </c>
       <c r="D47" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E47" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="F47" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="G47" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H47" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="I47" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="J47" t="s">
         <v>52</v>
       </c>
       <c r="K47" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="L47" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="M47" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N47"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>20253214</v>
+        <v>20253213</v>
       </c>
       <c r="B48" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C48" t="s">
         <v>39</v>
       </c>
       <c r="D48" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="E48" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="F48" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="G48" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H48" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="I48" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="J48" t="s">
         <v>52</v>
       </c>
       <c r="K48" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="L48" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="M48" t="s">
         <v>55</v>
@@ -4423,82 +4443,82 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>20253246</v>
+        <v>20253214</v>
       </c>
       <c r="B49" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D49" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E49" t="s">
-        <v>17</v>
+        <v>222</v>
       </c>
       <c r="F49" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="G49" t="s">
         <v>19</v>
       </c>
       <c r="H49" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="I49" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="J49" t="s">
-        <v>155</v>
+        <v>52</v>
       </c>
       <c r="K49" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="L49" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="M49" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N49"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>20253093</v>
+        <v>20253246</v>
       </c>
       <c r="B50" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="E50" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="F50" t="s">
-        <v>343</v>
+        <v>315</v>
       </c>
       <c r="G50" t="s">
         <v>19</v>
       </c>
       <c r="H50" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="I50" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="J50" t="s">
-        <v>22</v>
+        <v>163</v>
       </c>
       <c r="K50" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L50" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="M50" t="s">
         <v>37</v>
@@ -4507,40 +4527,40 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>20257213</v>
+        <v>20253093</v>
       </c>
       <c r="B51" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C51" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D51" t="s">
-        <v>287</v>
+        <v>350</v>
       </c>
       <c r="E51" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F51" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="G51" t="s">
         <v>19</v>
       </c>
       <c r="H51" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="I51" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="J51" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="K51" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="L51" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="M51" t="s">
         <v>37</v>
@@ -4549,19 +4569,19 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>20253054</v>
+        <v>20257213</v>
       </c>
       <c r="B52" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D52" t="s">
-        <v>355</v>
+        <v>295</v>
       </c>
       <c r="E52" t="s">
-        <v>356</v>
+        <v>83</v>
       </c>
       <c r="F52" t="s">
         <v>357</v>
@@ -4576,7 +4596,7 @@
         <v>359</v>
       </c>
       <c r="J52" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="K52" t="s">
         <v>360</v>
@@ -4585,46 +4605,46 @@
         <v>361</v>
       </c>
       <c r="M52" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N52"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>20257102</v>
+        <v>20253054</v>
       </c>
       <c r="B53" t="s">
         <v>362</v>
       </c>
       <c r="C53" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="E53" t="s">
         <v>73</v>
       </c>
       <c r="F53" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="G53" t="s">
         <v>19</v>
       </c>
       <c r="H53" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="I53" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="J53" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="K53" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="L53" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="M53" t="s">
         <v>55</v>
@@ -4633,64 +4653,64 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>20257129</v>
+        <v>20257102</v>
       </c>
       <c r="B54" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C54" t="s">
         <v>47</v>
       </c>
       <c r="D54" t="s">
-        <v>267</v>
+        <v>127</v>
       </c>
       <c r="E54" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="F54" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="G54" t="s">
         <v>19</v>
       </c>
       <c r="H54" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I54" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="J54" t="s">
         <v>52</v>
       </c>
       <c r="K54" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="L54" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="M54" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N54"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>20257138</v>
+        <v>20257129</v>
       </c>
       <c r="B55" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C55" t="s">
         <v>47</v>
       </c>
       <c r="D55" t="s">
-        <v>373</v>
+        <v>275</v>
       </c>
       <c r="E55" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="F55" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="G55" t="s">
         <v>19</v>
@@ -4711,46 +4731,46 @@
         <v>377</v>
       </c>
       <c r="M55" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N55"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>20253031</v>
+        <v>20257138</v>
       </c>
       <c r="B56" t="s">
         <v>378</v>
       </c>
       <c r="C56" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D56" t="s">
         <v>379</v>
       </c>
       <c r="E56" t="s">
+        <v>83</v>
+      </c>
+      <c r="F56" t="s">
+        <v>363</v>
+      </c>
+      <c r="G56" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" t="s">
         <v>380</v>
       </c>
-      <c r="F56" t="s">
+      <c r="I56" t="s">
         <v>381</v>
       </c>
-      <c r="G56" t="s">
-        <v>19</v>
-      </c>
-      <c r="H56" t="s">
+      <c r="J56" t="s">
+        <v>52</v>
+      </c>
+      <c r="K56" t="s">
         <v>382</v>
       </c>
-      <c r="I56" t="s">
+      <c r="L56" t="s">
         <v>383</v>
-      </c>
-      <c r="J56" t="s">
-        <v>22</v>
-      </c>
-      <c r="K56" t="s">
-        <v>384</v>
-      </c>
-      <c r="L56" t="s">
-        <v>385</v>
       </c>
       <c r="M56" t="s">
         <v>55</v>
@@ -4759,22 +4779,22 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>20257012</v>
+        <v>20253031</v>
       </c>
       <c r="B57" t="s">
+        <v>384</v>
+      </c>
+      <c r="C57" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" t="s">
+        <v>385</v>
+      </c>
+      <c r="E57" t="s">
         <v>386</v>
       </c>
-      <c r="C57" t="s">
-        <v>47</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="F57" t="s">
         <v>387</v>
-      </c>
-      <c r="E57" t="s">
-        <v>17</v>
-      </c>
-      <c r="F57" t="s">
-        <v>381</v>
       </c>
       <c r="G57" t="s">
         <v>19</v>
@@ -4786,7 +4806,7 @@
         <v>389</v>
       </c>
       <c r="J57" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="K57" t="s">
         <v>390</v>
@@ -4795,86 +4815,86 @@
         <v>391</v>
       </c>
       <c r="M57" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N57"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>20253008</v>
+        <v>20257012</v>
       </c>
       <c r="B58" t="s">
         <v>392</v>
       </c>
       <c r="C58" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D58" t="s">
         <v>393</v>
       </c>
-      <c r="E58"/>
+      <c r="E58" t="s">
+        <v>17</v>
+      </c>
       <c r="F58" t="s">
+        <v>387</v>
+      </c>
+      <c r="G58" t="s">
+        <v>19</v>
+      </c>
+      <c r="H58" t="s">
         <v>394</v>
       </c>
-      <c r="G58" t="s">
-        <v>19</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="I58" t="s">
         <v>395</v>
-      </c>
-      <c r="I58" t="s">
-        <v>396</v>
       </c>
       <c r="J58" t="s">
         <v>52</v>
       </c>
       <c r="K58" t="s">
+        <v>396</v>
+      </c>
+      <c r="L58" t="s">
         <v>397</v>
       </c>
-      <c r="L58" t="s">
-        <v>398</v>
-      </c>
       <c r="M58" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N58"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>20244404</v>
+        <v>20253008</v>
       </c>
       <c r="B59" t="s">
+        <v>398</v>
+      </c>
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" t="s">
         <v>399</v>
       </c>
-      <c r="C59" t="s">
-        <v>39</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="E59"/>
+      <c r="F59" t="s">
         <v>400</v>
       </c>
-      <c r="E59" t="s">
-        <v>214</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" t="s">
         <v>401</v>
       </c>
-      <c r="G59" t="s">
-        <v>19</v>
-      </c>
-      <c r="H59" t="s">
+      <c r="I59" t="s">
         <v>402</v>
-      </c>
-      <c r="I59" t="s">
-        <v>403</v>
       </c>
       <c r="J59" t="s">
         <v>52</v>
       </c>
       <c r="K59" t="s">
+        <v>403</v>
+      </c>
+      <c r="L59" t="s">
         <v>404</v>
-      </c>
-      <c r="L59" t="s">
-        <v>405</v>
       </c>
       <c r="M59" t="s">
         <v>55</v>
@@ -4883,40 +4903,40 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>20244419</v>
+        <v>20244404</v>
       </c>
       <c r="B60" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C60" t="s">
         <v>39</v>
       </c>
       <c r="D60" t="s">
-        <v>233</v>
+        <v>406</v>
       </c>
       <c r="E60" t="s">
-        <v>29</v>
+        <v>222</v>
       </c>
       <c r="F60" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="G60" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H60" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="I60" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="J60" t="s">
         <v>52</v>
       </c>
       <c r="K60" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="L60" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M60" t="s">
         <v>55</v>
@@ -4925,64 +4945,64 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>20247975</v>
+        <v>20244419</v>
       </c>
       <c r="B61" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C61" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D61" t="s">
-        <v>412</v>
+        <v>241</v>
       </c>
       <c r="E61" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F61" t="s">
+        <v>407</v>
+      </c>
+      <c r="G61" t="s">
+        <v>31</v>
+      </c>
+      <c r="H61" t="s">
         <v>413</v>
       </c>
-      <c r="G61" t="s">
-        <v>19</v>
-      </c>
-      <c r="H61" t="s">
+      <c r="I61" t="s">
         <v>414</v>
-      </c>
-      <c r="I61" t="s">
-        <v>415</v>
       </c>
       <c r="J61" t="s">
         <v>52</v>
       </c>
       <c r="K61" t="s">
+        <v>415</v>
+      </c>
+      <c r="L61" t="s">
         <v>416</v>
       </c>
-      <c r="L61" t="s">
-        <v>417</v>
-      </c>
       <c r="M61" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N61"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>20248043</v>
+        <v>20247975</v>
       </c>
       <c r="B62" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C62" t="s">
         <v>47</v>
       </c>
       <c r="D62" t="s">
+        <v>418</v>
+      </c>
+      <c r="E62" t="s">
+        <v>17</v>
+      </c>
+      <c r="F62" t="s">
         <v>419</v>
-      </c>
-      <c r="E62" t="s">
-        <v>214</v>
-      </c>
-      <c r="F62" t="s">
-        <v>413</v>
       </c>
       <c r="G62" t="s">
         <v>19</v>
@@ -5009,103 +5029,103 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>20244290</v>
+        <v>20248043</v>
       </c>
       <c r="B63" t="s">
         <v>424</v>
       </c>
       <c r="C63" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D63" t="s">
         <v>425</v>
       </c>
       <c r="E63" t="s">
-        <v>58</v>
+        <v>222</v>
       </c>
       <c r="F63" t="s">
+        <v>419</v>
+      </c>
+      <c r="G63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H63" t="s">
         <v>426</v>
       </c>
-      <c r="G63" t="s">
-        <v>19</v>
-      </c>
-      <c r="H63" t="s">
+      <c r="I63" t="s">
         <v>427</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
+        <v>52</v>
+      </c>
+      <c r="K63" t="s">
         <v>428</v>
       </c>
-      <c r="J63" t="s">
-        <v>22</v>
-      </c>
-      <c r="K63" t="s">
+      <c r="L63" t="s">
         <v>429</v>
       </c>
-      <c r="L63" t="s">
-        <v>430</v>
-      </c>
       <c r="M63" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N63"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>20244278</v>
+        <v>20244290</v>
       </c>
       <c r="B64" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C64" t="s">
         <v>39</v>
       </c>
       <c r="D64" t="s">
+        <v>431</v>
+      </c>
+      <c r="E64" t="s">
+        <v>58</v>
+      </c>
+      <c r="F64" t="s">
         <v>432</v>
       </c>
-      <c r="E64" t="s">
-        <v>73</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
+        <v>19</v>
+      </c>
+      <c r="H64" t="s">
         <v>433</v>
       </c>
-      <c r="G64" t="s">
-        <v>19</v>
-      </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>434</v>
-      </c>
-      <c r="I64" t="s">
-        <v>435</v>
       </c>
       <c r="J64" t="s">
         <v>22</v>
       </c>
       <c r="K64" t="s">
+        <v>435</v>
+      </c>
+      <c r="L64" t="s">
         <v>436</v>
       </c>
-      <c r="L64" t="s">
-        <v>437</v>
-      </c>
       <c r="M64" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N64"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>20244082</v>
+        <v>20244278</v>
       </c>
       <c r="B65" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C65" t="s">
         <v>39</v>
       </c>
       <c r="D65" t="s">
-        <v>299</v>
+        <v>438</v>
       </c>
       <c r="E65" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="F65" t="s">
         <v>439</v>
@@ -5129,13 +5149,13 @@
         <v>443</v>
       </c>
       <c r="M65" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N65"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>20244112</v>
+        <v>20244082</v>
       </c>
       <c r="B66" t="s">
         <v>444</v>
@@ -5144,13 +5164,13 @@
         <v>39</v>
       </c>
       <c r="D66" t="s">
+        <v>307</v>
+      </c>
+      <c r="E66" t="s">
+        <v>17</v>
+      </c>
+      <c r="F66" t="s">
         <v>445</v>
-      </c>
-      <c r="E66" t="s">
-        <v>58</v>
-      </c>
-      <c r="F66" t="s">
-        <v>439</v>
       </c>
       <c r="G66" t="s">
         <v>19</v>
@@ -5171,13 +5191,13 @@
         <v>449</v>
       </c>
       <c r="M66" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N66"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>20244131</v>
+        <v>20244112</v>
       </c>
       <c r="B67" t="s">
         <v>450</v>
@@ -5186,115 +5206,115 @@
         <v>39</v>
       </c>
       <c r="D67" t="s">
-        <v>57</v>
+        <v>451</v>
       </c>
       <c r="E67" t="s">
         <v>58</v>
       </c>
       <c r="F67" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="G67" t="s">
         <v>19</v>
       </c>
       <c r="H67" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="I67" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="J67" t="s">
         <v>22</v>
       </c>
       <c r="K67" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="L67" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M67" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N67"/>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>20244132</v>
+        <v>20244131</v>
       </c>
       <c r="B68" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C68" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="D68" t="s">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="E68" t="s">
-        <v>134</v>
+        <v>58</v>
       </c>
       <c r="F68" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="G68" t="s">
         <v>19</v>
       </c>
       <c r="H68" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="I68" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="J68" t="s">
         <v>22</v>
       </c>
       <c r="K68" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="L68" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="M68" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N68"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>20244133</v>
+        <v>20244132</v>
       </c>
       <c r="B69" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C69" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D69" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E69" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="F69" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="G69" t="s">
         <v>19</v>
       </c>
       <c r="H69" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="I69" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="J69" t="s">
         <v>22</v>
       </c>
       <c r="K69" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="L69" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="M69" t="s">
         <v>25</v>
@@ -5303,22 +5323,22 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>20244137</v>
+        <v>20244133</v>
       </c>
       <c r="B70" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C70" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D70" t="s">
-        <v>466</v>
+        <v>141</v>
       </c>
       <c r="E70" t="s">
-        <v>58</v>
+        <v>142</v>
       </c>
       <c r="F70" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="G70" t="s">
         <v>19</v>
@@ -5345,64 +5365,64 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>20243937</v>
+        <v>20244137</v>
       </c>
       <c r="B71" t="s">
         <v>471</v>
       </c>
       <c r="C71" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D71" t="s">
         <v>472</v>
       </c>
       <c r="E71" t="s">
-        <v>214</v>
+        <v>58</v>
       </c>
       <c r="F71" t="s">
+        <v>445</v>
+      </c>
+      <c r="G71" t="s">
+        <v>19</v>
+      </c>
+      <c r="H71" t="s">
         <v>473</v>
       </c>
-      <c r="G71" t="s">
-        <v>31</v>
-      </c>
-      <c r="H71" t="s">
+      <c r="I71" t="s">
         <v>474</v>
       </c>
-      <c r="I71" t="s">
+      <c r="J71" t="s">
+        <v>22</v>
+      </c>
+      <c r="K71" t="s">
         <v>475</v>
       </c>
-      <c r="J71" t="s">
-        <v>187</v>
-      </c>
-      <c r="K71" t="s">
+      <c r="L71" t="s">
         <v>476</v>
       </c>
-      <c r="L71" t="s">
-        <v>477</v>
-      </c>
       <c r="M71" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="N71"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>20243948</v>
+        <v>20243937</v>
       </c>
       <c r="B72" t="s">
+        <v>477</v>
+      </c>
+      <c r="C72" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" t="s">
         <v>478</v>
       </c>
-      <c r="C72" t="s">
-        <v>39</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
+        <v>222</v>
+      </c>
+      <c r="F72" t="s">
         <v>479</v>
-      </c>
-      <c r="E72" t="s">
-        <v>58</v>
-      </c>
-      <c r="F72" t="s">
-        <v>473</v>
       </c>
       <c r="G72" t="s">
         <v>31</v>
@@ -5414,7 +5434,7 @@
         <v>481</v>
       </c>
       <c r="J72" t="s">
-        <v>52</v>
+        <v>195</v>
       </c>
       <c r="K72" t="s">
         <v>482</v>
@@ -5423,31 +5443,31 @@
         <v>483</v>
       </c>
       <c r="M72" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N72"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>20247720</v>
+        <v>20243948</v>
       </c>
       <c r="B73" t="s">
         <v>484</v>
       </c>
       <c r="C73" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D73" t="s">
-        <v>267</v>
+        <v>485</v>
       </c>
       <c r="E73" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F73" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="G73" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H73" t="s">
         <v>486</v>
@@ -5465,13 +5485,13 @@
         <v>489</v>
       </c>
       <c r="M73" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N73"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>20247726</v>
+        <v>20247720</v>
       </c>
       <c r="B74" t="s">
         <v>490</v>
@@ -5480,115 +5500,115 @@
         <v>47</v>
       </c>
       <c r="D74" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="E74" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F74" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="G74" t="s">
         <v>19</v>
       </c>
       <c r="H74" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="I74" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="J74" t="s">
         <v>52</v>
       </c>
       <c r="K74" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="L74" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="M74" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N74"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>20247773</v>
+        <v>20247726</v>
       </c>
       <c r="B75" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C75" t="s">
         <v>47</v>
       </c>
       <c r="D75" t="s">
-        <v>126</v>
+        <v>307</v>
       </c>
       <c r="E75" t="s">
-        <v>127</v>
+        <v>17</v>
       </c>
       <c r="F75" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="G75" t="s">
         <v>19</v>
       </c>
       <c r="H75" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="I75" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="J75" t="s">
         <v>52</v>
       </c>
       <c r="K75" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L75" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="M75" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N75"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>20247774</v>
+        <v>20247773</v>
       </c>
       <c r="B76" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C76" t="s">
         <v>47</v>
       </c>
       <c r="D76" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="E76" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="F76" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="G76" t="s">
         <v>19</v>
       </c>
       <c r="H76" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="I76" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="J76" t="s">
         <v>52</v>
       </c>
       <c r="K76" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="L76" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="M76" t="s">
         <v>25</v>
@@ -5597,64 +5617,64 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>20243858</v>
+        <v>20247774</v>
       </c>
       <c r="B77" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C77" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D77" t="s">
-        <v>506</v>
+        <v>134</v>
       </c>
       <c r="E77" t="s">
-        <v>17</v>
+        <v>135</v>
       </c>
       <c r="F77" t="s">
+        <v>491</v>
+      </c>
+      <c r="G77" t="s">
+        <v>19</v>
+      </c>
+      <c r="H77" t="s">
         <v>507</v>
       </c>
-      <c r="G77" t="s">
-        <v>19</v>
-      </c>
-      <c r="H77" t="s">
+      <c r="I77" t="s">
         <v>508</v>
       </c>
-      <c r="I77" t="s">
+      <c r="J77" t="s">
+        <v>52</v>
+      </c>
+      <c r="K77" t="s">
         <v>509</v>
       </c>
-      <c r="J77" t="s">
-        <v>22</v>
-      </c>
-      <c r="K77" t="s">
+      <c r="L77" t="s">
         <v>510</v>
       </c>
-      <c r="L77" t="s">
-        <v>511</v>
-      </c>
       <c r="M77" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="N77"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>20243877</v>
+        <v>20243858</v>
       </c>
       <c r="B78" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C78" t="s">
         <v>39</v>
       </c>
       <c r="D78" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E78" t="s">
         <v>17</v>
       </c>
       <c r="F78" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="G78" t="s">
         <v>19</v>
@@ -5675,28 +5695,28 @@
         <v>517</v>
       </c>
       <c r="M78" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N78"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>20247622</v>
+        <v>20243877</v>
       </c>
       <c r="B79" t="s">
         <v>518</v>
       </c>
       <c r="C79" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D79" t="s">
-        <v>57</v>
+        <v>519</v>
       </c>
       <c r="E79" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="F79" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="G79" t="s">
         <v>19</v>
@@ -5708,7 +5728,7 @@
         <v>521</v>
       </c>
       <c r="J79" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="K79" t="s">
         <v>522</v>
@@ -5723,7 +5743,7 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>20247649</v>
+        <v>20247622</v>
       </c>
       <c r="B80" t="s">
         <v>524</v>
@@ -5732,13 +5752,13 @@
         <v>47</v>
       </c>
       <c r="D80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E80" t="s">
+        <v>58</v>
+      </c>
+      <c r="F80" t="s">
         <v>525</v>
-      </c>
-      <c r="E80" t="s">
-        <v>29</v>
-      </c>
-      <c r="F80" t="s">
-        <v>519</v>
       </c>
       <c r="G80" t="s">
         <v>19</v>
@@ -5765,64 +5785,64 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>20243709</v>
+        <v>20247649</v>
       </c>
       <c r="B81" t="s">
         <v>530</v>
       </c>
       <c r="C81" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D81" t="s">
         <v>531</v>
       </c>
       <c r="E81" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="F81" t="s">
+        <v>525</v>
+      </c>
+      <c r="G81" t="s">
+        <v>19</v>
+      </c>
+      <c r="H81" t="s">
         <v>532</v>
       </c>
-      <c r="G81" t="s">
-        <v>19</v>
-      </c>
-      <c r="H81" t="s">
+      <c r="I81" t="s">
         <v>533</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J81" t="s">
+        <v>52</v>
+      </c>
+      <c r="K81" t="s">
         <v>534</v>
       </c>
-      <c r="J81" t="s">
-        <v>22</v>
-      </c>
-      <c r="K81" t="s">
+      <c r="L81" t="s">
         <v>535</v>
       </c>
-      <c r="L81" t="s">
-        <v>536</v>
-      </c>
       <c r="M81" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N81"/>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>20243773</v>
+        <v>20243709</v>
       </c>
       <c r="B82" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C82" t="s">
         <v>39</v>
       </c>
       <c r="D82" t="s">
+        <v>537</v>
+      </c>
+      <c r="E82" t="s">
+        <v>83</v>
+      </c>
+      <c r="F82" t="s">
         <v>538</v>
-      </c>
-      <c r="E82" t="s">
-        <v>41</v>
-      </c>
-      <c r="F82" t="s">
-        <v>532</v>
       </c>
       <c r="G82" t="s">
         <v>19</v>
@@ -5843,124 +5863,124 @@
         <v>542</v>
       </c>
       <c r="M82" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N82"/>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>20243776</v>
+        <v>20243773</v>
       </c>
       <c r="B83" t="s">
         <v>543</v>
       </c>
       <c r="C83" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D83" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="E83" t="s">
         <v>41</v>
       </c>
       <c r="F83" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="G83" t="s">
         <v>19</v>
       </c>
       <c r="H83" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I83" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="J83" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="K83" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="L83" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="M83" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N83"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>20243609</v>
+        <v>20243776</v>
       </c>
       <c r="B84" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C84" t="s">
         <v>15</v>
       </c>
       <c r="D84" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="E84" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="F84" t="s">
+        <v>538</v>
+      </c>
+      <c r="G84" t="s">
+        <v>19</v>
+      </c>
+      <c r="H84" t="s">
         <v>550</v>
       </c>
-      <c r="G84" t="s">
-        <v>19</v>
-      </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>551</v>
       </c>
-      <c r="I84" t="s">
+      <c r="J84" t="s">
+        <v>52</v>
+      </c>
+      <c r="K84" t="s">
         <v>552</v>
       </c>
-      <c r="J84" t="s">
+      <c r="L84" t="s">
         <v>553</v>
       </c>
-      <c r="K84" t="s">
-        <v>554</v>
-      </c>
-      <c r="L84" t="s">
-        <v>555</v>
-      </c>
       <c r="M84" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N84"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>20243574</v>
+        <v>20243609</v>
       </c>
       <c r="B85" t="s">
+        <v>554</v>
+      </c>
+      <c r="C85" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85" t="s">
+        <v>555</v>
+      </c>
+      <c r="E85" t="s">
+        <v>17</v>
+      </c>
+      <c r="F85" t="s">
         <v>556</v>
       </c>
-      <c r="C85" t="s">
-        <v>39</v>
-      </c>
-      <c r="D85" t="s">
-        <v>240</v>
-      </c>
-      <c r="E85" t="s">
-        <v>214</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="G85" t="s">
+        <v>19</v>
+      </c>
+      <c r="H85" t="s">
         <v>557</v>
       </c>
-      <c r="G85" t="s">
-        <v>31</v>
-      </c>
-      <c r="H85" t="s">
+      <c r="I85" t="s">
         <v>558</v>
       </c>
-      <c r="I85" t="s">
+      <c r="J85" t="s">
         <v>559</v>
-      </c>
-      <c r="J85" t="s">
-        <v>52</v>
       </c>
       <c r="K85" t="s">
         <v>560</v>
@@ -5969,13 +5989,13 @@
         <v>561</v>
       </c>
       <c r="M85" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N85"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>20243557</v>
+        <v>20243574</v>
       </c>
       <c r="B86" t="s">
         <v>562</v>
@@ -5984,151 +6004,153 @@
         <v>39</v>
       </c>
       <c r="D86" t="s">
+        <v>248</v>
+      </c>
+      <c r="E86" t="s">
+        <v>222</v>
+      </c>
+      <c r="F86" t="s">
         <v>563</v>
       </c>
-      <c r="E86" t="s">
-        <v>214</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="G86" t="s">
+        <v>31</v>
+      </c>
+      <c r="H86" t="s">
         <v>564</v>
       </c>
-      <c r="G86" t="s">
-        <v>19</v>
-      </c>
-      <c r="H86" t="s">
+      <c r="I86" t="s">
         <v>565</v>
-      </c>
-      <c r="I86" t="s">
-        <v>566</v>
       </c>
       <c r="J86" t="s">
         <v>52</v>
       </c>
       <c r="K86" t="s">
+        <v>566</v>
+      </c>
+      <c r="L86" t="s">
         <v>567</v>
       </c>
-      <c r="L86" t="s">
-        <v>568</v>
-      </c>
       <c r="M86" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N86"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>20243471</v>
+        <v>20243557</v>
       </c>
       <c r="B87" t="s">
+        <v>568</v>
+      </c>
+      <c r="C87" t="s">
+        <v>39</v>
+      </c>
+      <c r="D87" t="s">
         <v>569</v>
       </c>
-      <c r="C87" t="s">
-        <v>15</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
+        <v>222</v>
+      </c>
+      <c r="F87" t="s">
         <v>570</v>
       </c>
-      <c r="E87"/>
-      <c r="F87" t="s">
+      <c r="G87" t="s">
+        <v>19</v>
+      </c>
+      <c r="H87" t="s">
         <v>571</v>
       </c>
-      <c r="G87" t="s">
-        <v>19</v>
-      </c>
-      <c r="H87" t="s">
+      <c r="I87" t="s">
         <v>572</v>
-      </c>
-      <c r="I87" t="s">
-        <v>573</v>
       </c>
       <c r="J87" t="s">
         <v>52</v>
       </c>
       <c r="K87" t="s">
+        <v>573</v>
+      </c>
+      <c r="L87" t="s">
         <v>574</v>
       </c>
-      <c r="L87" t="s">
-        <v>575</v>
-      </c>
       <c r="M87" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N87"/>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>20243468</v>
+        <v>20243471</v>
       </c>
       <c r="B88" t="s">
+        <v>575</v>
+      </c>
+      <c r="C88" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88" t="s">
         <v>576</v>
-      </c>
-      <c r="C88" t="s">
-        <v>71</v>
-      </c>
-      <c r="D88" t="s">
-        <v>577</v>
       </c>
       <c r="E88"/>
       <c r="F88" t="s">
+        <v>577</v>
+      </c>
+      <c r="G88" t="s">
+        <v>19</v>
+      </c>
+      <c r="H88" t="s">
         <v>578</v>
       </c>
-      <c r="G88" t="s">
-        <v>19</v>
-      </c>
-      <c r="H88" t="s">
+      <c r="I88" t="s">
         <v>579</v>
       </c>
-      <c r="I88" t="s">
+      <c r="J88" t="s">
+        <v>52</v>
+      </c>
+      <c r="K88" t="s">
         <v>580</v>
       </c>
-      <c r="J88" t="s">
-        <v>187</v>
-      </c>
-      <c r="K88" t="s">
+      <c r="L88" t="s">
         <v>581</v>
       </c>
-      <c r="L88" t="s">
-        <v>582</v>
-      </c>
       <c r="M88" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N88"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>20243467</v>
+        <v>20243468</v>
       </c>
       <c r="B89" t="s">
+        <v>582</v>
+      </c>
+      <c r="C89" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" t="s">
         <v>583</v>
-      </c>
-      <c r="C89" t="s">
-        <v>15</v>
-      </c>
-      <c r="D89" t="s">
-        <v>584</v>
       </c>
       <c r="E89"/>
       <c r="F89" t="s">
+        <v>584</v>
+      </c>
+      <c r="G89" t="s">
+        <v>19</v>
+      </c>
+      <c r="H89" t="s">
         <v>585</v>
       </c>
-      <c r="G89" t="s">
-        <v>31</v>
-      </c>
-      <c r="H89" t="s">
+      <c r="I89" t="s">
         <v>586</v>
       </c>
-      <c r="I89" t="s">
+      <c r="J89" t="s">
+        <v>195</v>
+      </c>
+      <c r="K89" t="s">
         <v>587</v>
       </c>
-      <c r="J89" t="s">
-        <v>52</v>
-      </c>
-      <c r="K89" t="s">
+      <c r="L89" t="s">
         <v>588</v>
-      </c>
-      <c r="L89" t="s">
-        <v>589</v>
       </c>
       <c r="M89" t="s">
         <v>55</v>
@@ -6137,61 +6159,59 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>20243318</v>
+        <v>20243467</v>
       </c>
       <c r="B90" t="s">
+        <v>589</v>
+      </c>
+      <c r="C90" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90" t="s">
         <v>590</v>
       </c>
-      <c r="C90" t="s">
-        <v>39</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="E90"/>
+      <c r="F90" t="s">
         <v>591</v>
       </c>
-      <c r="E90" t="s">
-        <v>41</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="G90" t="s">
+        <v>31</v>
+      </c>
+      <c r="H90" t="s">
         <v>592</v>
       </c>
-      <c r="G90" t="s">
-        <v>19</v>
-      </c>
-      <c r="H90" t="s">
+      <c r="I90" t="s">
         <v>593</v>
       </c>
-      <c r="I90" t="s">
+      <c r="J90" t="s">
+        <v>52</v>
+      </c>
+      <c r="K90" t="s">
         <v>594</v>
       </c>
-      <c r="J90" t="s">
-        <v>22</v>
-      </c>
-      <c r="K90" t="s">
+      <c r="L90" t="s">
         <v>595</v>
       </c>
-      <c r="L90" t="s">
-        <v>596</v>
-      </c>
       <c r="M90" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N90"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>20243234</v>
+        <v>20243318</v>
       </c>
       <c r="B91" t="s">
+        <v>596</v>
+      </c>
+      <c r="C91" t="s">
+        <v>39</v>
+      </c>
+      <c r="D91" t="s">
         <v>597</v>
       </c>
-      <c r="C91" t="s">
-        <v>15</v>
-      </c>
-      <c r="D91" t="s">
-        <v>299</v>
-      </c>
       <c r="E91" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="F91" t="s">
         <v>598</v>
@@ -6206,7 +6226,7 @@
         <v>600</v>
       </c>
       <c r="J91" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="K91" t="s">
         <v>601</v>
@@ -6215,28 +6235,28 @@
         <v>602</v>
       </c>
       <c r="M91" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N91"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>20243259</v>
+        <v>20243234</v>
       </c>
       <c r="B92" t="s">
         <v>603</v>
       </c>
       <c r="C92" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D92" t="s">
+        <v>307</v>
+      </c>
+      <c r="E92" t="s">
+        <v>17</v>
+      </c>
+      <c r="F92" t="s">
         <v>604</v>
-      </c>
-      <c r="E92" t="s">
-        <v>73</v>
-      </c>
-      <c r="F92" t="s">
-        <v>598</v>
       </c>
       <c r="G92" t="s">
         <v>19</v>
@@ -6263,40 +6283,40 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>20243169</v>
+        <v>20243259</v>
       </c>
       <c r="B93" t="s">
         <v>609</v>
       </c>
       <c r="C93" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D93" t="s">
         <v>610</v>
       </c>
       <c r="E93" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="F93" t="s">
+        <v>604</v>
+      </c>
+      <c r="G93" t="s">
+        <v>19</v>
+      </c>
+      <c r="H93" t="s">
         <v>611</v>
       </c>
-      <c r="G93" t="s">
-        <v>19</v>
-      </c>
-      <c r="H93" t="s">
+      <c r="I93" t="s">
         <v>612</v>
-      </c>
-      <c r="I93" t="s">
-        <v>613</v>
       </c>
       <c r="J93" t="s">
         <v>52</v>
       </c>
       <c r="K93" t="s">
+        <v>613</v>
+      </c>
+      <c r="L93" t="s">
         <v>614</v>
-      </c>
-      <c r="L93" t="s">
-        <v>615</v>
       </c>
       <c r="M93" t="s">
         <v>55</v>
@@ -6305,61 +6325,61 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>20247112</v>
+        <v>20243169</v>
       </c>
       <c r="B94" t="s">
+        <v>615</v>
+      </c>
+      <c r="C94" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94" t="s">
         <v>616</v>
       </c>
-      <c r="C94" t="s">
-        <v>47</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
+        <v>17</v>
+      </c>
+      <c r="F94" t="s">
         <v>617</v>
       </c>
-      <c r="E94" t="s">
-        <v>58</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="G94" t="s">
+        <v>19</v>
+      </c>
+      <c r="H94" t="s">
         <v>618</v>
       </c>
-      <c r="G94" t="s">
-        <v>19</v>
-      </c>
-      <c r="H94" t="s">
+      <c r="I94" t="s">
         <v>619</v>
-      </c>
-      <c r="I94" t="s">
-        <v>620</v>
       </c>
       <c r="J94" t="s">
         <v>52</v>
       </c>
       <c r="K94" t="s">
+        <v>620</v>
+      </c>
+      <c r="L94" t="s">
         <v>621</v>
       </c>
-      <c r="L94" t="s">
-        <v>622</v>
-      </c>
       <c r="M94" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N94"/>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>20247015</v>
+        <v>20247112</v>
       </c>
       <c r="B95" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C95" t="s">
         <v>47</v>
       </c>
       <c r="D95" t="s">
-        <v>267</v>
+        <v>623</v>
       </c>
       <c r="E95" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F95" t="s">
         <v>624</v>
@@ -6383,25 +6403,25 @@
         <v>628</v>
       </c>
       <c r="M95" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="N95"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>20234494</v>
+        <v>20247015</v>
       </c>
       <c r="B96" t="s">
         <v>629</v>
       </c>
       <c r="C96" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D96" t="s">
-        <v>140</v>
+        <v>275</v>
       </c>
       <c r="E96" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="F96" t="s">
         <v>630</v>
@@ -6431,7 +6451,7 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>20234461</v>
+        <v>20234494</v>
       </c>
       <c r="B97" t="s">
         <v>635</v>
@@ -6440,7 +6460,7 @@
         <v>39</v>
       </c>
       <c r="D97" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="E97" t="s">
         <v>58</v>
@@ -6467,13 +6487,13 @@
         <v>640</v>
       </c>
       <c r="M97" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N97"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>20234375</v>
+        <v>20234461</v>
       </c>
       <c r="B98" t="s">
         <v>641</v>
@@ -6482,118 +6502,160 @@
         <v>39</v>
       </c>
       <c r="D98" t="s">
+        <v>108</v>
+      </c>
+      <c r="E98" t="s">
+        <v>58</v>
+      </c>
+      <c r="F98" t="s">
         <v>642</v>
       </c>
-      <c r="E98" t="s">
-        <v>17</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="G98" t="s">
+        <v>19</v>
+      </c>
+      <c r="H98" t="s">
         <v>643</v>
       </c>
-      <c r="G98" t="s">
-        <v>19</v>
-      </c>
-      <c r="H98" t="s">
+      <c r="I98" t="s">
         <v>644</v>
-      </c>
-      <c r="I98" t="s">
-        <v>645</v>
       </c>
       <c r="J98" t="s">
         <v>52</v>
       </c>
       <c r="K98" t="s">
+        <v>645</v>
+      </c>
+      <c r="L98" t="s">
         <v>646</v>
       </c>
-      <c r="L98" t="s">
-        <v>647</v>
-      </c>
       <c r="M98" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="N98"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>20234353</v>
+        <v>20234375</v>
       </c>
       <c r="B99" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C99" t="s">
         <v>39</v>
       </c>
       <c r="D99" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E99" t="s">
         <v>17</v>
       </c>
       <c r="F99" t="s">
+        <v>649</v>
+      </c>
+      <c r="G99" t="s">
+        <v>19</v>
+      </c>
+      <c r="H99" t="s">
         <v>650</v>
       </c>
-      <c r="G99" t="s">
-        <v>19</v>
-      </c>
-      <c r="H99" t="s">
+      <c r="I99" t="s">
         <v>651</v>
-      </c>
-      <c r="I99" t="s">
-        <v>652</v>
       </c>
       <c r="J99" t="s">
         <v>52</v>
       </c>
       <c r="K99" t="s">
+        <v>652</v>
+      </c>
+      <c r="L99" t="s">
         <v>653</v>
       </c>
-      <c r="L99" t="s">
-        <v>654</v>
-      </c>
       <c r="M99" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="N99"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>20234346</v>
+        <v>20234353</v>
       </c>
       <c r="B100" t="s">
+        <v>654</v>
+      </c>
+      <c r="C100" t="s">
+        <v>39</v>
+      </c>
+      <c r="D100" t="s">
         <v>655</v>
       </c>
-      <c r="C100" t="s">
-        <v>15</v>
-      </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
+        <v>17</v>
+      </c>
+      <c r="F100" t="s">
         <v>656</v>
       </c>
-      <c r="E100"/>
-      <c r="F100" t="s">
+      <c r="G100" t="s">
+        <v>19</v>
+      </c>
+      <c r="H100" t="s">
         <v>657</v>
       </c>
-      <c r="G100" t="s">
-        <v>31</v>
-      </c>
-      <c r="H100" t="s">
+      <c r="I100" t="s">
         <v>658</v>
-      </c>
-      <c r="I100" t="s">
-        <v>659</v>
       </c>
       <c r="J100" t="s">
         <v>52</v>
       </c>
       <c r="K100" t="s">
+        <v>659</v>
+      </c>
+      <c r="L100" t="s">
         <v>660</v>
       </c>
-      <c r="L100" t="s">
+      <c r="M100" t="s">
+        <v>55</v>
+      </c>
+      <c r="N100"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>20234346</v>
+      </c>
+      <c r="B101" t="s">
         <v>661</v>
       </c>
-      <c r="M100" t="s">
+      <c r="C101" t="s">
+        <v>15</v>
+      </c>
+      <c r="D101" t="s">
+        <v>662</v>
+      </c>
+      <c r="E101"/>
+      <c r="F101" t="s">
+        <v>663</v>
+      </c>
+      <c r="G101" t="s">
+        <v>31</v>
+      </c>
+      <c r="H101" t="s">
+        <v>664</v>
+      </c>
+      <c r="I101" t="s">
+        <v>665</v>
+      </c>
+      <c r="J101" t="s">
+        <v>52</v>
+      </c>
+      <c r="K101" t="s">
+        <v>666</v>
+      </c>
+      <c r="L101" t="s">
+        <v>667</v>
+      </c>
+      <c r="M101" t="s">
         <v>37</v>
       </c>
-      <c r="N100"/>
+      <c r="N101"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update parliament data - 2026-02-25
</commit_message>
<xml_diff>
--- a/Objets_parlementaires_CDF_EFK.xlsx
+++ b/Objets_parlementaires_CDF_EFK.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="3621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3610" uniqueCount="3610">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -6237,7 +6237,7 @@
     <t xml:space="preserve">&lt;p&gt;Le Conseil fédéral a révisé le 1er novembre 2023 l’ordonnance sur les émoluments perçus par l’autorité fédérale de surveillance des fondations (OEmol-ASF), dont la nouvelle mouture entrera en vigueur le 1er janvier 2024. L’élément central de ce texte est une nouvelle augmentation des émoluments, qui aura des conséquences financières massives pour les fondations concernées. Ce qui m’amène à poser les questions suivantes :&amp;nbsp;&lt;br&gt;- Pourquoi n’est-il pas possible de passer d’un contrôle annuel de comptes annuels déjà révisés à un rythme pluriannuel assorti de contrôles approfondis en cas de suspicion, ce qui permettrait de réduire les dépenses de l’Autorité fédérale de surveillance des fondations (ASF) et par voie de conséquence la charge administrative et financière des fondations ?&lt;br&gt;- Le Conseil fédéral serait-il prêt à réserver un traitement à part aux fondations d’utilité publique dont le total du bilan est faible (&lt; 5 millions de CHF) et à prévoir pour elles une catégorie d’émoluments distincte et plus avantageuse assortie d’un rythme de révision plus lent (par ex. tous les 3 à 5 ans) ?&lt;/p&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Der Bundesrat hat am 01.11.2023 die Verordnung über die Gebühren der Eidgenössischen Stiftungsaufsicht (GebV-ESA) revidiert. Die neue Verordnung tritt auf den 01.01.2024 in Kraft. Der Kernpunkt der neuen Verordnung ist eine erneute Gebührenerhöhung – mit massiven finanziellen Auswirkungen für die betroffenen Stiftungen. Hierzu stellen sich folgende Fragen:&amp;nbsp;&lt;br&gt;- Warum kann der Aufwand der ESA und damit der finanzielle und administrative Aufwand der Stiftungen nicht reduziert werden, indem von einer alljährlichen Überprüfung bereits revidierter Jahresabschlüsse auf einen Mehrjahresrhythmus gewechselt wird und auf vertiefte Prüfungen in Verdachtsfällen?&lt;br&gt;- Wäre der Bundesrat bereit, gemeinnützigen Stiftungen mit geringer Bilanzsumme (&amp;lt; 5 Mio. CHF) differenziert zu behandeln und eine separate und günstigere Gebührenkategorie mit einem längeren Revisionsrhythmus einzuführen (z.B. alle 3 – 5 Jahre)?&lt;/p&gt;</t>
+    <t xml:space="preserve">&lt;p&gt;Der Bundesrat hat am 01.11.2023 die Verordnung über die Gebühren der Eidgenössischen Stiftungsaufsicht (GebV-ESA) revidiert. Die neue Verordnung tritt auf den 01.01.2024 in Kraft. Der Kernpunkt der neuen Verordnung ist eine erneute Gebührenerhöhung – mit massiven finanziellen Auswirkungen für die betroffenen Stiftungen. Hierzu stellen sich folgende Fragen:&amp;nbsp;&lt;br&gt;- Warum kann der Aufwand der ESA und damit der finanzielle und administrative Aufwand der Stiftungen nicht reduziert werden, indem von einer alljährlichen Überprüfung bereits revidierter Jahresabschlüsse auf einen Mehrjahresrhythmus gewechselt wird und auf vertiefte Prüfungen in Verdachtsfällen?&lt;br&gt;- Wäre der Bundesrat bereit, gemeinnützigen Stiftungen mit geringer Bilanzsumme (&lt; 5 Mio. CHF) differenziert zu behandeln und eine separate und günstigere Gebührenkategorie mit einem längeren Revisionsrhythmus einzuführen (z.B. alle 3 – 5 Jahre)?&lt;/p&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.parlament.ch/de/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20234353</t>
@@ -10110,9 +10110,6 @@
     <t xml:space="preserve">&lt;p&gt;Der Bundesrat wird beauftragt, die rechtlichen Grundlagen zu erlassen, damit baldmöglichst&amp;nbsp; qualitätsgesicherte, aktuelle und insbesondere international anschlussfähige und vergleichbare strukturierte Daten der Bundesverwaltung zur Mehrfachnutzung (unter anderem durch KI) für Forschung, Planung und Steuerung zur Verfügung gestellt werden.&amp;nbsp;Diesbezügliche verbindliche Standards für die Bundesverwaltung sind zu erlassen.&amp;nbsp;Der Bundesrat wird zudem beauftragt, eine prioritäre Auswahl jener Verwaltungsdaten zu definieren, die für eine zügige und KI-taugliche Mehrfachnutzung zuerst harmonisiert, standardisiert und technisch zugänglich gemacht werden sollen.&amp;nbsp;Insbesondere die öffentliche Bereitstellung weiterer Registerdaten ist zu prüfen. Gezielte Pilotversuche nach Art. 15 EMBAG können dies beschleunigen und sind vom Bundesrat mit den benötigten Mitteln zu beantragen.&lt;/p&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Eingereicht / Déposé</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.parlament.ch/de/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254620</t>
   </si>
   <si>
@@ -10846,36 +10843,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20253941</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bestand des Bundespersonals auf dem Stand von 2015 einfrieren. Bericht des Bundesrates zur Abschreibung der Motion 15.3494 (FK-SR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geler les effectifs de la Confédération au niveau de 2015. Rapport du Conseil fédéral sur le classement de la motion 15.3494 (CdF-CE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bloccare l'effettivo del personale della Confederazione al livello del 2015. Rapporto del Consiglio federale concernente lo stralcio della mozione 15.3494 (CdF-CS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.parlament.ch/de/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20180032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20180032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Staatspolitik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Politique d'Etat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Politica nazionale</t>
   </si>
 </sst>
 </file>
@@ -10923,8 +10890,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:V329" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:V329"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:V328" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:V328"/>
   <tableColumns count="22">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Numéro"/>
@@ -31051,27 +31018,29 @@
         <v>3364</v>
       </c>
       <c r="N303" t="s">
+        <v>1342</v>
+      </c>
+      <c r="O303" t="s">
         <v>3365</v>
       </c>
-      <c r="O303" t="s">
+      <c r="P303" t="s">
         <v>3366</v>
-      </c>
-      <c r="P303" t="s">
-        <v>3367</v>
       </c>
       <c r="Q303" t="s">
         <v>72</v>
       </c>
       <c r="R303"/>
-      <c r="S303"/>
+      <c r="S303" t="s">
+        <v>38</v>
+      </c>
       <c r="T303" t="s">
+        <v>3367</v>
+      </c>
+      <c r="U303" t="s">
         <v>3368</v>
       </c>
-      <c r="U303" t="s">
+      <c r="V303" t="s">
         <v>3369</v>
-      </c>
-      <c r="V303" t="s">
-        <v>3370</v>
       </c>
     </row>
     <row r="304">
@@ -31079,7 +31048,7 @@
         <v>20254696</v>
       </c>
       <c r="B304" t="s">
-        <v>3371</v>
+        <v>3370</v>
       </c>
       <c r="C304" t="s">
         <v>61</v>
@@ -31100,28 +31069,28 @@
         <v>536</v>
       </c>
       <c r="I304" t="s">
+        <v>3371</v>
+      </c>
+      <c r="J304" t="s">
         <v>3372</v>
       </c>
-      <c r="J304" t="s">
+      <c r="K304" t="s">
         <v>3373</v>
       </c>
-      <c r="K304" t="s">
+      <c r="L304" t="s">
         <v>3374</v>
       </c>
-      <c r="L304" t="s">
+      <c r="M304" t="s">
         <v>3375</v>
-      </c>
-      <c r="M304" t="s">
-        <v>3376</v>
       </c>
       <c r="N304" t="s">
         <v>1342</v>
       </c>
       <c r="O304" t="s">
+        <v>3376</v>
+      </c>
+      <c r="P304" t="s">
         <v>3377</v>
-      </c>
-      <c r="P304" t="s">
-        <v>3378</v>
       </c>
       <c r="Q304" t="s">
         <v>55</v>
@@ -31143,7 +31112,7 @@
         <v>20254562</v>
       </c>
       <c r="B305" t="s">
-        <v>3379</v>
+        <v>3378</v>
       </c>
       <c r="C305" t="s">
         <v>205</v>
@@ -31155,7 +31124,7 @@
         <v>45</v>
       </c>
       <c r="F305" t="s">
-        <v>3380</v>
+        <v>3379</v>
       </c>
       <c r="G305" t="s">
         <v>27</v>
@@ -31164,28 +31133,28 @@
         <v>80</v>
       </c>
       <c r="I305" t="s">
+        <v>3380</v>
+      </c>
+      <c r="J305" t="s">
         <v>3381</v>
       </c>
-      <c r="J305" t="s">
+      <c r="K305" t="s">
         <v>3382</v>
       </c>
-      <c r="K305" t="s">
+      <c r="L305" t="s">
         <v>3383</v>
       </c>
-      <c r="L305" t="s">
+      <c r="M305" t="s">
         <v>3384</v>
-      </c>
-      <c r="M305" t="s">
-        <v>3385</v>
       </c>
       <c r="N305" t="s">
         <v>1342</v>
       </c>
       <c r="O305" t="s">
+        <v>3385</v>
+      </c>
+      <c r="P305" t="s">
         <v>3386</v>
-      </c>
-      <c r="P305" t="s">
-        <v>3387</v>
       </c>
       <c r="Q305" t="s">
         <v>37</v>
@@ -31193,13 +31162,13 @@
       <c r="R305"/>
       <c r="S305"/>
       <c r="T305" t="s">
+        <v>3387</v>
+      </c>
+      <c r="U305" t="s">
         <v>3388</v>
       </c>
-      <c r="U305" t="s">
+      <c r="V305" t="s">
         <v>3389</v>
-      </c>
-      <c r="V305" t="s">
-        <v>3390</v>
       </c>
     </row>
     <row r="306">
@@ -31207,19 +31176,19 @@
         <v>20254594</v>
       </c>
       <c r="B306" t="s">
-        <v>3391</v>
+        <v>3390</v>
       </c>
       <c r="C306" t="s">
         <v>61</v>
       </c>
       <c r="D306" t="s">
-        <v>3392</v>
+        <v>3391</v>
       </c>
       <c r="E306" t="s">
         <v>45</v>
       </c>
       <c r="F306" t="s">
-        <v>3380</v>
+        <v>3379</v>
       </c>
       <c r="G306" t="s">
         <v>47</v>
@@ -31228,28 +31197,28 @@
         <v>64</v>
       </c>
       <c r="I306" t="s">
+        <v>3392</v>
+      </c>
+      <c r="J306" t="s">
         <v>3393</v>
       </c>
-      <c r="J306" t="s">
+      <c r="K306" t="s">
         <v>3394</v>
       </c>
-      <c r="K306" t="s">
+      <c r="L306" t="s">
         <v>3395</v>
       </c>
-      <c r="L306" t="s">
+      <c r="M306" t="s">
         <v>3396</v>
-      </c>
-      <c r="M306" t="s">
-        <v>3397</v>
       </c>
       <c r="N306" t="s">
         <v>1342</v>
       </c>
       <c r="O306" t="s">
+        <v>3397</v>
+      </c>
+      <c r="P306" t="s">
         <v>3398</v>
-      </c>
-      <c r="P306" t="s">
-        <v>3399</v>
       </c>
       <c r="Q306" t="s">
         <v>37</v>
@@ -31257,13 +31226,13 @@
       <c r="R306"/>
       <c r="S306"/>
       <c r="T306" t="s">
+        <v>3399</v>
+      </c>
+      <c r="U306" t="s">
         <v>3400</v>
       </c>
-      <c r="U306" t="s">
+      <c r="V306" t="s">
         <v>3401</v>
-      </c>
-      <c r="V306" t="s">
-        <v>3402</v>
       </c>
     </row>
     <row r="307">
@@ -31271,7 +31240,7 @@
         <v>20254614</v>
       </c>
       <c r="B307" t="s">
-        <v>3403</v>
+        <v>3402</v>
       </c>
       <c r="C307" t="s">
         <v>61</v>
@@ -31283,7 +31252,7 @@
         <v>132</v>
       </c>
       <c r="F307" t="s">
-        <v>3380</v>
+        <v>3379</v>
       </c>
       <c r="G307" t="s">
         <v>27</v>
@@ -31292,28 +31261,28 @@
         <v>64</v>
       </c>
       <c r="I307" t="s">
+        <v>3403</v>
+      </c>
+      <c r="J307" t="s">
         <v>3404</v>
       </c>
-      <c r="J307" t="s">
+      <c r="K307" t="s">
         <v>3405</v>
       </c>
-      <c r="K307" t="s">
+      <c r="L307" t="s">
         <v>3406</v>
       </c>
-      <c r="L307" t="s">
+      <c r="M307" t="s">
         <v>3407</v>
-      </c>
-      <c r="M307" t="s">
-        <v>3408</v>
       </c>
       <c r="N307" t="s">
         <v>1342</v>
       </c>
       <c r="O307" t="s">
+        <v>3408</v>
+      </c>
+      <c r="P307" t="s">
         <v>3409</v>
-      </c>
-      <c r="P307" t="s">
-        <v>3410</v>
       </c>
       <c r="Q307" t="s">
         <v>37</v>
@@ -31335,19 +31304,19 @@
         <v>20258194</v>
       </c>
       <c r="B308" t="s">
-        <v>3411</v>
+        <v>3410</v>
       </c>
       <c r="C308" t="s">
         <v>23</v>
       </c>
       <c r="D308" t="s">
-        <v>3412</v>
+        <v>3411</v>
       </c>
       <c r="E308" t="s">
         <v>25</v>
       </c>
       <c r="F308" t="s">
-        <v>3413</v>
+        <v>3412</v>
       </c>
       <c r="G308" t="s">
         <v>27</v>
@@ -31356,26 +31325,26 @@
         <v>64</v>
       </c>
       <c r="I308" t="s">
+        <v>3413</v>
+      </c>
+      <c r="J308" t="s">
         <v>3414</v>
-      </c>
-      <c r="J308" t="s">
-        <v>3415</v>
       </c>
       <c r="K308"/>
       <c r="L308" t="s">
+        <v>3415</v>
+      </c>
+      <c r="M308" t="s">
         <v>3416</v>
-      </c>
-      <c r="M308" t="s">
-        <v>3417</v>
       </c>
       <c r="N308" t="s">
         <v>34</v>
       </c>
       <c r="O308" t="s">
+        <v>3417</v>
+      </c>
+      <c r="P308" t="s">
         <v>3418</v>
-      </c>
-      <c r="P308" t="s">
-        <v>3419</v>
       </c>
       <c r="Q308" t="s">
         <v>37</v>
@@ -31397,7 +31366,7 @@
         <v>20258273</v>
       </c>
       <c r="B309" t="s">
-        <v>3420</v>
+        <v>3419</v>
       </c>
       <c r="C309" t="s">
         <v>23</v>
@@ -31409,7 +31378,7 @@
         <v>633</v>
       </c>
       <c r="F309" t="s">
-        <v>3413</v>
+        <v>3412</v>
       </c>
       <c r="G309" t="s">
         <v>27</v>
@@ -31418,26 +31387,26 @@
         <v>64</v>
       </c>
       <c r="I309" t="s">
+        <v>3420</v>
+      </c>
+      <c r="J309" t="s">
         <v>3421</v>
-      </c>
-      <c r="J309" t="s">
-        <v>3422</v>
       </c>
       <c r="K309"/>
       <c r="L309" t="s">
+        <v>3422</v>
+      </c>
+      <c r="M309" t="s">
         <v>3423</v>
-      </c>
-      <c r="M309" t="s">
-        <v>3424</v>
       </c>
       <c r="N309" t="s">
         <v>34</v>
       </c>
       <c r="O309" t="s">
+        <v>3424</v>
+      </c>
+      <c r="P309" t="s">
         <v>3425</v>
-      </c>
-      <c r="P309" t="s">
-        <v>3426</v>
       </c>
       <c r="Q309" t="s">
         <v>55</v>
@@ -31445,13 +31414,13 @@
       <c r="R309"/>
       <c r="S309"/>
       <c r="T309" t="s">
+        <v>3426</v>
+      </c>
+      <c r="U309" t="s">
         <v>3427</v>
       </c>
-      <c r="U309" t="s">
+      <c r="V309" t="s">
         <v>3428</v>
-      </c>
-      <c r="V309" t="s">
-        <v>3429</v>
       </c>
     </row>
     <row r="310">
@@ -31459,7 +31428,7 @@
         <v>20254463</v>
       </c>
       <c r="B310" t="s">
-        <v>3430</v>
+        <v>3429</v>
       </c>
       <c r="C310" t="s">
         <v>43</v>
@@ -31471,7 +31440,7 @@
         <v>633</v>
       </c>
       <c r="F310" t="s">
-        <v>3431</v>
+        <v>3430</v>
       </c>
       <c r="G310" t="s">
         <v>27</v>
@@ -31480,28 +31449,28 @@
         <v>28</v>
       </c>
       <c r="I310" t="s">
+        <v>3431</v>
+      </c>
+      <c r="J310" t="s">
         <v>3432</v>
       </c>
-      <c r="J310" t="s">
+      <c r="K310" t="s">
         <v>3433</v>
       </c>
-      <c r="K310" t="s">
+      <c r="L310" t="s">
         <v>3434</v>
       </c>
-      <c r="L310" t="s">
+      <c r="M310" t="s">
         <v>3435</v>
-      </c>
-      <c r="M310" t="s">
-        <v>3436</v>
       </c>
       <c r="N310" t="s">
         <v>34</v>
       </c>
       <c r="O310" t="s">
+        <v>3436</v>
+      </c>
+      <c r="P310" t="s">
         <v>3437</v>
-      </c>
-      <c r="P310" t="s">
-        <v>3438</v>
       </c>
       <c r="Q310" t="s">
         <v>72</v>
@@ -31523,19 +31492,19 @@
         <v>20254281</v>
       </c>
       <c r="B311" t="s">
-        <v>3439</v>
+        <v>3438</v>
       </c>
       <c r="C311" t="s">
         <v>205</v>
       </c>
       <c r="D311" t="s">
-        <v>3440</v>
+        <v>3439</v>
       </c>
       <c r="E311" t="s">
         <v>132</v>
       </c>
       <c r="F311" t="s">
-        <v>3441</v>
+        <v>3440</v>
       </c>
       <c r="G311" t="s">
         <v>27</v>
@@ -31544,28 +31513,28 @@
         <v>536</v>
       </c>
       <c r="I311" t="s">
+        <v>3441</v>
+      </c>
+      <c r="J311" t="s">
         <v>3442</v>
       </c>
-      <c r="J311" t="s">
+      <c r="K311" t="s">
         <v>3443</v>
       </c>
-      <c r="K311" t="s">
+      <c r="L311" t="s">
         <v>3444</v>
       </c>
-      <c r="L311" t="s">
+      <c r="M311" t="s">
         <v>3445</v>
-      </c>
-      <c r="M311" t="s">
-        <v>3446</v>
       </c>
       <c r="N311" t="s">
         <v>1342</v>
       </c>
       <c r="O311" t="s">
+        <v>3446</v>
+      </c>
+      <c r="P311" t="s">
         <v>3447</v>
-      </c>
-      <c r="P311" t="s">
-        <v>3448</v>
       </c>
       <c r="Q311" t="s">
         <v>55</v>
@@ -31587,7 +31556,7 @@
         <v>20254317</v>
       </c>
       <c r="B312" t="s">
-        <v>3449</v>
+        <v>3448</v>
       </c>
       <c r="C312" t="s">
         <v>43</v>
@@ -31599,7 +31568,7 @@
         <v>93</v>
       </c>
       <c r="F312" t="s">
-        <v>3441</v>
+        <v>3440</v>
       </c>
       <c r="G312" t="s">
         <v>27</v>
@@ -31608,28 +31577,28 @@
         <v>536</v>
       </c>
       <c r="I312" t="s">
+        <v>3449</v>
+      </c>
+      <c r="J312" t="s">
         <v>3450</v>
       </c>
-      <c r="J312" t="s">
+      <c r="K312" t="s">
         <v>3451</v>
       </c>
-      <c r="K312" t="s">
+      <c r="L312" t="s">
         <v>3452</v>
       </c>
-      <c r="L312" t="s">
+      <c r="M312" t="s">
         <v>3453</v>
-      </c>
-      <c r="M312" t="s">
-        <v>3454</v>
       </c>
       <c r="N312" t="s">
         <v>1342</v>
       </c>
       <c r="O312" t="s">
+        <v>3454</v>
+      </c>
+      <c r="P312" t="s">
         <v>3455</v>
-      </c>
-      <c r="P312" t="s">
-        <v>3456</v>
       </c>
       <c r="Q312" t="s">
         <v>55</v>
@@ -31637,13 +31606,13 @@
       <c r="R312"/>
       <c r="S312"/>
       <c r="T312" t="s">
+        <v>3456</v>
+      </c>
+      <c r="U312" t="s">
         <v>3457</v>
       </c>
-      <c r="U312" t="s">
+      <c r="V312" t="s">
         <v>3458</v>
-      </c>
-      <c r="V312" t="s">
-        <v>3459</v>
       </c>
     </row>
     <row r="313">
@@ -31651,19 +31620,19 @@
         <v>20254145</v>
       </c>
       <c r="B313" t="s">
-        <v>3460</v>
+        <v>3459</v>
       </c>
       <c r="C313" t="s">
         <v>43</v>
       </c>
       <c r="D313" t="s">
-        <v>3461</v>
+        <v>3460</v>
       </c>
       <c r="E313" t="s">
         <v>93</v>
       </c>
       <c r="F313" t="s">
-        <v>3462</v>
+        <v>3461</v>
       </c>
       <c r="G313" t="s">
         <v>47</v>
@@ -31672,28 +31641,28 @@
         <v>28</v>
       </c>
       <c r="I313" t="s">
+        <v>3462</v>
+      </c>
+      <c r="J313" t="s">
         <v>3463</v>
       </c>
-      <c r="J313" t="s">
+      <c r="K313" t="s">
         <v>3464</v>
       </c>
-      <c r="K313" t="s">
+      <c r="L313" t="s">
         <v>3465</v>
       </c>
-      <c r="L313" t="s">
+      <c r="M313" t="s">
         <v>3466</v>
-      </c>
-      <c r="M313" t="s">
-        <v>3467</v>
       </c>
       <c r="N313" t="s">
         <v>34</v>
       </c>
       <c r="O313" t="s">
+        <v>3467</v>
+      </c>
+      <c r="P313" t="s">
         <v>3468</v>
-      </c>
-      <c r="P313" t="s">
-        <v>3469</v>
       </c>
       <c r="Q313" t="s">
         <v>37</v>
@@ -31715,19 +31684,19 @@
         <v>20254188</v>
       </c>
       <c r="B314" t="s">
-        <v>3470</v>
+        <v>3469</v>
       </c>
       <c r="C314" t="s">
         <v>43</v>
       </c>
       <c r="D314" t="s">
-        <v>3471</v>
+        <v>3470</v>
       </c>
       <c r="E314" t="s">
         <v>93</v>
       </c>
       <c r="F314" t="s">
-        <v>3462</v>
+        <v>3461</v>
       </c>
       <c r="G314" t="s">
         <v>47</v>
@@ -31736,28 +31705,28 @@
         <v>64</v>
       </c>
       <c r="I314" t="s">
+        <v>3471</v>
+      </c>
+      <c r="J314" t="s">
         <v>3472</v>
       </c>
-      <c r="J314" t="s">
+      <c r="K314" t="s">
         <v>3473</v>
       </c>
-      <c r="K314" t="s">
+      <c r="L314" t="s">
         <v>3474</v>
       </c>
-      <c r="L314" t="s">
+      <c r="M314" t="s">
         <v>3475</v>
       </c>
-      <c r="M314" t="s">
+      <c r="N314" t="s">
         <v>3476</v>
       </c>
-      <c r="N314" t="s">
+      <c r="O314" t="s">
         <v>3477</v>
       </c>
-      <c r="O314" t="s">
+      <c r="P314" t="s">
         <v>3478</v>
-      </c>
-      <c r="P314" t="s">
-        <v>3479</v>
       </c>
       <c r="Q314" t="s">
         <v>37</v>
@@ -31779,7 +31748,7 @@
         <v>20254225</v>
       </c>
       <c r="B315" t="s">
-        <v>3480</v>
+        <v>3479</v>
       </c>
       <c r="C315" t="s">
         <v>61</v>
@@ -31791,7 +31760,7 @@
         <v>633</v>
       </c>
       <c r="F315" t="s">
-        <v>3462</v>
+        <v>3461</v>
       </c>
       <c r="G315" t="s">
         <v>27</v>
@@ -31800,28 +31769,28 @@
         <v>64</v>
       </c>
       <c r="I315" t="s">
+        <v>3480</v>
+      </c>
+      <c r="J315" t="s">
         <v>3481</v>
       </c>
-      <c r="J315" t="s">
+      <c r="K315" t="s">
         <v>3482</v>
       </c>
-      <c r="K315" t="s">
+      <c r="L315" t="s">
         <v>3483</v>
       </c>
-      <c r="L315" t="s">
+      <c r="M315" t="s">
         <v>3484</v>
-      </c>
-      <c r="M315" t="s">
-        <v>3485</v>
       </c>
       <c r="N315" t="s">
         <v>1342</v>
       </c>
       <c r="O315" t="s">
+        <v>3485</v>
+      </c>
+      <c r="P315" t="s">
         <v>3486</v>
-      </c>
-      <c r="P315" t="s">
-        <v>3487</v>
       </c>
       <c r="Q315" t="s">
         <v>55</v>
@@ -31829,13 +31798,13 @@
       <c r="R315"/>
       <c r="S315"/>
       <c r="T315" t="s">
+        <v>3487</v>
+      </c>
+      <c r="U315" t="s">
         <v>3488</v>
       </c>
-      <c r="U315" t="s">
+      <c r="V315" t="s">
         <v>3489</v>
-      </c>
-      <c r="V315" t="s">
-        <v>3490</v>
       </c>
     </row>
     <row r="316">
@@ -31843,19 +31812,19 @@
         <v>20254234</v>
       </c>
       <c r="B316" t="s">
-        <v>3491</v>
+        <v>3490</v>
       </c>
       <c r="C316" t="s">
         <v>43</v>
       </c>
       <c r="D316" t="s">
-        <v>3492</v>
+        <v>3491</v>
       </c>
       <c r="E316" t="s">
         <v>132</v>
       </c>
       <c r="F316" t="s">
-        <v>3462</v>
+        <v>3461</v>
       </c>
       <c r="G316" t="s">
         <v>27</v>
@@ -31864,28 +31833,28 @@
         <v>64</v>
       </c>
       <c r="I316" t="s">
+        <v>3492</v>
+      </c>
+      <c r="J316" t="s">
         <v>3493</v>
       </c>
-      <c r="J316" t="s">
+      <c r="K316" t="s">
         <v>3494</v>
       </c>
-      <c r="K316" t="s">
+      <c r="L316" t="s">
         <v>3495</v>
       </c>
-      <c r="L316" t="s">
+      <c r="M316" t="s">
         <v>3496</v>
-      </c>
-      <c r="M316" t="s">
-        <v>3497</v>
       </c>
       <c r="N316" t="s">
         <v>34</v>
       </c>
       <c r="O316" t="s">
+        <v>3497</v>
+      </c>
+      <c r="P316" t="s">
         <v>3498</v>
-      </c>
-      <c r="P316" t="s">
-        <v>3499</v>
       </c>
       <c r="Q316" t="s">
         <v>72</v>
@@ -31893,13 +31862,13 @@
       <c r="R316"/>
       <c r="S316"/>
       <c r="T316" t="s">
+        <v>3499</v>
+      </c>
+      <c r="U316" t="s">
         <v>3500</v>
       </c>
-      <c r="U316" t="s">
+      <c r="V316" t="s">
         <v>3501</v>
-      </c>
-      <c r="V316" t="s">
-        <v>3502</v>
       </c>
     </row>
     <row r="317">
@@ -31907,19 +31876,19 @@
         <v>20254071</v>
       </c>
       <c r="B317" t="s">
-        <v>3503</v>
+        <v>3502</v>
       </c>
       <c r="C317" t="s">
         <v>61</v>
       </c>
       <c r="D317" t="s">
-        <v>3504</v>
+        <v>3503</v>
       </c>
       <c r="E317" t="s">
         <v>93</v>
       </c>
       <c r="F317" t="s">
-        <v>3505</v>
+        <v>3504</v>
       </c>
       <c r="G317" t="s">
         <v>47</v>
@@ -31928,28 +31897,28 @@
         <v>64</v>
       </c>
       <c r="I317" t="s">
+        <v>3505</v>
+      </c>
+      <c r="J317" t="s">
         <v>3506</v>
       </c>
-      <c r="J317" t="s">
+      <c r="K317" t="s">
         <v>3507</v>
       </c>
-      <c r="K317" t="s">
+      <c r="L317" t="s">
         <v>3508</v>
       </c>
-      <c r="L317" t="s">
+      <c r="M317" t="s">
         <v>3509</v>
-      </c>
-      <c r="M317" t="s">
-        <v>3510</v>
       </c>
       <c r="N317" t="s">
         <v>34</v>
       </c>
       <c r="O317" t="s">
+        <v>3510</v>
+      </c>
+      <c r="P317" t="s">
         <v>3511</v>
-      </c>
-      <c r="P317" t="s">
-        <v>3512</v>
       </c>
       <c r="Q317" t="s">
         <v>37</v>
@@ -31957,13 +31926,13 @@
       <c r="R317"/>
       <c r="S317"/>
       <c r="T317" t="s">
+        <v>3512</v>
+      </c>
+      <c r="U317" t="s">
         <v>3513</v>
       </c>
-      <c r="U317" t="s">
+      <c r="V317" t="s">
         <v>3514</v>
-      </c>
-      <c r="V317" t="s">
-        <v>3515</v>
       </c>
     </row>
     <row r="318">
@@ -31971,7 +31940,7 @@
         <v>20254024</v>
       </c>
       <c r="B318" t="s">
-        <v>3516</v>
+        <v>3515</v>
       </c>
       <c r="C318" t="s">
         <v>61</v>
@@ -31983,7 +31952,7 @@
         <v>132</v>
       </c>
       <c r="F318" t="s">
-        <v>3517</v>
+        <v>3516</v>
       </c>
       <c r="G318" t="s">
         <v>27</v>
@@ -31992,28 +31961,28 @@
         <v>119</v>
       </c>
       <c r="I318" t="s">
+        <v>3517</v>
+      </c>
+      <c r="J318" t="s">
         <v>3518</v>
       </c>
-      <c r="J318" t="s">
+      <c r="K318" t="s">
         <v>3519</v>
       </c>
-      <c r="K318" t="s">
+      <c r="L318" t="s">
         <v>3520</v>
       </c>
-      <c r="L318" t="s">
+      <c r="M318" t="s">
         <v>3521</v>
-      </c>
-      <c r="M318" t="s">
-        <v>3522</v>
       </c>
       <c r="N318" t="s">
         <v>1342</v>
       </c>
       <c r="O318" t="s">
+        <v>3522</v>
+      </c>
+      <c r="P318" t="s">
         <v>3523</v>
-      </c>
-      <c r="P318" t="s">
-        <v>3524</v>
       </c>
       <c r="Q318" t="s">
         <v>55</v>
@@ -32035,7 +32004,7 @@
         <v>20257863</v>
       </c>
       <c r="B319" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="C319" t="s">
         <v>23</v>
@@ -32047,7 +32016,7 @@
         <v>1826</v>
       </c>
       <c r="F319" t="s">
-        <v>3517</v>
+        <v>3516</v>
       </c>
       <c r="G319" t="s">
         <v>27</v>
@@ -32056,26 +32025,26 @@
         <v>28</v>
       </c>
       <c r="I319" t="s">
+        <v>3525</v>
+      </c>
+      <c r="J319" t="s">
         <v>3526</v>
-      </c>
-      <c r="J319" t="s">
-        <v>3527</v>
       </c>
       <c r="K319"/>
       <c r="L319" t="s">
+        <v>3527</v>
+      </c>
+      <c r="M319" t="s">
         <v>3528</v>
-      </c>
-      <c r="M319" t="s">
-        <v>3529</v>
       </c>
       <c r="N319" t="s">
         <v>34</v>
       </c>
       <c r="O319" t="s">
+        <v>3529</v>
+      </c>
+      <c r="P319" t="s">
         <v>3530</v>
-      </c>
-      <c r="P319" t="s">
-        <v>3531</v>
       </c>
       <c r="Q319" t="s">
         <v>37</v>
@@ -32097,7 +32066,7 @@
         <v>20257888</v>
       </c>
       <c r="B320" t="s">
-        <v>3532</v>
+        <v>3531</v>
       </c>
       <c r="C320" t="s">
         <v>23</v>
@@ -32109,7 +32078,7 @@
         <v>1473</v>
       </c>
       <c r="F320" t="s">
-        <v>3517</v>
+        <v>3516</v>
       </c>
       <c r="G320" t="s">
         <v>27</v>
@@ -32118,26 +32087,26 @@
         <v>119</v>
       </c>
       <c r="I320" t="s">
+        <v>3532</v>
+      </c>
+      <c r="J320" t="s">
         <v>3533</v>
-      </c>
-      <c r="J320" t="s">
-        <v>3534</v>
       </c>
       <c r="K320"/>
       <c r="L320" t="s">
+        <v>3534</v>
+      </c>
+      <c r="M320" t="s">
         <v>3535</v>
-      </c>
-      <c r="M320" t="s">
-        <v>3536</v>
       </c>
       <c r="N320" t="s">
         <v>34</v>
       </c>
       <c r="O320" t="s">
+        <v>3536</v>
+      </c>
+      <c r="P320" t="s">
         <v>3537</v>
-      </c>
-      <c r="P320" t="s">
-        <v>3538</v>
       </c>
       <c r="Q320" t="s">
         <v>72</v>
@@ -32159,7 +32128,7 @@
         <v>20257890</v>
       </c>
       <c r="B321" t="s">
-        <v>3539</v>
+        <v>3538</v>
       </c>
       <c r="C321" t="s">
         <v>23</v>
@@ -32171,7 +32140,7 @@
         <v>633</v>
       </c>
       <c r="F321" t="s">
-        <v>3517</v>
+        <v>3516</v>
       </c>
       <c r="G321" t="s">
         <v>27</v>
@@ -32180,26 +32149,26 @@
         <v>536</v>
       </c>
       <c r="I321" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J321" t="s">
         <v>3540</v>
-      </c>
-      <c r="J321" t="s">
-        <v>3541</v>
       </c>
       <c r="K321"/>
       <c r="L321" t="s">
+        <v>3541</v>
+      </c>
+      <c r="M321" t="s">
         <v>3542</v>
-      </c>
-      <c r="M321" t="s">
-        <v>3543</v>
       </c>
       <c r="N321" t="s">
         <v>34</v>
       </c>
       <c r="O321" t="s">
+        <v>3543</v>
+      </c>
+      <c r="P321" t="s">
         <v>3544</v>
-      </c>
-      <c r="P321" t="s">
-        <v>3545</v>
       </c>
       <c r="Q321" t="s">
         <v>55</v>
@@ -32221,17 +32190,17 @@
         <v>20254003</v>
       </c>
       <c r="B322" t="s">
-        <v>3546</v>
+        <v>3545</v>
       </c>
       <c r="C322" t="s">
         <v>205</v>
       </c>
       <c r="D322" t="s">
-        <v>3547</v>
+        <v>3546</v>
       </c>
       <c r="E322"/>
       <c r="F322" t="s">
-        <v>3548</v>
+        <v>3547</v>
       </c>
       <c r="G322" t="s">
         <v>27</v>
@@ -32240,28 +32209,28 @@
         <v>28</v>
       </c>
       <c r="I322" t="s">
+        <v>3548</v>
+      </c>
+      <c r="J322" t="s">
         <v>3549</v>
       </c>
-      <c r="J322" t="s">
+      <c r="K322" t="s">
         <v>3550</v>
       </c>
-      <c r="K322" t="s">
+      <c r="L322" t="s">
         <v>3551</v>
       </c>
-      <c r="L322" t="s">
+      <c r="M322" t="s">
         <v>3552</v>
-      </c>
-      <c r="M322" t="s">
-        <v>3553</v>
       </c>
       <c r="N322" t="s">
         <v>1342</v>
       </c>
       <c r="O322" t="s">
+        <v>3553</v>
+      </c>
+      <c r="P322" t="s">
         <v>3554</v>
-      </c>
-      <c r="P322" t="s">
-        <v>3555</v>
       </c>
       <c r="Q322" t="s">
         <v>37</v>
@@ -32269,13 +32238,13 @@
       <c r="R322"/>
       <c r="S322"/>
       <c r="T322" t="s">
+        <v>3555</v>
+      </c>
+      <c r="U322" t="s">
         <v>3556</v>
       </c>
-      <c r="U322" t="s">
+      <c r="V322" t="s">
         <v>3557</v>
-      </c>
-      <c r="V322" t="s">
-        <v>3558</v>
       </c>
     </row>
     <row r="323">
@@ -32283,7 +32252,7 @@
         <v>20253984</v>
       </c>
       <c r="B323" t="s">
-        <v>3559</v>
+        <v>3558</v>
       </c>
       <c r="C323" t="s">
         <v>43</v>
@@ -32293,7 +32262,7 @@
       </c>
       <c r="E323"/>
       <c r="F323" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="G323" t="s">
         <v>27</v>
@@ -32302,28 +32271,28 @@
         <v>28</v>
       </c>
       <c r="I323" t="s">
+        <v>3462</v>
+      </c>
+      <c r="J323" t="s">
         <v>3463</v>
       </c>
-      <c r="J323" t="s">
+      <c r="K323" t="s">
         <v>3464</v>
       </c>
-      <c r="K323" t="s">
-        <v>3465</v>
-      </c>
       <c r="L323" t="s">
+        <v>3560</v>
+      </c>
+      <c r="M323" t="s">
         <v>3561</v>
-      </c>
-      <c r="M323" t="s">
-        <v>3562</v>
       </c>
       <c r="N323" t="s">
         <v>1329</v>
       </c>
       <c r="O323" t="s">
+        <v>3562</v>
+      </c>
+      <c r="P323" t="s">
         <v>3563</v>
-      </c>
-      <c r="P323" t="s">
-        <v>3564</v>
       </c>
       <c r="Q323" t="s">
         <v>37</v>
@@ -32345,7 +32314,7 @@
         <v>20257663</v>
       </c>
       <c r="B324" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="C324" t="s">
         <v>23</v>
@@ -32357,7 +32326,7 @@
         <v>25</v>
       </c>
       <c r="F324" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="G324" t="s">
         <v>27</v>
@@ -32366,26 +32335,26 @@
         <v>119</v>
       </c>
       <c r="I324" t="s">
+        <v>3565</v>
+      </c>
+      <c r="J324" t="s">
         <v>3566</v>
-      </c>
-      <c r="J324" t="s">
-        <v>3567</v>
       </c>
       <c r="K324"/>
       <c r="L324" t="s">
+        <v>3567</v>
+      </c>
+      <c r="M324" t="s">
         <v>3568</v>
-      </c>
-      <c r="M324" t="s">
-        <v>3569</v>
       </c>
       <c r="N324" t="s">
         <v>34</v>
       </c>
       <c r="O324" t="s">
+        <v>3569</v>
+      </c>
+      <c r="P324" t="s">
         <v>3570</v>
-      </c>
-      <c r="P324" t="s">
-        <v>3571</v>
       </c>
       <c r="Q324" t="s">
         <v>37</v>
@@ -32393,13 +32362,13 @@
       <c r="R324"/>
       <c r="S324"/>
       <c r="T324" t="s">
+        <v>3571</v>
+      </c>
+      <c r="U324" t="s">
         <v>3572</v>
       </c>
-      <c r="U324" t="s">
+      <c r="V324" t="s">
         <v>3573</v>
-      </c>
-      <c r="V324" t="s">
-        <v>3574</v>
       </c>
     </row>
     <row r="325">
@@ -32407,19 +32376,19 @@
         <v>20257698</v>
       </c>
       <c r="B325" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="C325" t="s">
         <v>23</v>
       </c>
       <c r="D325" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
       <c r="E325" t="s">
         <v>132</v>
       </c>
       <c r="F325" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="G325" t="s">
         <v>27</v>
@@ -32428,26 +32397,26 @@
         <v>119</v>
       </c>
       <c r="I325" t="s">
+        <v>3576</v>
+      </c>
+      <c r="J325" t="s">
         <v>3577</v>
-      </c>
-      <c r="J325" t="s">
-        <v>3578</v>
       </c>
       <c r="K325"/>
       <c r="L325" t="s">
+        <v>3578</v>
+      </c>
+      <c r="M325" t="s">
         <v>3579</v>
-      </c>
-      <c r="M325" t="s">
-        <v>3580</v>
       </c>
       <c r="N325" t="s">
         <v>34</v>
       </c>
       <c r="O325" t="s">
+        <v>3580</v>
+      </c>
+      <c r="P325" t="s">
         <v>3581</v>
-      </c>
-      <c r="P325" t="s">
-        <v>3582</v>
       </c>
       <c r="Q325" t="s">
         <v>37</v>
@@ -32469,19 +32438,19 @@
         <v>20253971</v>
       </c>
       <c r="B326" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="C326" t="s">
         <v>61</v>
       </c>
       <c r="D326" t="s">
-        <v>3584</v>
+        <v>3583</v>
       </c>
       <c r="E326" t="s">
         <v>93</v>
       </c>
       <c r="F326" t="s">
-        <v>3585</v>
+        <v>3584</v>
       </c>
       <c r="G326" t="s">
         <v>47</v>
@@ -32490,28 +32459,28 @@
         <v>536</v>
       </c>
       <c r="I326" t="s">
+        <v>3585</v>
+      </c>
+      <c r="J326" t="s">
         <v>3586</v>
       </c>
-      <c r="J326" t="s">
+      <c r="K326" t="s">
         <v>3587</v>
       </c>
-      <c r="K326" t="s">
+      <c r="L326" t="s">
         <v>3588</v>
       </c>
-      <c r="L326" t="s">
+      <c r="M326" t="s">
         <v>3589</v>
-      </c>
-      <c r="M326" t="s">
-        <v>3590</v>
       </c>
       <c r="N326" t="s">
         <v>34</v>
       </c>
       <c r="O326" t="s">
+        <v>3590</v>
+      </c>
+      <c r="P326" t="s">
         <v>3591</v>
-      </c>
-      <c r="P326" t="s">
-        <v>3592</v>
       </c>
       <c r="Q326" t="s">
         <v>55</v>
@@ -32519,13 +32488,13 @@
       <c r="R326"/>
       <c r="S326"/>
       <c r="T326" t="s">
+        <v>3456</v>
+      </c>
+      <c r="U326" t="s">
         <v>3457</v>
       </c>
-      <c r="U326" t="s">
+      <c r="V326" t="s">
         <v>3458</v>
-      </c>
-      <c r="V326" t="s">
-        <v>3459</v>
       </c>
     </row>
     <row r="327">
@@ -32533,7 +32502,7 @@
         <v>20257601</v>
       </c>
       <c r="B327" t="s">
-        <v>3593</v>
+        <v>3592</v>
       </c>
       <c r="C327" t="s">
         <v>23</v>
@@ -32545,7 +32514,7 @@
         <v>1473</v>
       </c>
       <c r="F327" t="s">
-        <v>3594</v>
+        <v>3593</v>
       </c>
       <c r="G327" t="s">
         <v>27</v>
@@ -32554,26 +32523,26 @@
         <v>64</v>
       </c>
       <c r="I327" t="s">
+        <v>3594</v>
+      </c>
+      <c r="J327" t="s">
         <v>3595</v>
-      </c>
-      <c r="J327" t="s">
-        <v>3596</v>
       </c>
       <c r="K327"/>
       <c r="L327" t="s">
+        <v>3596</v>
+      </c>
+      <c r="M327" t="s">
         <v>3597</v>
-      </c>
-      <c r="M327" t="s">
-        <v>3598</v>
       </c>
       <c r="N327" t="s">
         <v>34</v>
       </c>
       <c r="O327" t="s">
+        <v>3598</v>
+      </c>
+      <c r="P327" t="s">
         <v>3599</v>
-      </c>
-      <c r="P327" t="s">
-        <v>3600</v>
       </c>
       <c r="Q327" t="s">
         <v>55</v>
@@ -32595,17 +32564,17 @@
         <v>20253941</v>
       </c>
       <c r="B328" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="C328" t="s">
         <v>43</v>
       </c>
       <c r="D328" t="s">
-        <v>3602</v>
+        <v>3601</v>
       </c>
       <c r="E328"/>
       <c r="F328" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
       <c r="G328" t="s">
         <v>27</v>
@@ -32614,28 +32583,28 @@
         <v>1533</v>
       </c>
       <c r="I328" t="s">
+        <v>3603</v>
+      </c>
+      <c r="J328" t="s">
         <v>3604</v>
       </c>
-      <c r="J328" t="s">
+      <c r="K328" t="s">
         <v>3605</v>
       </c>
-      <c r="K328" t="s">
+      <c r="L328" t="s">
         <v>3606</v>
       </c>
-      <c r="L328" t="s">
+      <c r="M328" t="s">
         <v>3607</v>
-      </c>
-      <c r="M328" t="s">
-        <v>3608</v>
       </c>
       <c r="N328" t="s">
         <v>1965</v>
       </c>
       <c r="O328" t="s">
+        <v>3608</v>
+      </c>
+      <c r="P328" t="s">
         <v>3609</v>
-      </c>
-      <c r="P328" t="s">
-        <v>3610</v>
       </c>
       <c r="Q328" t="s">
         <v>37</v>
@@ -32645,60 +32614,6 @@
       <c r="T328"/>
       <c r="U328"/>
       <c r="V328"/>
-    </row>
-    <row r="329">
-      <c r="A329" t="n">
-        <v>20180032</v>
-      </c>
-      <c r="B329" t="s">
-        <v>3611</v>
-      </c>
-      <c r="C329" t="s">
-        <v>3612</v>
-      </c>
-      <c r="D329"/>
-      <c r="E329"/>
-      <c r="F329" t="s">
-        <v>673</v>
-      </c>
-      <c r="G329"/>
-      <c r="H329" t="s">
-        <v>28</v>
-      </c>
-      <c r="I329" t="s">
-        <v>3613</v>
-      </c>
-      <c r="J329" t="s">
-        <v>3614</v>
-      </c>
-      <c r="K329" t="s">
-        <v>3615</v>
-      </c>
-      <c r="L329"/>
-      <c r="M329"/>
-      <c r="N329" t="s">
-        <v>34</v>
-      </c>
-      <c r="O329" t="s">
-        <v>3616</v>
-      </c>
-      <c r="P329" t="s">
-        <v>3617</v>
-      </c>
-      <c r="Q329" t="s">
-        <v>975</v>
-      </c>
-      <c r="R329"/>
-      <c r="S329"/>
-      <c r="T329" t="s">
-        <v>3618</v>
-      </c>
-      <c r="U329" t="s">
-        <v>3619</v>
-      </c>
-      <c r="V329" t="s">
-        <v>3620</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update parliament data - 2026-02-27
</commit_message>
<xml_diff>
--- a/Objets_parlementaires_CDF_EFK.xlsx
+++ b/Objets_parlementaires_CDF_EFK.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3619" uniqueCount="3619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="3621">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -10140,10 +10140,16 @@
     <t xml:space="preserve">&lt;p&gt;Der Bundesrat wird beauftragt, die rechtlichen Grundlagen zu erlassen, damit baldmöglichst&amp;nbsp; qualitätsgesicherte, aktuelle und insbesondere international anschlussfähige und vergleichbare strukturierte Daten der Bundesverwaltung zur Mehrfachnutzung (unter anderem durch KI) für Forschung, Planung und Steuerung zur Verfügung gestellt werden.&amp;nbsp;Diesbezügliche verbindliche Standards für die Bundesverwaltung sind zu erlassen.&amp;nbsp;Der Bundesrat wird zudem beauftragt, eine prioritäre Auswahl jener Verwaltungsdaten zu definieren, die für eine zügige und KI-taugliche Mehrfachnutzung zuerst harmonisiert, standardisiert und technisch zugänglich gemacht werden sollen.&amp;nbsp;Insbesondere die öffentliche Bereitstellung weiterer Registerdaten ist zu prüfen. Gezielte Pilotversuche nach Art. 15 EMBAG können dies beschleunigen und sind vom Bundesrat mit den benötigten Mitteln zu beantragen.&lt;/p&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">In Ständerat geplant / Planifié au Conseil des Etats</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.parlament.ch/de/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254620</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.parlament.ch/fr/ratsbetrieb/suche-curia-vista/geschaeft?AffairId=20254620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2026-02-27</t>
   </si>
   <si>
     <t xml:space="preserve">Staatspolitik|Medien und Kommunikation|Menschenrechte</t>
@@ -31111,27 +31117,29 @@
         <v>3374</v>
       </c>
       <c r="N304" t="s">
-        <v>34</v>
+        <v>3375</v>
       </c>
       <c r="O304" t="s">
-        <v>3375</v>
+        <v>3376</v>
       </c>
       <c r="P304" t="s">
-        <v>3376</v>
+        <v>3377</v>
       </c>
       <c r="Q304" t="s">
         <v>89</v>
       </c>
       <c r="R304"/>
-      <c r="S304"/>
+      <c r="S304" t="s">
+        <v>3378</v>
+      </c>
       <c r="T304" t="s">
-        <v>3377</v>
+        <v>3379</v>
       </c>
       <c r="U304" t="s">
-        <v>3378</v>
+        <v>3380</v>
       </c>
       <c r="V304" t="s">
-        <v>3379</v>
+        <v>3381</v>
       </c>
     </row>
     <row r="305">
@@ -31139,7 +31147,7 @@
         <v>20254696</v>
       </c>
       <c r="B305" t="s">
-        <v>3380</v>
+        <v>3382</v>
       </c>
       <c r="C305" t="s">
         <v>23</v>
@@ -31160,28 +31168,28 @@
         <v>548</v>
       </c>
       <c r="I305" t="s">
-        <v>3381</v>
+        <v>3383</v>
       </c>
       <c r="J305" t="s">
-        <v>3382</v>
+        <v>3384</v>
       </c>
       <c r="K305" t="s">
-        <v>3383</v>
+        <v>3385</v>
       </c>
       <c r="L305" t="s">
-        <v>3384</v>
+        <v>3386</v>
       </c>
       <c r="M305" t="s">
-        <v>3385</v>
+        <v>3387</v>
       </c>
       <c r="N305" t="s">
         <v>34</v>
       </c>
       <c r="O305" t="s">
-        <v>3386</v>
+        <v>3388</v>
       </c>
       <c r="P305" t="s">
-        <v>3387</v>
+        <v>3389</v>
       </c>
       <c r="Q305" t="s">
         <v>73</v>
@@ -31203,7 +31211,7 @@
         <v>20254562</v>
       </c>
       <c r="B306" t="s">
-        <v>3388</v>
+        <v>3390</v>
       </c>
       <c r="C306" t="s">
         <v>217</v>
@@ -31224,28 +31232,28 @@
         <v>97</v>
       </c>
       <c r="I306" t="s">
-        <v>3389</v>
+        <v>3391</v>
       </c>
       <c r="J306" t="s">
-        <v>3390</v>
+        <v>3392</v>
       </c>
       <c r="K306" t="s">
-        <v>3391</v>
+        <v>3393</v>
       </c>
       <c r="L306" t="s">
-        <v>3392</v>
+        <v>3394</v>
       </c>
       <c r="M306" t="s">
-        <v>3393</v>
+        <v>3395</v>
       </c>
       <c r="N306" t="s">
         <v>34</v>
       </c>
       <c r="O306" t="s">
-        <v>3394</v>
+        <v>3396</v>
       </c>
       <c r="P306" t="s">
-        <v>3395</v>
+        <v>3397</v>
       </c>
       <c r="Q306" t="s">
         <v>37</v>
@@ -31253,13 +31261,13 @@
       <c r="R306"/>
       <c r="S306"/>
       <c r="T306" t="s">
-        <v>3396</v>
+        <v>3398</v>
       </c>
       <c r="U306" t="s">
-        <v>3397</v>
+        <v>3399</v>
       </c>
       <c r="V306" t="s">
-        <v>3398</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="307">
@@ -31267,13 +31275,13 @@
         <v>20254594</v>
       </c>
       <c r="B307" t="s">
-        <v>3399</v>
+        <v>3401</v>
       </c>
       <c r="C307" t="s">
         <v>23</v>
       </c>
       <c r="D307" t="s">
-        <v>3400</v>
+        <v>3402</v>
       </c>
       <c r="E307" t="s">
         <v>63</v>
@@ -31288,42 +31296,44 @@
         <v>81</v>
       </c>
       <c r="I307" t="s">
-        <v>3401</v>
+        <v>3403</v>
       </c>
       <c r="J307" t="s">
-        <v>3402</v>
+        <v>3404</v>
       </c>
       <c r="K307" t="s">
-        <v>3403</v>
+        <v>3405</v>
       </c>
       <c r="L307" t="s">
-        <v>3404</v>
+        <v>3406</v>
       </c>
       <c r="M307" t="s">
-        <v>3405</v>
+        <v>3407</v>
       </c>
       <c r="N307" t="s">
-        <v>34</v>
+        <v>3375</v>
       </c>
       <c r="O307" t="s">
-        <v>3406</v>
+        <v>3408</v>
       </c>
       <c r="P307" t="s">
-        <v>3407</v>
+        <v>3409</v>
       </c>
       <c r="Q307" t="s">
         <v>37</v>
       </c>
       <c r="R307"/>
-      <c r="S307"/>
+      <c r="S307" t="s">
+        <v>3378</v>
+      </c>
       <c r="T307" t="s">
-        <v>3408</v>
+        <v>3410</v>
       </c>
       <c r="U307" t="s">
-        <v>3409</v>
+        <v>3411</v>
       </c>
       <c r="V307" t="s">
-        <v>3410</v>
+        <v>3412</v>
       </c>
     </row>
     <row r="308">
@@ -31331,7 +31341,7 @@
         <v>20254614</v>
       </c>
       <c r="B308" t="s">
-        <v>3411</v>
+        <v>3413</v>
       </c>
       <c r="C308" t="s">
         <v>23</v>
@@ -31352,28 +31362,28 @@
         <v>81</v>
       </c>
       <c r="I308" t="s">
-        <v>3412</v>
+        <v>3414</v>
       </c>
       <c r="J308" t="s">
-        <v>3413</v>
+        <v>3415</v>
       </c>
       <c r="K308" t="s">
-        <v>3414</v>
+        <v>3416</v>
       </c>
       <c r="L308" t="s">
-        <v>3415</v>
+        <v>3417</v>
       </c>
       <c r="M308" t="s">
-        <v>3416</v>
+        <v>3418</v>
       </c>
       <c r="N308" t="s">
         <v>34</v>
       </c>
       <c r="O308" t="s">
-        <v>3417</v>
+        <v>3419</v>
       </c>
       <c r="P308" t="s">
-        <v>3418</v>
+        <v>3420</v>
       </c>
       <c r="Q308" t="s">
         <v>37</v>
@@ -31395,19 +31405,19 @@
         <v>20258194</v>
       </c>
       <c r="B309" t="s">
-        <v>3419</v>
+        <v>3421</v>
       </c>
       <c r="C309" t="s">
         <v>43</v>
       </c>
       <c r="D309" t="s">
-        <v>3420</v>
+        <v>3422</v>
       </c>
       <c r="E309" t="s">
         <v>45</v>
       </c>
       <c r="F309" t="s">
-        <v>3421</v>
+        <v>3423</v>
       </c>
       <c r="G309" t="s">
         <v>27</v>
@@ -31416,26 +31426,26 @@
         <v>81</v>
       </c>
       <c r="I309" t="s">
-        <v>3422</v>
+        <v>3424</v>
       </c>
       <c r="J309" t="s">
-        <v>3423</v>
+        <v>3425</v>
       </c>
       <c r="K309"/>
       <c r="L309" t="s">
-        <v>3424</v>
+        <v>3426</v>
       </c>
       <c r="M309" t="s">
-        <v>3425</v>
+        <v>3427</v>
       </c>
       <c r="N309" t="s">
         <v>53</v>
       </c>
       <c r="O309" t="s">
-        <v>3426</v>
+        <v>3428</v>
       </c>
       <c r="P309" t="s">
-        <v>3427</v>
+        <v>3429</v>
       </c>
       <c r="Q309" t="s">
         <v>37</v>
@@ -31457,7 +31467,7 @@
         <v>20258273</v>
       </c>
       <c r="B310" t="s">
-        <v>3428</v>
+        <v>3430</v>
       </c>
       <c r="C310" t="s">
         <v>43</v>
@@ -31469,7 +31479,7 @@
         <v>645</v>
       </c>
       <c r="F310" t="s">
-        <v>3421</v>
+        <v>3423</v>
       </c>
       <c r="G310" t="s">
         <v>27</v>
@@ -31478,26 +31488,26 @@
         <v>81</v>
       </c>
       <c r="I310" t="s">
-        <v>3429</v>
+        <v>3431</v>
       </c>
       <c r="J310" t="s">
-        <v>3430</v>
+        <v>3432</v>
       </c>
       <c r="K310"/>
       <c r="L310" t="s">
-        <v>3431</v>
+        <v>3433</v>
       </c>
       <c r="M310" t="s">
-        <v>3432</v>
+        <v>3434</v>
       </c>
       <c r="N310" t="s">
         <v>53</v>
       </c>
       <c r="O310" t="s">
-        <v>3433</v>
+        <v>3435</v>
       </c>
       <c r="P310" t="s">
-        <v>3434</v>
+        <v>3436</v>
       </c>
       <c r="Q310" t="s">
         <v>73</v>
@@ -31505,13 +31515,13 @@
       <c r="R310"/>
       <c r="S310"/>
       <c r="T310" t="s">
-        <v>3435</v>
+        <v>3437</v>
       </c>
       <c r="U310" t="s">
-        <v>3436</v>
+        <v>3438</v>
       </c>
       <c r="V310" t="s">
-        <v>3437</v>
+        <v>3439</v>
       </c>
     </row>
     <row r="311">
@@ -31519,7 +31529,7 @@
         <v>20254463</v>
       </c>
       <c r="B311" t="s">
-        <v>3438</v>
+        <v>3440</v>
       </c>
       <c r="C311" t="s">
         <v>61</v>
@@ -31531,7 +31541,7 @@
         <v>645</v>
       </c>
       <c r="F311" t="s">
-        <v>3439</v>
+        <v>3441</v>
       </c>
       <c r="G311" t="s">
         <v>27</v>
@@ -31540,28 +31550,28 @@
         <v>47</v>
       </c>
       <c r="I311" t="s">
-        <v>3440</v>
+        <v>3442</v>
       </c>
       <c r="J311" t="s">
-        <v>3441</v>
+        <v>3443</v>
       </c>
       <c r="K311" t="s">
-        <v>3442</v>
+        <v>3444</v>
       </c>
       <c r="L311" t="s">
-        <v>3443</v>
+        <v>3445</v>
       </c>
       <c r="M311" t="s">
-        <v>3444</v>
+        <v>3446</v>
       </c>
       <c r="N311" t="s">
         <v>53</v>
       </c>
       <c r="O311" t="s">
-        <v>3445</v>
+        <v>3447</v>
       </c>
       <c r="P311" t="s">
-        <v>3446</v>
+        <v>3448</v>
       </c>
       <c r="Q311" t="s">
         <v>89</v>
@@ -31583,19 +31593,19 @@
         <v>20254281</v>
       </c>
       <c r="B312" t="s">
-        <v>3447</v>
+        <v>3449</v>
       </c>
       <c r="C312" t="s">
         <v>217</v>
       </c>
       <c r="D312" t="s">
-        <v>3448</v>
+        <v>3450</v>
       </c>
       <c r="E312" t="s">
         <v>144</v>
       </c>
       <c r="F312" t="s">
-        <v>3449</v>
+        <v>3451</v>
       </c>
       <c r="G312" t="s">
         <v>27</v>
@@ -31604,28 +31614,28 @@
         <v>548</v>
       </c>
       <c r="I312" t="s">
-        <v>3450</v>
+        <v>3452</v>
       </c>
       <c r="J312" t="s">
-        <v>3451</v>
+        <v>3453</v>
       </c>
       <c r="K312" t="s">
-        <v>3452</v>
+        <v>3454</v>
       </c>
       <c r="L312" t="s">
-        <v>3453</v>
+        <v>3455</v>
       </c>
       <c r="M312" t="s">
-        <v>3454</v>
+        <v>3456</v>
       </c>
       <c r="N312" t="s">
         <v>34</v>
       </c>
       <c r="O312" t="s">
-        <v>3455</v>
+        <v>3457</v>
       </c>
       <c r="P312" t="s">
-        <v>3456</v>
+        <v>3458</v>
       </c>
       <c r="Q312" t="s">
         <v>73</v>
@@ -31647,7 +31657,7 @@
         <v>20254317</v>
       </c>
       <c r="B313" t="s">
-        <v>3457</v>
+        <v>3459</v>
       </c>
       <c r="C313" t="s">
         <v>61</v>
@@ -31659,7 +31669,7 @@
         <v>25</v>
       </c>
       <c r="F313" t="s">
-        <v>3449</v>
+        <v>3451</v>
       </c>
       <c r="G313" t="s">
         <v>27</v>
@@ -31668,28 +31678,28 @@
         <v>548</v>
       </c>
       <c r="I313" t="s">
-        <v>3458</v>
+        <v>3460</v>
       </c>
       <c r="J313" t="s">
-        <v>3459</v>
+        <v>3461</v>
       </c>
       <c r="K313" t="s">
-        <v>3460</v>
+        <v>3462</v>
       </c>
       <c r="L313" t="s">
-        <v>3461</v>
+        <v>3463</v>
       </c>
       <c r="M313" t="s">
-        <v>3462</v>
+        <v>3464</v>
       </c>
       <c r="N313" t="s">
         <v>34</v>
       </c>
       <c r="O313" t="s">
-        <v>3463</v>
+        <v>3465</v>
       </c>
       <c r="P313" t="s">
-        <v>3464</v>
+        <v>3466</v>
       </c>
       <c r="Q313" t="s">
         <v>73</v>
@@ -31697,13 +31707,13 @@
       <c r="R313"/>
       <c r="S313"/>
       <c r="T313" t="s">
-        <v>3465</v>
+        <v>3467</v>
       </c>
       <c r="U313" t="s">
-        <v>3466</v>
+        <v>3468</v>
       </c>
       <c r="V313" t="s">
-        <v>3467</v>
+        <v>3469</v>
       </c>
     </row>
     <row r="314">
@@ -31711,19 +31721,19 @@
         <v>20254145</v>
       </c>
       <c r="B314" t="s">
-        <v>3468</v>
+        <v>3470</v>
       </c>
       <c r="C314" t="s">
         <v>61</v>
       </c>
       <c r="D314" t="s">
-        <v>3469</v>
+        <v>3471</v>
       </c>
       <c r="E314" t="s">
         <v>25</v>
       </c>
       <c r="F314" t="s">
-        <v>3470</v>
+        <v>3472</v>
       </c>
       <c r="G314" t="s">
         <v>65</v>
@@ -31732,28 +31742,28 @@
         <v>47</v>
       </c>
       <c r="I314" t="s">
-        <v>3471</v>
+        <v>3473</v>
       </c>
       <c r="J314" t="s">
-        <v>3472</v>
+        <v>3474</v>
       </c>
       <c r="K314" t="s">
-        <v>3473</v>
+        <v>3475</v>
       </c>
       <c r="L314" t="s">
-        <v>3474</v>
+        <v>3476</v>
       </c>
       <c r="M314" t="s">
-        <v>3475</v>
+        <v>3477</v>
       </c>
       <c r="N314" t="s">
         <v>53</v>
       </c>
       <c r="O314" t="s">
-        <v>3476</v>
+        <v>3478</v>
       </c>
       <c r="P314" t="s">
-        <v>3477</v>
+        <v>3479</v>
       </c>
       <c r="Q314" t="s">
         <v>37</v>
@@ -31775,19 +31785,19 @@
         <v>20254188</v>
       </c>
       <c r="B315" t="s">
-        <v>3478</v>
+        <v>3480</v>
       </c>
       <c r="C315" t="s">
         <v>61</v>
       </c>
       <c r="D315" t="s">
-        <v>3479</v>
+        <v>3481</v>
       </c>
       <c r="E315" t="s">
         <v>25</v>
       </c>
       <c r="F315" t="s">
-        <v>3470</v>
+        <v>3472</v>
       </c>
       <c r="G315" t="s">
         <v>65</v>
@@ -31796,28 +31806,28 @@
         <v>81</v>
       </c>
       <c r="I315" t="s">
-        <v>3480</v>
+        <v>3482</v>
       </c>
       <c r="J315" t="s">
-        <v>3481</v>
+        <v>3483</v>
       </c>
       <c r="K315" t="s">
-        <v>3482</v>
+        <v>3484</v>
       </c>
       <c r="L315" t="s">
-        <v>3483</v>
+        <v>3485</v>
       </c>
       <c r="M315" t="s">
-        <v>3484</v>
+        <v>3486</v>
       </c>
       <c r="N315" t="s">
-        <v>3485</v>
+        <v>3487</v>
       </c>
       <c r="O315" t="s">
-        <v>3486</v>
+        <v>3488</v>
       </c>
       <c r="P315" t="s">
-        <v>3487</v>
+        <v>3489</v>
       </c>
       <c r="Q315" t="s">
         <v>37</v>
@@ -31839,7 +31849,7 @@
         <v>20254225</v>
       </c>
       <c r="B316" t="s">
-        <v>3488</v>
+        <v>3490</v>
       </c>
       <c r="C316" t="s">
         <v>23</v>
@@ -31851,7 +31861,7 @@
         <v>645</v>
       </c>
       <c r="F316" t="s">
-        <v>3470</v>
+        <v>3472</v>
       </c>
       <c r="G316" t="s">
         <v>27</v>
@@ -31860,28 +31870,28 @@
         <v>81</v>
       </c>
       <c r="I316" t="s">
-        <v>3489</v>
+        <v>3491</v>
       </c>
       <c r="J316" t="s">
-        <v>3490</v>
+        <v>3492</v>
       </c>
       <c r="K316" t="s">
-        <v>3491</v>
+        <v>3493</v>
       </c>
       <c r="L316" t="s">
-        <v>3492</v>
+        <v>3494</v>
       </c>
       <c r="M316" t="s">
-        <v>3493</v>
+        <v>3495</v>
       </c>
       <c r="N316" t="s">
         <v>34</v>
       </c>
       <c r="O316" t="s">
-        <v>3494</v>
+        <v>3496</v>
       </c>
       <c r="P316" t="s">
-        <v>3495</v>
+        <v>3497</v>
       </c>
       <c r="Q316" t="s">
         <v>73</v>
@@ -31889,13 +31899,13 @@
       <c r="R316"/>
       <c r="S316"/>
       <c r="T316" t="s">
-        <v>3496</v>
+        <v>3498</v>
       </c>
       <c r="U316" t="s">
-        <v>3497</v>
+        <v>3499</v>
       </c>
       <c r="V316" t="s">
-        <v>3498</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="317">
@@ -31903,19 +31913,19 @@
         <v>20254234</v>
       </c>
       <c r="B317" t="s">
-        <v>3499</v>
+        <v>3501</v>
       </c>
       <c r="C317" t="s">
         <v>61</v>
       </c>
       <c r="D317" t="s">
-        <v>3500</v>
+        <v>3502</v>
       </c>
       <c r="E317" t="s">
         <v>144</v>
       </c>
       <c r="F317" t="s">
-        <v>3470</v>
+        <v>3472</v>
       </c>
       <c r="G317" t="s">
         <v>27</v>
@@ -31924,28 +31934,28 @@
         <v>81</v>
       </c>
       <c r="I317" t="s">
-        <v>3501</v>
+        <v>3503</v>
       </c>
       <c r="J317" t="s">
-        <v>3502</v>
+        <v>3504</v>
       </c>
       <c r="K317" t="s">
-        <v>3503</v>
+        <v>3505</v>
       </c>
       <c r="L317" t="s">
-        <v>3504</v>
+        <v>3506</v>
       </c>
       <c r="M317" t="s">
-        <v>3505</v>
+        <v>3507</v>
       </c>
       <c r="N317" t="s">
         <v>53</v>
       </c>
       <c r="O317" t="s">
-        <v>3506</v>
+        <v>3508</v>
       </c>
       <c r="P317" t="s">
-        <v>3507</v>
+        <v>3509</v>
       </c>
       <c r="Q317" t="s">
         <v>89</v>
@@ -31953,13 +31963,13 @@
       <c r="R317"/>
       <c r="S317"/>
       <c r="T317" t="s">
-        <v>3508</v>
+        <v>3510</v>
       </c>
       <c r="U317" t="s">
-        <v>3509</v>
+        <v>3511</v>
       </c>
       <c r="V317" t="s">
-        <v>3510</v>
+        <v>3512</v>
       </c>
     </row>
     <row r="318">
@@ -31967,19 +31977,19 @@
         <v>20254071</v>
       </c>
       <c r="B318" t="s">
-        <v>3511</v>
+        <v>3513</v>
       </c>
       <c r="C318" t="s">
         <v>23</v>
       </c>
       <c r="D318" t="s">
-        <v>3512</v>
+        <v>3514</v>
       </c>
       <c r="E318" t="s">
         <v>25</v>
       </c>
       <c r="F318" t="s">
-        <v>3513</v>
+        <v>3515</v>
       </c>
       <c r="G318" t="s">
         <v>65</v>
@@ -31988,28 +31998,28 @@
         <v>81</v>
       </c>
       <c r="I318" t="s">
-        <v>3514</v>
+        <v>3516</v>
       </c>
       <c r="J318" t="s">
-        <v>3515</v>
+        <v>3517</v>
       </c>
       <c r="K318" t="s">
-        <v>3516</v>
+        <v>3518</v>
       </c>
       <c r="L318" t="s">
-        <v>3517</v>
+        <v>3519</v>
       </c>
       <c r="M318" t="s">
-        <v>3518</v>
+        <v>3520</v>
       </c>
       <c r="N318" t="s">
         <v>53</v>
       </c>
       <c r="O318" t="s">
-        <v>3519</v>
+        <v>3521</v>
       </c>
       <c r="P318" t="s">
-        <v>3520</v>
+        <v>3522</v>
       </c>
       <c r="Q318" t="s">
         <v>37</v>
@@ -32017,13 +32027,13 @@
       <c r="R318"/>
       <c r="S318"/>
       <c r="T318" t="s">
-        <v>3521</v>
+        <v>3523</v>
       </c>
       <c r="U318" t="s">
-        <v>3522</v>
+        <v>3524</v>
       </c>
       <c r="V318" t="s">
-        <v>3523</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="319">
@@ -32031,7 +32041,7 @@
         <v>20254024</v>
       </c>
       <c r="B319" t="s">
-        <v>3524</v>
+        <v>3526</v>
       </c>
       <c r="C319" t="s">
         <v>23</v>
@@ -32043,7 +32053,7 @@
         <v>144</v>
       </c>
       <c r="F319" t="s">
-        <v>3525</v>
+        <v>3527</v>
       </c>
       <c r="G319" t="s">
         <v>27</v>
@@ -32052,28 +32062,28 @@
         <v>28</v>
       </c>
       <c r="I319" t="s">
-        <v>3526</v>
+        <v>3528</v>
       </c>
       <c r="J319" t="s">
-        <v>3527</v>
+        <v>3529</v>
       </c>
       <c r="K319" t="s">
-        <v>3528</v>
+        <v>3530</v>
       </c>
       <c r="L319" t="s">
-        <v>3529</v>
+        <v>3531</v>
       </c>
       <c r="M319" t="s">
-        <v>3530</v>
+        <v>3532</v>
       </c>
       <c r="N319" t="s">
         <v>34</v>
       </c>
       <c r="O319" t="s">
-        <v>3531</v>
+        <v>3533</v>
       </c>
       <c r="P319" t="s">
-        <v>3532</v>
+        <v>3534</v>
       </c>
       <c r="Q319" t="s">
         <v>73</v>
@@ -32095,7 +32105,7 @@
         <v>20257863</v>
       </c>
       <c r="B320" t="s">
-        <v>3533</v>
+        <v>3535</v>
       </c>
       <c r="C320" t="s">
         <v>43</v>
@@ -32107,7 +32117,7 @@
         <v>1836</v>
       </c>
       <c r="F320" t="s">
-        <v>3525</v>
+        <v>3527</v>
       </c>
       <c r="G320" t="s">
         <v>27</v>
@@ -32116,26 +32126,26 @@
         <v>47</v>
       </c>
       <c r="I320" t="s">
-        <v>3534</v>
+        <v>3536</v>
       </c>
       <c r="J320" t="s">
-        <v>3535</v>
+        <v>3537</v>
       </c>
       <c r="K320"/>
       <c r="L320" t="s">
-        <v>3536</v>
+        <v>3538</v>
       </c>
       <c r="M320" t="s">
-        <v>3537</v>
+        <v>3539</v>
       </c>
       <c r="N320" t="s">
         <v>53</v>
       </c>
       <c r="O320" t="s">
-        <v>3538</v>
+        <v>3540</v>
       </c>
       <c r="P320" t="s">
-        <v>3539</v>
+        <v>3541</v>
       </c>
       <c r="Q320" t="s">
         <v>37</v>
@@ -32157,7 +32167,7 @@
         <v>20257888</v>
       </c>
       <c r="B321" t="s">
-        <v>3540</v>
+        <v>3542</v>
       </c>
       <c r="C321" t="s">
         <v>43</v>
@@ -32169,7 +32179,7 @@
         <v>1483</v>
       </c>
       <c r="F321" t="s">
-        <v>3525</v>
+        <v>3527</v>
       </c>
       <c r="G321" t="s">
         <v>27</v>
@@ -32178,26 +32188,26 @@
         <v>28</v>
       </c>
       <c r="I321" t="s">
-        <v>3541</v>
+        <v>3543</v>
       </c>
       <c r="J321" t="s">
-        <v>3542</v>
+        <v>3544</v>
       </c>
       <c r="K321"/>
       <c r="L321" t="s">
-        <v>3543</v>
+        <v>3545</v>
       </c>
       <c r="M321" t="s">
-        <v>3544</v>
+        <v>3546</v>
       </c>
       <c r="N321" t="s">
         <v>53</v>
       </c>
       <c r="O321" t="s">
-        <v>3545</v>
+        <v>3547</v>
       </c>
       <c r="P321" t="s">
-        <v>3546</v>
+        <v>3548</v>
       </c>
       <c r="Q321" t="s">
         <v>89</v>
@@ -32219,7 +32229,7 @@
         <v>20257890</v>
       </c>
       <c r="B322" t="s">
-        <v>3547</v>
+        <v>3549</v>
       </c>
       <c r="C322" t="s">
         <v>43</v>
@@ -32231,7 +32241,7 @@
         <v>645</v>
       </c>
       <c r="F322" t="s">
-        <v>3525</v>
+        <v>3527</v>
       </c>
       <c r="G322" t="s">
         <v>27</v>
@@ -32240,26 +32250,26 @@
         <v>548</v>
       </c>
       <c r="I322" t="s">
-        <v>3548</v>
+        <v>3550</v>
       </c>
       <c r="J322" t="s">
-        <v>3549</v>
+        <v>3551</v>
       </c>
       <c r="K322"/>
       <c r="L322" t="s">
-        <v>3550</v>
+        <v>3552</v>
       </c>
       <c r="M322" t="s">
-        <v>3551</v>
+        <v>3553</v>
       </c>
       <c r="N322" t="s">
         <v>53</v>
       </c>
       <c r="O322" t="s">
-        <v>3552</v>
+        <v>3554</v>
       </c>
       <c r="P322" t="s">
-        <v>3553</v>
+        <v>3555</v>
       </c>
       <c r="Q322" t="s">
         <v>73</v>
@@ -32281,17 +32291,17 @@
         <v>20254003</v>
       </c>
       <c r="B323" t="s">
-        <v>3554</v>
+        <v>3556</v>
       </c>
       <c r="C323" t="s">
         <v>217</v>
       </c>
       <c r="D323" t="s">
-        <v>3555</v>
+        <v>3557</v>
       </c>
       <c r="E323"/>
       <c r="F323" t="s">
-        <v>3556</v>
+        <v>3558</v>
       </c>
       <c r="G323" t="s">
         <v>27</v>
@@ -32300,28 +32310,28 @@
         <v>47</v>
       </c>
       <c r="I323" t="s">
-        <v>3557</v>
+        <v>3559</v>
       </c>
       <c r="J323" t="s">
-        <v>3558</v>
+        <v>3560</v>
       </c>
       <c r="K323" t="s">
-        <v>3559</v>
+        <v>3561</v>
       </c>
       <c r="L323" t="s">
-        <v>3560</v>
+        <v>3562</v>
       </c>
       <c r="M323" t="s">
-        <v>3561</v>
+        <v>3563</v>
       </c>
       <c r="N323" t="s">
         <v>34</v>
       </c>
       <c r="O323" t="s">
-        <v>3562</v>
+        <v>3564</v>
       </c>
       <c r="P323" t="s">
-        <v>3563</v>
+        <v>3565</v>
       </c>
       <c r="Q323" t="s">
         <v>37</v>
@@ -32329,13 +32339,13 @@
       <c r="R323"/>
       <c r="S323"/>
       <c r="T323" t="s">
-        <v>3564</v>
+        <v>3566</v>
       </c>
       <c r="U323" t="s">
-        <v>3565</v>
+        <v>3567</v>
       </c>
       <c r="V323" t="s">
-        <v>3566</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="324">
@@ -32343,7 +32353,7 @@
         <v>20253984</v>
       </c>
       <c r="B324" t="s">
-        <v>3567</v>
+        <v>3569</v>
       </c>
       <c r="C324" t="s">
         <v>61</v>
@@ -32353,7 +32363,7 @@
       </c>
       <c r="E324"/>
       <c r="F324" t="s">
-        <v>3568</v>
+        <v>3570</v>
       </c>
       <c r="G324" t="s">
         <v>27</v>
@@ -32362,34 +32372,36 @@
         <v>47</v>
       </c>
       <c r="I324" t="s">
-        <v>3471</v>
+        <v>3473</v>
       </c>
       <c r="J324" t="s">
-        <v>3472</v>
+        <v>3474</v>
       </c>
       <c r="K324" t="s">
-        <v>3473</v>
+        <v>3475</v>
       </c>
       <c r="L324" t="s">
-        <v>3569</v>
+        <v>3571</v>
       </c>
       <c r="M324" t="s">
-        <v>3570</v>
+        <v>3572</v>
       </c>
       <c r="N324" t="s">
-        <v>1341</v>
+        <v>3375</v>
       </c>
       <c r="O324" t="s">
-        <v>3571</v>
+        <v>3573</v>
       </c>
       <c r="P324" t="s">
-        <v>3572</v>
+        <v>3574</v>
       </c>
       <c r="Q324" t="s">
         <v>37</v>
       </c>
       <c r="R324"/>
-      <c r="S324"/>
+      <c r="S324" t="s">
+        <v>3378</v>
+      </c>
       <c r="T324" t="s">
         <v>117</v>
       </c>
@@ -32405,7 +32417,7 @@
         <v>20257663</v>
       </c>
       <c r="B325" t="s">
-        <v>3573</v>
+        <v>3575</v>
       </c>
       <c r="C325" t="s">
         <v>43</v>
@@ -32417,7 +32429,7 @@
         <v>45</v>
       </c>
       <c r="F325" t="s">
-        <v>3568</v>
+        <v>3570</v>
       </c>
       <c r="G325" t="s">
         <v>27</v>
@@ -32426,26 +32438,26 @@
         <v>28</v>
       </c>
       <c r="I325" t="s">
-        <v>3574</v>
+        <v>3576</v>
       </c>
       <c r="J325" t="s">
-        <v>3575</v>
+        <v>3577</v>
       </c>
       <c r="K325"/>
       <c r="L325" t="s">
-        <v>3576</v>
+        <v>3578</v>
       </c>
       <c r="M325" t="s">
-        <v>3577</v>
+        <v>3579</v>
       </c>
       <c r="N325" t="s">
         <v>53</v>
       </c>
       <c r="O325" t="s">
-        <v>3578</v>
+        <v>3580</v>
       </c>
       <c r="P325" t="s">
-        <v>3579</v>
+        <v>3581</v>
       </c>
       <c r="Q325" t="s">
         <v>37</v>
@@ -32453,13 +32465,13 @@
       <c r="R325"/>
       <c r="S325"/>
       <c r="T325" t="s">
-        <v>3580</v>
+        <v>3582</v>
       </c>
       <c r="U325" t="s">
-        <v>3581</v>
+        <v>3583</v>
       </c>
       <c r="V325" t="s">
-        <v>3582</v>
+        <v>3584</v>
       </c>
     </row>
     <row r="326">
@@ -32467,19 +32479,19 @@
         <v>20257698</v>
       </c>
       <c r="B326" t="s">
-        <v>3583</v>
+        <v>3585</v>
       </c>
       <c r="C326" t="s">
         <v>43</v>
       </c>
       <c r="D326" t="s">
-        <v>3584</v>
+        <v>3586</v>
       </c>
       <c r="E326" t="s">
         <v>144</v>
       </c>
       <c r="F326" t="s">
-        <v>3568</v>
+        <v>3570</v>
       </c>
       <c r="G326" t="s">
         <v>27</v>
@@ -32488,26 +32500,26 @@
         <v>28</v>
       </c>
       <c r="I326" t="s">
-        <v>3585</v>
+        <v>3587</v>
       </c>
       <c r="J326" t="s">
-        <v>3586</v>
+        <v>3588</v>
       </c>
       <c r="K326"/>
       <c r="L326" t="s">
-        <v>3587</v>
+        <v>3589</v>
       </c>
       <c r="M326" t="s">
-        <v>3588</v>
+        <v>3590</v>
       </c>
       <c r="N326" t="s">
         <v>53</v>
       </c>
       <c r="O326" t="s">
-        <v>3589</v>
+        <v>3591</v>
       </c>
       <c r="P326" t="s">
-        <v>3590</v>
+        <v>3592</v>
       </c>
       <c r="Q326" t="s">
         <v>37</v>
@@ -32529,19 +32541,19 @@
         <v>20253971</v>
       </c>
       <c r="B327" t="s">
-        <v>3591</v>
+        <v>3593</v>
       </c>
       <c r="C327" t="s">
         <v>23</v>
       </c>
       <c r="D327" t="s">
-        <v>3592</v>
+        <v>3594</v>
       </c>
       <c r="E327" t="s">
         <v>25</v>
       </c>
       <c r="F327" t="s">
-        <v>3593</v>
+        <v>3595</v>
       </c>
       <c r="G327" t="s">
         <v>65</v>
@@ -32550,28 +32562,28 @@
         <v>548</v>
       </c>
       <c r="I327" t="s">
-        <v>3594</v>
+        <v>3596</v>
       </c>
       <c r="J327" t="s">
-        <v>3595</v>
+        <v>3597</v>
       </c>
       <c r="K327" t="s">
-        <v>3596</v>
+        <v>3598</v>
       </c>
       <c r="L327" t="s">
-        <v>3597</v>
+        <v>3599</v>
       </c>
       <c r="M327" t="s">
-        <v>3598</v>
+        <v>3600</v>
       </c>
       <c r="N327" t="s">
         <v>53</v>
       </c>
       <c r="O327" t="s">
-        <v>3599</v>
+        <v>3601</v>
       </c>
       <c r="P327" t="s">
-        <v>3600</v>
+        <v>3602</v>
       </c>
       <c r="Q327" t="s">
         <v>73</v>
@@ -32579,13 +32591,13 @@
       <c r="R327"/>
       <c r="S327"/>
       <c r="T327" t="s">
-        <v>3465</v>
+        <v>3467</v>
       </c>
       <c r="U327" t="s">
-        <v>3466</v>
+        <v>3468</v>
       </c>
       <c r="V327" t="s">
-        <v>3467</v>
+        <v>3469</v>
       </c>
     </row>
     <row r="328">
@@ -32593,7 +32605,7 @@
         <v>20257601</v>
       </c>
       <c r="B328" t="s">
-        <v>3601</v>
+        <v>3603</v>
       </c>
       <c r="C328" t="s">
         <v>43</v>
@@ -32605,7 +32617,7 @@
         <v>1483</v>
       </c>
       <c r="F328" t="s">
-        <v>3602</v>
+        <v>3604</v>
       </c>
       <c r="G328" t="s">
         <v>27</v>
@@ -32614,26 +32626,26 @@
         <v>81</v>
       </c>
       <c r="I328" t="s">
-        <v>3603</v>
+        <v>3605</v>
       </c>
       <c r="J328" t="s">
-        <v>3604</v>
+        <v>3606</v>
       </c>
       <c r="K328"/>
       <c r="L328" t="s">
-        <v>3605</v>
+        <v>3607</v>
       </c>
       <c r="M328" t="s">
-        <v>3606</v>
+        <v>3608</v>
       </c>
       <c r="N328" t="s">
         <v>53</v>
       </c>
       <c r="O328" t="s">
-        <v>3607</v>
+        <v>3609</v>
       </c>
       <c r="P328" t="s">
-        <v>3608</v>
+        <v>3610</v>
       </c>
       <c r="Q328" t="s">
         <v>73</v>
@@ -32655,17 +32667,17 @@
         <v>20253941</v>
       </c>
       <c r="B329" t="s">
-        <v>3609</v>
+        <v>3611</v>
       </c>
       <c r="C329" t="s">
         <v>61</v>
       </c>
       <c r="D329" t="s">
-        <v>3610</v>
+        <v>3612</v>
       </c>
       <c r="E329"/>
       <c r="F329" t="s">
-        <v>3611</v>
+        <v>3613</v>
       </c>
       <c r="G329" t="s">
         <v>27</v>
@@ -32674,28 +32686,28 @@
         <v>1543</v>
       </c>
       <c r="I329" t="s">
-        <v>3612</v>
+        <v>3614</v>
       </c>
       <c r="J329" t="s">
-        <v>3613</v>
+        <v>3615</v>
       </c>
       <c r="K329" t="s">
-        <v>3614</v>
+        <v>3616</v>
       </c>
       <c r="L329" t="s">
-        <v>3615</v>
+        <v>3617</v>
       </c>
       <c r="M329" t="s">
-        <v>3616</v>
+        <v>3618</v>
       </c>
       <c r="N329" t="s">
         <v>1975</v>
       </c>
       <c r="O329" t="s">
-        <v>3617</v>
+        <v>3619</v>
       </c>
       <c r="P329" t="s">
-        <v>3618</v>
+        <v>3620</v>
       </c>
       <c r="Q329" t="s">
         <v>37</v>

</xml_diff>